<commit_message>
Adding MPIT4030-680M-LF inductor to BOM
</commit_message>
<xml_diff>
--- a/BOM/MIMXRT1064 MCU Module  - BOM.xlsx
+++ b/BOM/MIMXRT1064 MCU Module  - BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\32470\Documents\GitHub\MIMXRT1064-MCU-Module\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F45505A9-9E81-477D-A287-FC51989A99B0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41749008-04AA-43FC-B02E-842824F829C6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="262">
   <si>
     <t>MIMXRT1064 MCU Module  - BOM</t>
   </si>
@@ -786,6 +786,27 @@
   </si>
   <si>
     <t>2988</t>
+  </si>
+  <si>
+    <t>520mA 68uH ±20% SMD Power Inductors</t>
+  </si>
+  <si>
+    <t>SMD</t>
+  </si>
+  <si>
+    <t>68uH</t>
+  </si>
+  <si>
+    <t>microgate</t>
+  </si>
+  <si>
+    <t>MPIT4030-680M-LF</t>
+  </si>
+  <si>
+    <t>C281305</t>
+  </si>
+  <si>
+    <t>$0.081</t>
   </si>
 </sst>
 </file>
@@ -967,7 +988,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="94">
+  <cellXfs count="101">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -989,7 +1010,6 @@
     <xf numFmtId="49" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="4" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -1052,7 +1072,6 @@
     <xf numFmtId="0" fontId="6" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1105,7 +1124,30 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="14" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="14" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1326,10 +1368,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:V952"/>
+  <dimension ref="A1:V953"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29:N29"/>
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15.75" customHeight="1" zeroHeight="1"/>
@@ -1430,22 +1472,22 @@
       <c r="V2" s="1"/>
     </row>
     <row r="3" spans="1:22" ht="13">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="92" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="17"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="17"/>
-      <c r="J3" s="17"/>
-      <c r="K3" s="17"/>
-      <c r="L3" s="17"/>
-      <c r="M3" s="17"/>
-      <c r="N3" s="17"/>
+      <c r="B3" s="92"/>
+      <c r="C3" s="92"/>
+      <c r="D3" s="92"/>
+      <c r="E3" s="92"/>
+      <c r="F3" s="92"/>
+      <c r="G3" s="92"/>
+      <c r="H3" s="92"/>
+      <c r="I3" s="92"/>
+      <c r="J3" s="92"/>
+      <c r="K3" s="92"/>
+      <c r="L3" s="92"/>
+      <c r="M3" s="92"/>
+      <c r="N3" s="92"/>
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
@@ -1456,40 +1498,40 @@
       <c r="V3" s="1"/>
     </row>
     <row r="4" spans="1:22" s="6" customFormat="1" ht="13">
-      <c r="A4" s="18"/>
-      <c r="B4" s="19" t="s">
+      <c r="A4" s="17"/>
+      <c r="B4" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="20" t="s">
+      <c r="C4" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="18" t="s">
+      <c r="D4" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18" t="s">
+      <c r="E4" s="17"/>
+      <c r="F4" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="G4" s="19" t="s">
+      <c r="G4" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="H4" s="18" t="s">
+      <c r="H4" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="I4" s="19" t="s">
+      <c r="I4" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="J4" s="21" t="s">
+      <c r="J4" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="K4" s="18"/>
-      <c r="L4" s="22" t="s">
+      <c r="K4" s="17"/>
+      <c r="L4" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="M4" s="20" t="s">
+      <c r="M4" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="N4" s="18"/>
+      <c r="N4" s="17"/>
       <c r="O4" s="5"/>
       <c r="P4" s="5"/>
       <c r="Q4" s="5"/>
@@ -1500,40 +1542,40 @@
       <c r="V4" s="5"/>
     </row>
     <row r="5" spans="1:22" s="8" customFormat="1" ht="13">
-      <c r="A5" s="23"/>
-      <c r="B5" s="24" t="s">
+      <c r="A5" s="22"/>
+      <c r="B5" s="23" t="s">
         <v>248</v>
       </c>
-      <c r="C5" s="25" t="s">
+      <c r="C5" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="23" t="s">
+      <c r="D5" s="22" t="s">
         <v>244</v>
       </c>
-      <c r="E5" s="23"/>
-      <c r="F5" s="23" t="s">
+      <c r="E5" s="22"/>
+      <c r="F5" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="G5" s="26" t="s">
+      <c r="G5" s="25" t="s">
         <v>245</v>
       </c>
-      <c r="H5" s="23" t="s">
+      <c r="H5" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="I5" s="24" t="s">
+      <c r="I5" s="23" t="s">
         <v>247</v>
       </c>
-      <c r="J5" s="27" t="s">
+      <c r="J5" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="K5" s="23"/>
-      <c r="L5" s="28" t="s">
+      <c r="K5" s="22"/>
+      <c r="L5" s="27" t="s">
         <v>246</v>
       </c>
-      <c r="M5" s="25" t="s">
+      <c r="M5" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="N5" s="23"/>
+      <c r="N5" s="22"/>
       <c r="O5" s="7"/>
       <c r="P5" s="7"/>
       <c r="Q5" s="7"/>
@@ -1544,40 +1586,40 @@
       <c r="V5" s="7"/>
     </row>
     <row r="6" spans="1:22" s="6" customFormat="1" ht="13">
-      <c r="A6" s="18"/>
-      <c r="B6" s="19" t="s">
+      <c r="A6" s="17"/>
+      <c r="B6" s="18" t="s">
         <v>200</v>
       </c>
-      <c r="C6" s="20" t="s">
+      <c r="C6" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="18" t="s">
+      <c r="D6" s="17" t="s">
         <v>198</v>
       </c>
-      <c r="E6" s="18"/>
-      <c r="F6" s="18" t="s">
+      <c r="E6" s="17"/>
+      <c r="F6" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="G6" s="19" t="s">
+      <c r="G6" s="18" t="s">
         <v>197</v>
       </c>
-      <c r="H6" s="18" t="s">
+      <c r="H6" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="I6" s="29" t="s">
+      <c r="I6" s="28" t="s">
         <v>201</v>
       </c>
-      <c r="J6" s="30" t="s">
+      <c r="J6" s="29" t="s">
         <v>202</v>
       </c>
-      <c r="K6" s="18"/>
-      <c r="L6" s="31">
+      <c r="K6" s="17"/>
+      <c r="L6" s="30">
         <v>4500</v>
       </c>
-      <c r="M6" s="20" t="s">
+      <c r="M6" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="N6" s="18"/>
+      <c r="N6" s="17"/>
       <c r="O6" s="5"/>
       <c r="P6" s="5"/>
       <c r="Q6" s="5"/>
@@ -1588,40 +1630,40 @@
       <c r="V6" s="5"/>
     </row>
     <row r="7" spans="1:22" s="8" customFormat="1" ht="13">
-      <c r="A7" s="32"/>
-      <c r="B7" s="26" t="s">
+      <c r="A7" s="31"/>
+      <c r="B7" s="25" t="s">
         <v>199</v>
       </c>
-      <c r="C7" s="33" t="s">
+      <c r="C7" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="32" t="s">
+      <c r="D7" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="32"/>
-      <c r="F7" s="32" t="s">
+      <c r="E7" s="31"/>
+      <c r="F7" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="G7" s="32" t="s">
+      <c r="G7" s="31" t="s">
         <v>195</v>
       </c>
-      <c r="H7" s="32" t="s">
+      <c r="H7" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="I7" s="34" t="s">
+      <c r="I7" s="33" t="s">
         <v>196</v>
       </c>
-      <c r="J7" s="35" t="s">
+      <c r="J7" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="K7" s="32"/>
-      <c r="L7" s="36">
+      <c r="K7" s="31"/>
+      <c r="L7" s="35">
         <v>751492</v>
       </c>
-      <c r="M7" s="33" t="s">
+      <c r="M7" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="N7" s="32"/>
+      <c r="N7" s="31"/>
       <c r="O7" s="13"/>
       <c r="P7" s="13"/>
       <c r="Q7" s="13"/>
@@ -1632,40 +1674,40 @@
       <c r="V7" s="13"/>
     </row>
     <row r="8" spans="1:22" s="6" customFormat="1" ht="13">
-      <c r="A8" s="18"/>
-      <c r="B8" s="19" t="s">
+      <c r="A8" s="17"/>
+      <c r="B8" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="20" t="s">
+      <c r="C8" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="18" t="s">
+      <c r="D8" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18" t="s">
+      <c r="E8" s="17"/>
+      <c r="F8" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="G8" s="19" t="s">
+      <c r="G8" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="H8" s="18" t="s">
+      <c r="H8" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="I8" s="19" t="s">
+      <c r="I8" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="J8" s="21" t="s">
+      <c r="J8" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="K8" s="18"/>
-      <c r="L8" s="22" t="s">
+      <c r="K8" s="17"/>
+      <c r="L8" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="M8" s="20" t="s">
+      <c r="M8" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="N8" s="18"/>
+      <c r="N8" s="17"/>
       <c r="O8" s="5"/>
       <c r="P8" s="5"/>
       <c r="Q8" s="5"/>
@@ -1676,40 +1718,40 @@
       <c r="V8" s="5"/>
     </row>
     <row r="9" spans="1:22" s="8" customFormat="1" ht="13">
-      <c r="A9" s="32"/>
-      <c r="B9" s="37" t="s">
+      <c r="A9" s="31"/>
+      <c r="B9" s="36" t="s">
         <v>35</v>
       </c>
-      <c r="C9" s="33" t="s">
+      <c r="C9" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="32" t="s">
+      <c r="D9" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="E9" s="32"/>
-      <c r="F9" s="32" t="s">
+      <c r="E9" s="31"/>
+      <c r="F9" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="G9" s="37" t="s">
+      <c r="G9" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="H9" s="32" t="s">
+      <c r="H9" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="I9" s="38" t="s">
+      <c r="I9" s="37" t="s">
         <v>38</v>
       </c>
-      <c r="J9" s="39" t="s">
+      <c r="J9" s="38" t="s">
         <v>23</v>
       </c>
-      <c r="K9" s="32"/>
-      <c r="L9" s="40" t="s">
+      <c r="K9" s="31"/>
+      <c r="L9" s="39" t="s">
         <v>39</v>
       </c>
-      <c r="M9" s="33" t="s">
+      <c r="M9" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="N9" s="32"/>
+      <c r="N9" s="31"/>
       <c r="O9" s="13"/>
       <c r="P9" s="13"/>
       <c r="Q9" s="13"/>
@@ -1720,40 +1762,40 @@
       <c r="V9" s="13"/>
     </row>
     <row r="10" spans="1:22" s="6" customFormat="1" ht="13">
-      <c r="A10" s="18"/>
-      <c r="B10" s="19" t="s">
+      <c r="A10" s="17"/>
+      <c r="B10" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="C10" s="20" t="s">
+      <c r="C10" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="18" t="s">
+      <c r="D10" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18" t="s">
+      <c r="E10" s="17"/>
+      <c r="F10" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="G10" s="19" t="s">
+      <c r="G10" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="H10" s="18" t="s">
+      <c r="H10" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="I10" s="19" t="s">
+      <c r="I10" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="J10" s="21" t="s">
+      <c r="J10" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="K10" s="18"/>
-      <c r="L10" s="22" t="s">
+      <c r="K10" s="17"/>
+      <c r="L10" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="M10" s="20" t="s">
+      <c r="M10" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="N10" s="18"/>
+      <c r="N10" s="17"/>
       <c r="O10" s="5"/>
       <c r="P10" s="5"/>
       <c r="Q10" s="5"/>
@@ -1764,40 +1806,40 @@
       <c r="V10" s="5"/>
     </row>
     <row r="11" spans="1:22" s="8" customFormat="1" ht="17.25" customHeight="1">
-      <c r="A11" s="32"/>
-      <c r="B11" s="37" t="s">
+      <c r="A11" s="31"/>
+      <c r="B11" s="36" t="s">
         <v>45</v>
       </c>
-      <c r="C11" s="33" t="s">
+      <c r="C11" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="32" t="s">
+      <c r="D11" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="E11" s="32"/>
-      <c r="F11" s="32" t="s">
+      <c r="E11" s="31"/>
+      <c r="F11" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="G11" s="37" t="s">
+      <c r="G11" s="36" t="s">
         <v>47</v>
       </c>
-      <c r="H11" s="32" t="s">
+      <c r="H11" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="I11" s="37" t="s">
+      <c r="I11" s="36" t="s">
         <v>48</v>
       </c>
-      <c r="J11" s="39" t="s">
+      <c r="J11" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="K11" s="32"/>
-      <c r="L11" s="40" t="s">
+      <c r="K11" s="31"/>
+      <c r="L11" s="39" t="s">
         <v>49</v>
       </c>
-      <c r="M11" s="33" t="s">
+      <c r="M11" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="N11" s="32"/>
+      <c r="N11" s="31"/>
       <c r="O11" s="13"/>
       <c r="P11" s="13"/>
       <c r="Q11" s="13"/>
@@ -1808,40 +1850,40 @@
       <c r="V11" s="13"/>
     </row>
     <row r="12" spans="1:22" s="6" customFormat="1" ht="13">
-      <c r="A12" s="18"/>
-      <c r="B12" s="19" t="s">
+      <c r="A12" s="17"/>
+      <c r="B12" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="C12" s="20" t="s">
+      <c r="C12" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="18" t="s">
+      <c r="D12" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="E12" s="18"/>
-      <c r="F12" s="18" t="s">
+      <c r="E12" s="17"/>
+      <c r="F12" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="G12" s="19" t="s">
+      <c r="G12" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="H12" s="18" t="s">
+      <c r="H12" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="I12" s="19" t="s">
+      <c r="I12" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="J12" s="21" t="s">
+      <c r="J12" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="K12" s="18"/>
-      <c r="L12" s="22" t="s">
+      <c r="K12" s="17"/>
+      <c r="L12" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="M12" s="20" t="s">
+      <c r="M12" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="N12" s="18"/>
+      <c r="N12" s="17"/>
       <c r="O12" s="5"/>
       <c r="P12" s="5"/>
       <c r="Q12" s="5"/>
@@ -1852,40 +1894,40 @@
       <c r="V12" s="5"/>
     </row>
     <row r="13" spans="1:22" s="8" customFormat="1" ht="13">
-      <c r="A13" s="32"/>
-      <c r="B13" s="37" t="s">
+      <c r="A13" s="31"/>
+      <c r="B13" s="36" t="s">
         <v>55</v>
       </c>
-      <c r="C13" s="33" t="s">
+      <c r="C13" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="D13" s="32" t="s">
+      <c r="D13" s="31" t="s">
         <v>56</v>
       </c>
-      <c r="E13" s="32"/>
-      <c r="F13" s="32" t="s">
+      <c r="E13" s="31"/>
+      <c r="F13" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="G13" s="37" t="s">
+      <c r="G13" s="36" t="s">
         <v>57</v>
       </c>
-      <c r="H13" s="32" t="s">
+      <c r="H13" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="I13" s="37" t="s">
+      <c r="I13" s="36" t="s">
         <v>58</v>
       </c>
-      <c r="J13" s="39" t="s">
+      <c r="J13" s="38" t="s">
         <v>23</v>
       </c>
-      <c r="K13" s="32"/>
-      <c r="L13" s="40" t="s">
+      <c r="K13" s="31"/>
+      <c r="L13" s="39" t="s">
         <v>59</v>
       </c>
-      <c r="M13" s="33" t="s">
+      <c r="M13" s="32" t="s">
         <v>60</v>
       </c>
-      <c r="N13" s="32"/>
+      <c r="N13" s="31"/>
       <c r="O13" s="13"/>
       <c r="P13" s="13"/>
       <c r="Q13" s="13"/>
@@ -1896,22 +1938,22 @@
       <c r="V13" s="13"/>
     </row>
     <row r="14" spans="1:22" ht="13">
-      <c r="A14" s="17" t="s">
+      <c r="A14" s="92" t="s">
         <v>61</v>
       </c>
-      <c r="B14" s="17"/>
-      <c r="C14" s="17"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="17"/>
-      <c r="G14" s="17"/>
-      <c r="H14" s="17"/>
-      <c r="I14" s="17"/>
-      <c r="J14" s="17"/>
-      <c r="K14" s="17"/>
-      <c r="L14" s="17"/>
-      <c r="M14" s="17"/>
-      <c r="N14" s="17"/>
+      <c r="B14" s="92"/>
+      <c r="C14" s="92"/>
+      <c r="D14" s="92"/>
+      <c r="E14" s="92"/>
+      <c r="F14" s="92"/>
+      <c r="G14" s="92"/>
+      <c r="H14" s="92"/>
+      <c r="I14" s="92"/>
+      <c r="J14" s="92"/>
+      <c r="K14" s="92"/>
+      <c r="L14" s="92"/>
+      <c r="M14" s="92"/>
+      <c r="N14" s="92"/>
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
       <c r="Q14" s="1"/>
@@ -1922,40 +1964,40 @@
       <c r="V14" s="1"/>
     </row>
     <row r="15" spans="1:22" ht="13">
-      <c r="A15" s="41"/>
-      <c r="B15" s="41" t="s">
+      <c r="A15" s="40"/>
+      <c r="B15" s="40" t="s">
         <v>62</v>
       </c>
-      <c r="C15" s="42" t="s">
+      <c r="C15" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="D15" s="41" t="s">
+      <c r="D15" s="40" t="s">
         <v>63</v>
       </c>
-      <c r="E15" s="41"/>
-      <c r="F15" s="43" t="s">
+      <c r="E15" s="40"/>
+      <c r="F15" s="42" t="s">
         <v>64</v>
       </c>
-      <c r="G15" s="41" t="s">
+      <c r="G15" s="40" t="s">
         <v>65</v>
       </c>
-      <c r="H15" s="41" t="s">
+      <c r="H15" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="I15" s="43" t="s">
+      <c r="I15" s="42" t="s">
         <v>66</v>
       </c>
-      <c r="J15" s="44" t="s">
+      <c r="J15" s="43" t="s">
         <v>67</v>
       </c>
-      <c r="K15" s="41"/>
-      <c r="L15" s="45" t="s">
+      <c r="K15" s="40"/>
+      <c r="L15" s="44" t="s">
         <v>68</v>
       </c>
-      <c r="M15" s="42" t="s">
+      <c r="M15" s="41" t="s">
         <v>60</v>
       </c>
-      <c r="N15" s="41"/>
+      <c r="N15" s="40"/>
       <c r="O15" s="2"/>
       <c r="P15" s="2"/>
       <c r="Q15" s="2"/>
@@ -1966,40 +2008,40 @@
       <c r="V15" s="2"/>
     </row>
     <row r="16" spans="1:22" ht="13">
-      <c r="A16" s="46"/>
-      <c r="B16" s="47" t="s">
+      <c r="A16" s="45"/>
+      <c r="B16" s="46" t="s">
         <v>69</v>
       </c>
-      <c r="C16" s="48" t="s">
+      <c r="C16" s="47" t="s">
         <v>17</v>
       </c>
-      <c r="D16" s="46" t="s">
+      <c r="D16" s="45" t="s">
         <v>70</v>
       </c>
-      <c r="E16" s="46"/>
-      <c r="F16" s="47" t="s">
+      <c r="E16" s="45"/>
+      <c r="F16" s="46" t="s">
         <v>64</v>
       </c>
-      <c r="G16" s="46" t="s">
+      <c r="G16" s="45" t="s">
         <v>71</v>
       </c>
-      <c r="H16" s="46" t="s">
+      <c r="H16" s="45" t="s">
         <v>21</v>
       </c>
-      <c r="I16" s="47" t="s">
+      <c r="I16" s="46" t="s">
         <v>72</v>
       </c>
-      <c r="J16" s="49" t="s">
+      <c r="J16" s="48" t="s">
         <v>73</v>
       </c>
-      <c r="K16" s="46"/>
-      <c r="L16" s="50" t="s">
+      <c r="K16" s="45"/>
+      <c r="L16" s="49" t="s">
         <v>74</v>
       </c>
-      <c r="M16" s="48" t="s">
+      <c r="M16" s="47" t="s">
         <v>60</v>
       </c>
-      <c r="N16" s="46"/>
+      <c r="N16" s="45"/>
       <c r="O16" s="2"/>
       <c r="P16" s="2"/>
       <c r="Q16" s="2"/>
@@ -2010,40 +2052,40 @@
       <c r="V16" s="2"/>
     </row>
     <row r="17" spans="1:22" ht="13">
-      <c r="A17" s="41"/>
-      <c r="B17" s="41" t="s">
+      <c r="A17" s="40"/>
+      <c r="B17" s="40" t="s">
         <v>75</v>
       </c>
-      <c r="C17" s="42" t="s">
+      <c r="C17" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="D17" s="41" t="s">
+      <c r="D17" s="40" t="s">
         <v>76</v>
       </c>
-      <c r="E17" s="41"/>
-      <c r="F17" s="43" t="s">
+      <c r="E17" s="40"/>
+      <c r="F17" s="42" t="s">
         <v>77</v>
       </c>
-      <c r="G17" s="43" t="s">
+      <c r="G17" s="42" t="s">
         <v>78</v>
       </c>
-      <c r="H17" s="41" t="s">
+      <c r="H17" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="I17" s="43" t="s">
+      <c r="I17" s="42" t="s">
         <v>79</v>
       </c>
-      <c r="J17" s="44" t="s">
+      <c r="J17" s="43" t="s">
         <v>28</v>
       </c>
-      <c r="K17" s="41"/>
-      <c r="L17" s="45" t="s">
+      <c r="K17" s="40"/>
+      <c r="L17" s="44" t="s">
         <v>80</v>
       </c>
-      <c r="M17" s="42" t="s">
+      <c r="M17" s="41" t="s">
         <v>25</v>
       </c>
-      <c r="N17" s="41"/>
+      <c r="N17" s="40"/>
       <c r="O17" s="2"/>
       <c r="P17" s="2"/>
       <c r="Q17" s="2"/>
@@ -2054,40 +2096,40 @@
       <c r="V17" s="2"/>
     </row>
     <row r="18" spans="1:22" ht="13">
-      <c r="A18" s="46"/>
-      <c r="B18" s="46" t="s">
+      <c r="A18" s="45"/>
+      <c r="B18" s="45" t="s">
         <v>81</v>
       </c>
-      <c r="C18" s="48" t="s">
+      <c r="C18" s="47" t="s">
         <v>17</v>
       </c>
-      <c r="D18" s="46" t="s">
+      <c r="D18" s="45" t="s">
         <v>82</v>
       </c>
-      <c r="E18" s="46"/>
-      <c r="F18" s="47" t="s">
+      <c r="E18" s="45"/>
+      <c r="F18" s="46" t="s">
         <v>83</v>
       </c>
-      <c r="G18" s="47" t="s">
+      <c r="G18" s="46" t="s">
         <v>84</v>
       </c>
-      <c r="H18" s="46" t="s">
+      <c r="H18" s="45" t="s">
         <v>21</v>
       </c>
-      <c r="I18" s="47" t="s">
+      <c r="I18" s="46" t="s">
         <v>85</v>
       </c>
-      <c r="J18" s="49" t="s">
+      <c r="J18" s="48" t="s">
         <v>86</v>
       </c>
-      <c r="K18" s="46"/>
-      <c r="L18" s="50" t="s">
+      <c r="K18" s="45"/>
+      <c r="L18" s="49" t="s">
         <v>87</v>
       </c>
-      <c r="M18" s="48" t="s">
+      <c r="M18" s="47" t="s">
         <v>25</v>
       </c>
-      <c r="N18" s="46"/>
+      <c r="N18" s="45"/>
       <c r="O18" s="2"/>
       <c r="P18" s="2"/>
       <c r="Q18" s="2"/>
@@ -2098,40 +2140,40 @@
       <c r="V18" s="2"/>
     </row>
     <row r="19" spans="1:22" ht="13">
-      <c r="A19" s="41"/>
-      <c r="B19" s="43" t="s">
+      <c r="A19" s="40"/>
+      <c r="B19" s="42" t="s">
         <v>88</v>
       </c>
-      <c r="C19" s="42" t="s">
+      <c r="C19" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="D19" s="41" t="s">
+      <c r="D19" s="40" t="s">
         <v>89</v>
       </c>
-      <c r="E19" s="41"/>
-      <c r="F19" s="43" t="s">
+      <c r="E19" s="40"/>
+      <c r="F19" s="42" t="s">
         <v>83</v>
       </c>
-      <c r="G19" s="43" t="s">
+      <c r="G19" s="42" t="s">
         <v>90</v>
       </c>
-      <c r="H19" s="41" t="s">
+      <c r="H19" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="I19" s="43" t="s">
+      <c r="I19" s="42" t="s">
         <v>91</v>
       </c>
-      <c r="J19" s="44" t="s">
+      <c r="J19" s="43" t="s">
         <v>92</v>
       </c>
-      <c r="K19" s="41"/>
-      <c r="L19" s="45" t="s">
+      <c r="K19" s="40"/>
+      <c r="L19" s="44" t="s">
         <v>93</v>
       </c>
-      <c r="M19" s="42" t="s">
+      <c r="M19" s="41" t="s">
         <v>25</v>
       </c>
-      <c r="N19" s="41"/>
+      <c r="N19" s="40"/>
       <c r="O19" s="2"/>
       <c r="P19" s="2"/>
       <c r="Q19" s="2"/>
@@ -2142,40 +2184,40 @@
       <c r="V19" s="2"/>
     </row>
     <row r="20" spans="1:22" ht="13">
-      <c r="A20" s="46"/>
-      <c r="B20" s="47" t="s">
+      <c r="A20" s="45"/>
+      <c r="B20" s="46" t="s">
         <v>94</v>
       </c>
-      <c r="C20" s="48" t="s">
+      <c r="C20" s="47" t="s">
         <v>17</v>
       </c>
-      <c r="D20" s="46" t="s">
+      <c r="D20" s="45" t="s">
         <v>95</v>
       </c>
-      <c r="E20" s="46"/>
-      <c r="F20" s="47" t="s">
+      <c r="E20" s="45"/>
+      <c r="F20" s="46" t="s">
         <v>83</v>
       </c>
-      <c r="G20" s="47" t="s">
+      <c r="G20" s="46" t="s">
         <v>96</v>
       </c>
-      <c r="H20" s="46" t="s">
+      <c r="H20" s="45" t="s">
         <v>21</v>
       </c>
-      <c r="I20" s="47" t="s">
+      <c r="I20" s="46" t="s">
         <v>97</v>
       </c>
-      <c r="J20" s="49" t="s">
+      <c r="J20" s="48" t="s">
         <v>98</v>
       </c>
-      <c r="K20" s="46"/>
-      <c r="L20" s="50" t="s">
+      <c r="K20" s="45"/>
+      <c r="L20" s="49" t="s">
         <v>99</v>
       </c>
-      <c r="M20" s="48" t="s">
+      <c r="M20" s="47" t="s">
         <v>25</v>
       </c>
-      <c r="N20" s="46"/>
+      <c r="N20" s="45"/>
       <c r="O20" s="2"/>
       <c r="P20" s="2"/>
       <c r="Q20" s="2"/>
@@ -2186,40 +2228,40 @@
       <c r="V20" s="2"/>
     </row>
     <row r="21" spans="1:22" ht="13">
-      <c r="A21" s="41"/>
-      <c r="B21" s="43" t="s">
+      <c r="A21" s="40"/>
+      <c r="B21" s="42" t="s">
         <v>100</v>
       </c>
-      <c r="C21" s="42" t="s">
+      <c r="C21" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="D21" s="41" t="s">
+      <c r="D21" s="40" t="s">
         <v>101</v>
       </c>
-      <c r="E21" s="41"/>
-      <c r="F21" s="43" t="s">
+      <c r="E21" s="40"/>
+      <c r="F21" s="42" t="s">
         <v>83</v>
       </c>
-      <c r="G21" s="43" t="s">
+      <c r="G21" s="42" t="s">
         <v>102</v>
       </c>
-      <c r="H21" s="41" t="s">
+      <c r="H21" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="I21" s="43" t="s">
+      <c r="I21" s="42" t="s">
         <v>103</v>
       </c>
-      <c r="J21" s="44" t="s">
+      <c r="J21" s="43" t="s">
         <v>104</v>
       </c>
-      <c r="K21" s="41"/>
-      <c r="L21" s="45" t="s">
+      <c r="K21" s="40"/>
+      <c r="L21" s="44" t="s">
         <v>105</v>
       </c>
-      <c r="M21" s="42" t="s">
+      <c r="M21" s="41" t="s">
         <v>25</v>
       </c>
-      <c r="N21" s="41"/>
+      <c r="N21" s="40"/>
       <c r="O21" s="2"/>
       <c r="P21" s="2"/>
       <c r="Q21" s="2"/>
@@ -2230,40 +2272,40 @@
       <c r="V21" s="2"/>
     </row>
     <row r="22" spans="1:22" ht="13">
-      <c r="A22" s="46"/>
-      <c r="B22" s="47" t="s">
+      <c r="A22" s="45"/>
+      <c r="B22" s="46" t="s">
         <v>106</v>
       </c>
-      <c r="C22" s="48" t="s">
+      <c r="C22" s="47" t="s">
         <v>17</v>
       </c>
-      <c r="D22" s="46" t="s">
+      <c r="D22" s="45" t="s">
         <v>107</v>
       </c>
-      <c r="E22" s="46"/>
-      <c r="F22" s="47" t="s">
+      <c r="E22" s="45"/>
+      <c r="F22" s="46" t="s">
         <v>83</v>
       </c>
-      <c r="G22" s="47" t="s">
+      <c r="G22" s="46" t="s">
         <v>108</v>
       </c>
-      <c r="H22" s="46" t="s">
+      <c r="H22" s="45" t="s">
         <v>21</v>
       </c>
-      <c r="I22" s="47" t="s">
+      <c r="I22" s="46" t="s">
         <v>109</v>
       </c>
-      <c r="J22" s="49" t="s">
+      <c r="J22" s="48" t="s">
         <v>110</v>
       </c>
-      <c r="K22" s="46"/>
-      <c r="L22" s="50" t="s">
+      <c r="K22" s="45"/>
+      <c r="L22" s="49" t="s">
         <v>111</v>
       </c>
-      <c r="M22" s="48" t="s">
+      <c r="M22" s="47" t="s">
         <v>25</v>
       </c>
-      <c r="N22" s="46"/>
+      <c r="N22" s="45"/>
       <c r="O22" s="2"/>
       <c r="P22" s="2"/>
       <c r="Q22" s="2"/>
@@ -2274,40 +2316,40 @@
       <c r="V22" s="2"/>
     </row>
     <row r="23" spans="1:22" ht="13">
-      <c r="A23" s="41"/>
-      <c r="B23" s="43" t="s">
+      <c r="A23" s="40"/>
+      <c r="B23" s="42" t="s">
         <v>112</v>
       </c>
-      <c r="C23" s="42" t="s">
+      <c r="C23" s="41" t="s">
         <v>26</v>
       </c>
-      <c r="D23" s="41" t="s">
+      <c r="D23" s="40" t="s">
         <v>113</v>
       </c>
-      <c r="E23" s="41"/>
-      <c r="F23" s="43" t="s">
+      <c r="E23" s="40"/>
+      <c r="F23" s="42" t="s">
         <v>83</v>
       </c>
-      <c r="G23" s="43" t="s">
+      <c r="G23" s="42" t="s">
         <v>114</v>
       </c>
-      <c r="H23" s="41" t="s">
+      <c r="H23" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="I23" s="43" t="s">
+      <c r="I23" s="42" t="s">
         <v>115</v>
       </c>
-      <c r="J23" s="44" t="s">
+      <c r="J23" s="43" t="s">
         <v>116</v>
       </c>
-      <c r="K23" s="41"/>
-      <c r="L23" s="45" t="s">
+      <c r="K23" s="40"/>
+      <c r="L23" s="44" t="s">
         <v>117</v>
       </c>
-      <c r="M23" s="42" t="s">
+      <c r="M23" s="41" t="s">
         <v>25</v>
       </c>
-      <c r="N23" s="41"/>
+      <c r="N23" s="40"/>
       <c r="O23" s="2"/>
       <c r="P23" s="2"/>
       <c r="Q23" s="2"/>
@@ -2318,40 +2360,40 @@
       <c r="V23" s="2"/>
     </row>
     <row r="24" spans="1:22" ht="13">
-      <c r="A24" s="46"/>
-      <c r="B24" s="47" t="s">
+      <c r="A24" s="45"/>
+      <c r="B24" s="46" t="s">
         <v>118</v>
       </c>
-      <c r="C24" s="48" t="s">
+      <c r="C24" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="D24" s="46" t="s">
+      <c r="D24" s="45" t="s">
         <v>119</v>
       </c>
-      <c r="E24" s="46"/>
-      <c r="F24" s="47" t="s">
+      <c r="E24" s="45"/>
+      <c r="F24" s="46" t="s">
         <v>83</v>
       </c>
-      <c r="G24" s="47" t="s">
+      <c r="G24" s="46" t="s">
         <v>120</v>
       </c>
-      <c r="H24" s="46" t="s">
+      <c r="H24" s="45" t="s">
         <v>21</v>
       </c>
-      <c r="I24" s="47" t="s">
+      <c r="I24" s="46" t="s">
         <v>121</v>
       </c>
-      <c r="J24" s="49" t="s">
+      <c r="J24" s="48" t="s">
         <v>122</v>
       </c>
-      <c r="K24" s="46"/>
-      <c r="L24" s="50" t="s">
+      <c r="K24" s="45"/>
+      <c r="L24" s="49" t="s">
         <v>123</v>
       </c>
-      <c r="M24" s="48" t="s">
+      <c r="M24" s="47" t="s">
         <v>25</v>
       </c>
-      <c r="N24" s="46"/>
+      <c r="N24" s="45"/>
       <c r="O24" s="2"/>
       <c r="P24" s="2"/>
       <c r="Q24" s="2"/>
@@ -2362,22 +2404,22 @@
       <c r="V24" s="2"/>
     </row>
     <row r="25" spans="1:22" ht="13">
-      <c r="A25" s="17" t="s">
+      <c r="A25" s="92" t="s">
         <v>124</v>
       </c>
-      <c r="B25" s="17"/>
-      <c r="C25" s="17"/>
-      <c r="D25" s="17"/>
-      <c r="E25" s="17"/>
-      <c r="F25" s="17"/>
-      <c r="G25" s="17"/>
-      <c r="H25" s="17"/>
-      <c r="I25" s="17"/>
-      <c r="J25" s="17"/>
-      <c r="K25" s="17"/>
-      <c r="L25" s="17"/>
-      <c r="M25" s="17"/>
-      <c r="N25" s="17"/>
+      <c r="B25" s="92"/>
+      <c r="C25" s="92"/>
+      <c r="D25" s="92"/>
+      <c r="E25" s="92"/>
+      <c r="F25" s="92"/>
+      <c r="G25" s="92"/>
+      <c r="H25" s="92"/>
+      <c r="I25" s="92"/>
+      <c r="J25" s="92"/>
+      <c r="K25" s="92"/>
+      <c r="L25" s="92"/>
+      <c r="M25" s="92"/>
+      <c r="N25" s="92"/>
       <c r="O25" s="2"/>
       <c r="P25" s="2"/>
       <c r="Q25" s="2"/>
@@ -2388,40 +2430,40 @@
       <c r="V25" s="2"/>
     </row>
     <row r="26" spans="1:22" s="6" customFormat="1" ht="13">
-      <c r="A26" s="51"/>
-      <c r="B26" s="52" t="s">
+      <c r="A26" s="50"/>
+      <c r="B26" s="51" t="s">
         <v>243</v>
       </c>
-      <c r="C26" s="53" t="s">
+      <c r="C26" s="52" t="s">
         <v>17</v>
       </c>
-      <c r="D26" s="51" t="s">
+      <c r="D26" s="50" t="s">
         <v>242</v>
       </c>
-      <c r="E26" s="51"/>
-      <c r="F26" s="51" t="s">
+      <c r="E26" s="50"/>
+      <c r="F26" s="50" t="s">
         <v>241</v>
       </c>
-      <c r="G26" s="51" t="s">
+      <c r="G26" s="50" t="s">
         <v>238</v>
       </c>
-      <c r="H26" s="41" t="s">
+      <c r="H26" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="I26" s="52" t="s">
+      <c r="I26" s="51" t="s">
         <v>240</v>
       </c>
-      <c r="J26" s="54" t="s">
+      <c r="J26" s="53" t="s">
         <v>239</v>
       </c>
-      <c r="K26" s="51"/>
-      <c r="L26" s="55">
+      <c r="K26" s="50"/>
+      <c r="L26" s="54">
         <v>20488</v>
       </c>
-      <c r="M26" s="42" t="s">
+      <c r="M26" s="41" t="s">
         <v>60</v>
       </c>
-      <c r="N26" s="51"/>
+      <c r="N26" s="50"/>
       <c r="O26" s="5"/>
       <c r="P26" s="5"/>
       <c r="Q26" s="5"/>
@@ -2432,40 +2474,40 @@
       <c r="V26" s="5"/>
     </row>
     <row r="27" spans="1:22" s="8" customFormat="1" ht="13">
-      <c r="A27" s="23"/>
-      <c r="B27" s="23" t="s">
+      <c r="A27" s="22"/>
+      <c r="B27" s="22" t="s">
         <v>125</v>
       </c>
-      <c r="C27" s="25" t="s">
+      <c r="C27" s="24" t="s">
         <v>126</v>
       </c>
-      <c r="D27" s="23" t="s">
+      <c r="D27" s="22" t="s">
         <v>127</v>
       </c>
-      <c r="E27" s="23"/>
-      <c r="F27" s="23" t="s">
+      <c r="E27" s="22"/>
+      <c r="F27" s="22" t="s">
         <v>128</v>
       </c>
-      <c r="G27" s="23" t="s">
+      <c r="G27" s="22" t="s">
         <v>129</v>
       </c>
-      <c r="H27" s="23" t="s">
+      <c r="H27" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="I27" s="23" t="s">
+      <c r="I27" s="22" t="s">
         <v>130</v>
       </c>
-      <c r="J27" s="23" t="s">
+      <c r="J27" s="22" t="s">
         <v>131</v>
       </c>
-      <c r="K27" s="23"/>
-      <c r="L27" s="25" t="s">
+      <c r="K27" s="22"/>
+      <c r="L27" s="24" t="s">
         <v>132</v>
       </c>
-      <c r="M27" s="25" t="s">
+      <c r="M27" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="N27" s="23"/>
+      <c r="N27" s="22"/>
       <c r="O27" s="7"/>
       <c r="P27" s="7"/>
       <c r="Q27" s="7"/>
@@ -2476,40 +2518,40 @@
       <c r="V27" s="7"/>
     </row>
     <row r="28" spans="1:22" s="6" customFormat="1" ht="13">
-      <c r="A28" s="56"/>
-      <c r="B28" s="57" t="s">
+      <c r="A28" s="55"/>
+      <c r="B28" s="56" t="s">
         <v>133</v>
       </c>
-      <c r="C28" s="58" t="s">
+      <c r="C28" s="57" t="s">
         <v>134</v>
       </c>
-      <c r="D28" s="56" t="s">
+      <c r="D28" s="55" t="s">
         <v>135</v>
       </c>
-      <c r="E28" s="56"/>
-      <c r="F28" s="56" t="s">
+      <c r="E28" s="55"/>
+      <c r="F28" s="55" t="s">
         <v>128</v>
       </c>
-      <c r="G28" s="57" t="s">
+      <c r="G28" s="56" t="s">
         <v>136</v>
       </c>
-      <c r="H28" s="56" t="s">
+      <c r="H28" s="55" t="s">
         <v>21</v>
       </c>
-      <c r="I28" s="57" t="s">
+      <c r="I28" s="56" t="s">
         <v>137</v>
       </c>
-      <c r="J28" s="59" t="s">
+      <c r="J28" s="58" t="s">
         <v>138</v>
       </c>
-      <c r="K28" s="56"/>
-      <c r="L28" s="58" t="s">
+      <c r="K28" s="55"/>
+      <c r="L28" s="57" t="s">
         <v>139</v>
       </c>
-      <c r="M28" s="53" t="s">
+      <c r="M28" s="52" t="s">
         <v>60</v>
       </c>
-      <c r="N28" s="56"/>
+      <c r="N28" s="55"/>
       <c r="O28" s="5"/>
       <c r="P28" s="5"/>
       <c r="Q28" s="5"/>
@@ -2519,67 +2561,67 @@
       <c r="U28" s="5"/>
       <c r="V28" s="5"/>
     </row>
-    <row r="29" spans="1:22" ht="13">
-      <c r="A29" s="17" t="s">
+    <row r="29" spans="1:22" s="100" customFormat="1" ht="13">
+      <c r="A29" s="94"/>
+      <c r="B29" s="95" t="s">
+        <v>255</v>
+      </c>
+      <c r="C29" s="96" t="s">
+        <v>256</v>
+      </c>
+      <c r="D29" s="94" t="s">
+        <v>257</v>
+      </c>
+      <c r="E29" s="94"/>
+      <c r="F29" s="94" t="s">
+        <v>258</v>
+      </c>
+      <c r="G29" s="95" t="s">
+        <v>259</v>
+      </c>
+      <c r="H29" s="94" t="s">
+        <v>21</v>
+      </c>
+      <c r="I29" s="95" t="s">
+        <v>260</v>
+      </c>
+      <c r="J29" s="97" t="s">
+        <v>261</v>
+      </c>
+      <c r="K29" s="94"/>
+      <c r="L29" s="95">
+        <v>965</v>
+      </c>
+      <c r="M29" s="98" t="s">
+        <v>60</v>
+      </c>
+      <c r="N29" s="94"/>
+      <c r="O29" s="99"/>
+      <c r="P29" s="99"/>
+      <c r="Q29" s="99"/>
+      <c r="R29" s="99"/>
+      <c r="S29" s="99"/>
+      <c r="T29" s="99"/>
+      <c r="U29" s="99"/>
+      <c r="V29" s="99"/>
+    </row>
+    <row r="30" spans="1:22" ht="13">
+      <c r="A30" s="92" t="s">
         <v>140</v>
       </c>
-      <c r="B29" s="17"/>
-      <c r="C29" s="17"/>
-      <c r="D29" s="17"/>
-      <c r="E29" s="17"/>
-      <c r="F29" s="17"/>
-      <c r="G29" s="17"/>
-      <c r="H29" s="17"/>
-      <c r="I29" s="17"/>
-      <c r="J29" s="17"/>
-      <c r="K29" s="17"/>
-      <c r="L29" s="17"/>
-      <c r="M29" s="17"/>
-      <c r="N29" s="17"/>
-      <c r="O29" s="2"/>
-      <c r="P29" s="2"/>
-      <c r="Q29" s="2"/>
-      <c r="R29" s="2"/>
-      <c r="S29" s="2"/>
-      <c r="T29" s="2"/>
-      <c r="U29" s="2"/>
-      <c r="V29" s="2"/>
-    </row>
-    <row r="30" spans="1:22" ht="13">
-      <c r="A30" s="41"/>
-      <c r="B30" s="41" t="s">
-        <v>141</v>
-      </c>
-      <c r="C30" s="42" t="s">
-        <v>26</v>
-      </c>
-      <c r="D30" s="41" t="s">
-        <v>142</v>
-      </c>
-      <c r="E30" s="41"/>
-      <c r="F30" s="41" t="s">
-        <v>143</v>
-      </c>
-      <c r="G30" s="41" t="s">
-        <v>144</v>
-      </c>
-      <c r="H30" s="41" t="s">
-        <v>21</v>
-      </c>
-      <c r="I30" s="41" t="s">
-        <v>145</v>
-      </c>
-      <c r="J30" s="41" t="s">
-        <v>146</v>
-      </c>
-      <c r="K30" s="41"/>
-      <c r="L30" s="45" t="s">
-        <v>147</v>
-      </c>
-      <c r="M30" s="42" t="s">
-        <v>60</v>
-      </c>
-      <c r="N30" s="41"/>
+      <c r="B30" s="92"/>
+      <c r="C30" s="92"/>
+      <c r="D30" s="92"/>
+      <c r="E30" s="92"/>
+      <c r="F30" s="92"/>
+      <c r="G30" s="92"/>
+      <c r="H30" s="92"/>
+      <c r="I30" s="92"/>
+      <c r="J30" s="92"/>
+      <c r="K30" s="92"/>
+      <c r="L30" s="92"/>
+      <c r="M30" s="92"/>
+      <c r="N30" s="92"/>
       <c r="O30" s="2"/>
       <c r="P30" s="2"/>
       <c r="Q30" s="2"/>
@@ -2590,22 +2632,40 @@
       <c r="V30" s="2"/>
     </row>
     <row r="31" spans="1:22" ht="13">
-      <c r="A31" s="60" t="s">
-        <v>148</v>
-      </c>
-      <c r="B31" s="60"/>
-      <c r="C31" s="60"/>
-      <c r="D31" s="60"/>
-      <c r="E31" s="60"/>
-      <c r="F31" s="60"/>
-      <c r="G31" s="60"/>
-      <c r="H31" s="60"/>
-      <c r="I31" s="60"/>
-      <c r="J31" s="60"/>
-      <c r="K31" s="60"/>
-      <c r="L31" s="60"/>
-      <c r="M31" s="60"/>
-      <c r="N31" s="60"/>
+      <c r="A31" s="40"/>
+      <c r="B31" s="40" t="s">
+        <v>141</v>
+      </c>
+      <c r="C31" s="41" t="s">
+        <v>26</v>
+      </c>
+      <c r="D31" s="40" t="s">
+        <v>142</v>
+      </c>
+      <c r="E31" s="40"/>
+      <c r="F31" s="40" t="s">
+        <v>143</v>
+      </c>
+      <c r="G31" s="40" t="s">
+        <v>144</v>
+      </c>
+      <c r="H31" s="40" t="s">
+        <v>21</v>
+      </c>
+      <c r="I31" s="40" t="s">
+        <v>145</v>
+      </c>
+      <c r="J31" s="40" t="s">
+        <v>146</v>
+      </c>
+      <c r="K31" s="40"/>
+      <c r="L31" s="44" t="s">
+        <v>147</v>
+      </c>
+      <c r="M31" s="41" t="s">
+        <v>60</v>
+      </c>
+      <c r="N31" s="40"/>
       <c r="O31" s="2"/>
       <c r="P31" s="2"/>
       <c r="Q31" s="2"/>
@@ -2616,40 +2676,22 @@
       <c r="V31" s="2"/>
     </row>
     <row r="32" spans="1:22" ht="13">
-      <c r="A32" s="61"/>
-      <c r="B32" s="62" t="s">
-        <v>149</v>
-      </c>
-      <c r="C32" s="43" t="s">
-        <v>150</v>
-      </c>
-      <c r="D32" s="63"/>
-      <c r="E32" s="64"/>
-      <c r="F32" s="43" t="s">
-        <v>151</v>
-      </c>
-      <c r="G32" s="64" t="s">
-        <v>152</v>
-      </c>
-      <c r="H32" s="64" t="s">
-        <v>21</v>
-      </c>
-      <c r="I32" s="43" t="s">
-        <v>153</v>
-      </c>
-      <c r="J32" s="44" t="s">
-        <v>154</v>
-      </c>
-      <c r="K32" s="65"/>
-      <c r="L32" s="66" t="s">
-        <v>155</v>
-      </c>
-      <c r="M32" s="66" t="s">
-        <v>60</v>
-      </c>
-      <c r="N32" s="64" t="s">
-        <v>156</v>
-      </c>
+      <c r="A32" s="91" t="s">
+        <v>148</v>
+      </c>
+      <c r="B32" s="91"/>
+      <c r="C32" s="91"/>
+      <c r="D32" s="91"/>
+      <c r="E32" s="91"/>
+      <c r="F32" s="91"/>
+      <c r="G32" s="91"/>
+      <c r="H32" s="91"/>
+      <c r="I32" s="91"/>
+      <c r="J32" s="91"/>
+      <c r="K32" s="91"/>
+      <c r="L32" s="91"/>
+      <c r="M32" s="91"/>
+      <c r="N32" s="91"/>
       <c r="O32" s="2"/>
       <c r="P32" s="2"/>
       <c r="Q32" s="2"/>
@@ -2659,281 +2701,281 @@
       <c r="U32" s="2"/>
       <c r="V32" s="2"/>
     </row>
-    <row r="33" spans="1:22" s="10" customFormat="1" ht="13">
-      <c r="A33" s="67"/>
-      <c r="B33" s="34" t="s">
+    <row r="33" spans="1:22" ht="13">
+      <c r="A33" s="59"/>
+      <c r="B33" s="60" t="s">
+        <v>149</v>
+      </c>
+      <c r="C33" s="42" t="s">
+        <v>150</v>
+      </c>
+      <c r="D33" s="61"/>
+      <c r="E33" s="62"/>
+      <c r="F33" s="42" t="s">
+        <v>151</v>
+      </c>
+      <c r="G33" s="62" t="s">
+        <v>152</v>
+      </c>
+      <c r="H33" s="62" t="s">
+        <v>21</v>
+      </c>
+      <c r="I33" s="42" t="s">
+        <v>153</v>
+      </c>
+      <c r="J33" s="43" t="s">
+        <v>154</v>
+      </c>
+      <c r="K33" s="63"/>
+      <c r="L33" s="64" t="s">
+        <v>155</v>
+      </c>
+      <c r="M33" s="64" t="s">
+        <v>60</v>
+      </c>
+      <c r="N33" s="62" t="s">
+        <v>156</v>
+      </c>
+      <c r="O33" s="2"/>
+      <c r="P33" s="2"/>
+      <c r="Q33" s="2"/>
+      <c r="R33" s="2"/>
+      <c r="S33" s="2"/>
+      <c r="T33" s="2"/>
+      <c r="U33" s="2"/>
+      <c r="V33" s="2"/>
+    </row>
+    <row r="34" spans="1:22" s="10" customFormat="1" ht="13">
+      <c r="A34" s="65"/>
+      <c r="B34" s="33" t="s">
         <v>237</v>
       </c>
-      <c r="C33" s="34" t="s">
+      <c r="C34" s="33" t="s">
         <v>235</v>
       </c>
-      <c r="D33" s="68"/>
-      <c r="E33" s="69"/>
-      <c r="F33" s="34" t="s">
+      <c r="D34" s="66"/>
+      <c r="E34" s="67"/>
+      <c r="F34" s="33" t="s">
         <v>234</v>
       </c>
-      <c r="G33" s="34" t="s">
+      <c r="G34" s="33" t="s">
         <v>232</v>
       </c>
-      <c r="H33" s="69" t="s">
+      <c r="H34" s="67" t="s">
         <v>21</v>
       </c>
-      <c r="I33" s="34" t="s">
+      <c r="I34" s="33" t="s">
         <v>233</v>
       </c>
-      <c r="J33" s="70" t="s">
+      <c r="J34" s="68" t="s">
         <v>236</v>
       </c>
-      <c r="K33" s="71"/>
-      <c r="L33" s="36">
+      <c r="K34" s="69"/>
+      <c r="L34" s="35">
         <v>1266</v>
       </c>
-      <c r="M33" s="72" t="s">
+      <c r="M34" s="70" t="s">
         <v>60</v>
       </c>
-      <c r="N33" s="69"/>
-      <c r="O33" s="7"/>
-      <c r="P33" s="7"/>
-      <c r="Q33" s="7"/>
-      <c r="R33" s="7"/>
-      <c r="S33" s="7"/>
-      <c r="T33" s="7"/>
-      <c r="U33" s="7"/>
-      <c r="V33" s="7"/>
-    </row>
-    <row r="34" spans="1:22" s="6" customFormat="1" ht="13">
-      <c r="A34" s="56"/>
-      <c r="B34" s="73" t="s">
+      <c r="N34" s="67"/>
+      <c r="O34" s="7"/>
+      <c r="P34" s="7"/>
+      <c r="Q34" s="7"/>
+      <c r="R34" s="7"/>
+      <c r="S34" s="7"/>
+      <c r="T34" s="7"/>
+      <c r="U34" s="7"/>
+      <c r="V34" s="7"/>
+    </row>
+    <row r="35" spans="1:22" s="6" customFormat="1" ht="13">
+      <c r="A35" s="55"/>
+      <c r="B35" s="71" t="s">
         <v>157</v>
       </c>
-      <c r="C34" s="57" t="s">
+      <c r="C35" s="56" t="s">
         <v>158</v>
       </c>
-      <c r="D34" s="56" t="s">
+      <c r="D35" s="55" t="s">
         <v>159</v>
       </c>
-      <c r="E34" s="56"/>
-      <c r="F34" s="56" t="s">
+      <c r="E35" s="55"/>
+      <c r="F35" s="55" t="s">
         <v>160</v>
       </c>
-      <c r="G34" s="74" t="s">
+      <c r="G35" s="72" t="s">
         <v>161</v>
       </c>
-      <c r="H34" s="56" t="s">
+      <c r="H35" s="55" t="s">
         <v>21</v>
       </c>
-      <c r="I34" s="57" t="s">
+      <c r="I35" s="56" t="s">
         <v>162</v>
       </c>
-      <c r="J34" s="73" t="s">
+      <c r="J35" s="71" t="s">
         <v>163</v>
       </c>
-      <c r="K34" s="75"/>
-      <c r="L34" s="58">
+      <c r="K35" s="73"/>
+      <c r="L35" s="57">
         <v>280</v>
       </c>
-      <c r="M34" s="53" t="s">
+      <c r="M35" s="52" t="s">
         <v>60</v>
       </c>
-      <c r="N34" s="56"/>
-      <c r="O34" s="9"/>
-      <c r="P34" s="9"/>
-      <c r="Q34" s="9"/>
-      <c r="R34" s="9"/>
-      <c r="S34" s="9"/>
-      <c r="T34" s="9"/>
-      <c r="U34" s="9"/>
-      <c r="V34" s="9"/>
-    </row>
-    <row r="35" spans="1:22" s="8" customFormat="1" ht="13">
-      <c r="A35" s="23"/>
-      <c r="B35" s="23" t="s">
+      <c r="N35" s="55"/>
+      <c r="O35" s="9"/>
+      <c r="P35" s="9"/>
+      <c r="Q35" s="9"/>
+      <c r="R35" s="9"/>
+      <c r="S35" s="9"/>
+      <c r="T35" s="9"/>
+      <c r="U35" s="9"/>
+      <c r="V35" s="9"/>
+    </row>
+    <row r="36" spans="1:22" s="8" customFormat="1" ht="13">
+      <c r="A36" s="22"/>
+      <c r="B36" s="22" t="s">
         <v>164</v>
       </c>
-      <c r="C35" s="23" t="s">
+      <c r="C36" s="22" t="s">
         <v>165</v>
       </c>
-      <c r="D35" s="23" t="s">
+      <c r="D36" s="22" t="s">
         <v>166</v>
       </c>
-      <c r="E35" s="23"/>
-      <c r="F35" s="23" t="s">
+      <c r="E36" s="22"/>
+      <c r="F36" s="22" t="s">
         <v>160</v>
       </c>
-      <c r="G35" s="23" t="s">
+      <c r="G36" s="22" t="s">
         <v>167</v>
       </c>
-      <c r="H35" s="23" t="s">
+      <c r="H36" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="I35" s="23" t="s">
+      <c r="I36" s="22" t="s">
         <v>168</v>
       </c>
-      <c r="J35" s="23" t="s">
+      <c r="J36" s="22" t="s">
         <v>169</v>
       </c>
-      <c r="K35" s="76"/>
-      <c r="L35" s="25">
+      <c r="K36" s="74"/>
+      <c r="L36" s="24">
         <v>2304</v>
       </c>
-      <c r="M35" s="25" t="s">
+      <c r="M36" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="N35" s="23"/>
-      <c r="O35" s="11"/>
-      <c r="P35" s="11"/>
-      <c r="Q35" s="11"/>
-      <c r="R35" s="11"/>
-      <c r="S35" s="11"/>
-      <c r="T35" s="11"/>
-      <c r="U35" s="11"/>
-      <c r="V35" s="11"/>
-    </row>
-    <row r="36" spans="1:22" ht="13">
-      <c r="A36" s="41"/>
-      <c r="B36" s="77" t="s">
+      <c r="N36" s="22"/>
+      <c r="O36" s="11"/>
+      <c r="P36" s="11"/>
+      <c r="Q36" s="11"/>
+      <c r="R36" s="11"/>
+      <c r="S36" s="11"/>
+      <c r="T36" s="11"/>
+      <c r="U36" s="11"/>
+      <c r="V36" s="11"/>
+    </row>
+    <row r="37" spans="1:22" ht="13">
+      <c r="A37" s="40"/>
+      <c r="B37" s="75" t="s">
         <v>208</v>
       </c>
-      <c r="C36" s="77" t="s">
+      <c r="C37" s="75" t="s">
         <v>207</v>
       </c>
-      <c r="D36" s="41"/>
-      <c r="E36" s="41"/>
-      <c r="F36" s="77" t="s">
+      <c r="D37" s="40"/>
+      <c r="E37" s="40"/>
+      <c r="F37" s="75" t="s">
         <v>206</v>
       </c>
-      <c r="G36" s="41" t="s">
+      <c r="G37" s="40" t="s">
         <v>203</v>
       </c>
-      <c r="H36" s="41" t="s">
+      <c r="H37" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="I36" s="77" t="s">
+      <c r="I37" s="75" t="s">
         <v>204</v>
       </c>
-      <c r="J36" s="78" t="s">
+      <c r="J37" s="76" t="s">
         <v>205</v>
       </c>
-      <c r="K36" s="79"/>
-      <c r="L36" s="80">
+      <c r="K37" s="77"/>
+      <c r="L37" s="78">
         <v>5850</v>
       </c>
-      <c r="M36" s="42" t="s">
+      <c r="M37" s="41" t="s">
         <v>60</v>
       </c>
-      <c r="N36" s="41"/>
-      <c r="O36" s="3"/>
-      <c r="P36" s="3"/>
-      <c r="Q36" s="3"/>
-      <c r="R36" s="3"/>
-      <c r="S36" s="3"/>
-      <c r="T36" s="3"/>
-      <c r="U36" s="3"/>
-      <c r="V36" s="3"/>
-    </row>
-    <row r="37" spans="1:22" s="10" customFormat="1" ht="13">
-      <c r="A37" s="23"/>
-      <c r="B37" s="34" t="s">
+      <c r="N37" s="40"/>
+      <c r="O37" s="3"/>
+      <c r="P37" s="3"/>
+      <c r="Q37" s="3"/>
+      <c r="R37" s="3"/>
+      <c r="S37" s="3"/>
+      <c r="T37" s="3"/>
+      <c r="U37" s="3"/>
+      <c r="V37" s="3"/>
+    </row>
+    <row r="38" spans="1:22" s="10" customFormat="1" ht="13">
+      <c r="A38" s="22"/>
+      <c r="B38" s="33" t="s">
         <v>213</v>
       </c>
-      <c r="C37" s="34" t="s">
+      <c r="C38" s="33" t="s">
         <v>212</v>
       </c>
-      <c r="D37" s="23"/>
-      <c r="E37" s="23"/>
-      <c r="F37" s="34" t="s">
+      <c r="D38" s="22"/>
+      <c r="E38" s="22"/>
+      <c r="F38" s="33" t="s">
         <v>206</v>
       </c>
-      <c r="G37" s="23" t="s">
+      <c r="G38" s="22" t="s">
         <v>209</v>
       </c>
-      <c r="H37" s="23" t="s">
+      <c r="H38" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="I37" s="34" t="s">
+      <c r="I38" s="33" t="s">
         <v>210</v>
       </c>
-      <c r="J37" s="70" t="s">
+      <c r="J38" s="68" t="s">
         <v>211</v>
       </c>
-      <c r="K37" s="76"/>
-      <c r="L37" s="36">
+      <c r="K38" s="74"/>
+      <c r="L38" s="35">
         <v>4376</v>
       </c>
-      <c r="M37" s="25" t="s">
+      <c r="M38" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="N37" s="23"/>
-      <c r="O37" s="12"/>
-      <c r="P37" s="12"/>
-      <c r="Q37" s="12"/>
-      <c r="R37" s="12"/>
-      <c r="S37" s="12"/>
-      <c r="T37" s="12"/>
-      <c r="U37" s="12"/>
-      <c r="V37" s="12"/>
-    </row>
-    <row r="38" spans="1:22" ht="13">
-      <c r="A38" s="17" t="s">
+      <c r="N38" s="22"/>
+      <c r="O38" s="12"/>
+      <c r="P38" s="12"/>
+      <c r="Q38" s="12"/>
+      <c r="R38" s="12"/>
+      <c r="S38" s="12"/>
+      <c r="T38" s="12"/>
+      <c r="U38" s="12"/>
+      <c r="V38" s="12"/>
+    </row>
+    <row r="39" spans="1:22" ht="13">
+      <c r="A39" s="92" t="s">
         <v>170</v>
       </c>
-      <c r="B38" s="17"/>
-      <c r="C38" s="17"/>
-      <c r="D38" s="17"/>
-      <c r="E38" s="17"/>
-      <c r="F38" s="17"/>
-      <c r="G38" s="17"/>
-      <c r="H38" s="17"/>
-      <c r="I38" s="17"/>
-      <c r="J38" s="17"/>
-      <c r="K38" s="17"/>
-      <c r="L38" s="17"/>
-      <c r="M38" s="17"/>
-      <c r="N38" s="17"/>
-      <c r="O38" s="2"/>
-      <c r="P38" s="2"/>
-      <c r="Q38" s="2"/>
-      <c r="R38" s="2"/>
-      <c r="S38" s="2"/>
-      <c r="T38" s="2"/>
-      <c r="U38" s="2"/>
-      <c r="V38" s="2"/>
-    </row>
-    <row r="39" spans="1:22" ht="13">
-      <c r="A39" s="41"/>
-      <c r="B39" s="81" t="s">
-        <v>171</v>
-      </c>
-      <c r="C39" s="82" t="s">
-        <v>172</v>
-      </c>
-      <c r="D39" s="41"/>
-      <c r="E39" s="41"/>
-      <c r="F39" s="81" t="s">
-        <v>173</v>
-      </c>
-      <c r="G39" s="81" t="s">
-        <v>174</v>
-      </c>
-      <c r="H39" s="81" t="s">
-        <v>21</v>
-      </c>
-      <c r="I39" s="81" t="s">
-        <v>175</v>
-      </c>
-      <c r="J39" s="83" t="s">
-        <v>176</v>
-      </c>
-      <c r="K39" s="79"/>
-      <c r="L39" s="42" t="s">
-        <v>177</v>
-      </c>
-      <c r="M39" s="42" t="s">
-        <v>60</v>
-      </c>
-      <c r="N39" s="41" t="s">
-        <v>178</v>
-      </c>
+      <c r="B39" s="92"/>
+      <c r="C39" s="92"/>
+      <c r="D39" s="92"/>
+      <c r="E39" s="92"/>
+      <c r="F39" s="92"/>
+      <c r="G39" s="92"/>
+      <c r="H39" s="92"/>
+      <c r="I39" s="92"/>
+      <c r="J39" s="92"/>
+      <c r="K39" s="92"/>
+      <c r="L39" s="92"/>
+      <c r="M39" s="92"/>
+      <c r="N39" s="92"/>
       <c r="O39" s="2"/>
       <c r="P39" s="2"/>
       <c r="Q39" s="2"/>
@@ -2943,195 +2985,193 @@
       <c r="U39" s="2"/>
       <c r="V39" s="2"/>
     </row>
-    <row r="40" spans="1:22" s="8" customFormat="1" ht="13">
-      <c r="A40" s="23"/>
-      <c r="B40" s="24" t="s">
+    <row r="40" spans="1:22" ht="13">
+      <c r="A40" s="40"/>
+      <c r="B40" s="79" t="s">
+        <v>171</v>
+      </c>
+      <c r="C40" s="80" t="s">
+        <v>172</v>
+      </c>
+      <c r="D40" s="40"/>
+      <c r="E40" s="40"/>
+      <c r="F40" s="79" t="s">
+        <v>173</v>
+      </c>
+      <c r="G40" s="79" t="s">
+        <v>174</v>
+      </c>
+      <c r="H40" s="79" t="s">
+        <v>21</v>
+      </c>
+      <c r="I40" s="79" t="s">
+        <v>175</v>
+      </c>
+      <c r="J40" s="81" t="s">
+        <v>176</v>
+      </c>
+      <c r="K40" s="77"/>
+      <c r="L40" s="41" t="s">
+        <v>177</v>
+      </c>
+      <c r="M40" s="41" t="s">
+        <v>60</v>
+      </c>
+      <c r="N40" s="40" t="s">
+        <v>178</v>
+      </c>
+      <c r="O40" s="2"/>
+      <c r="P40" s="2"/>
+      <c r="Q40" s="2"/>
+      <c r="R40" s="2"/>
+      <c r="S40" s="2"/>
+      <c r="T40" s="2"/>
+      <c r="U40" s="2"/>
+      <c r="V40" s="2"/>
+    </row>
+    <row r="41" spans="1:22" s="8" customFormat="1" ht="13">
+      <c r="A41" s="22"/>
+      <c r="B41" s="23" t="s">
         <v>251</v>
       </c>
-      <c r="C40" s="84" t="s">
+      <c r="C41" s="82" t="s">
         <v>172</v>
       </c>
-      <c r="D40" s="23"/>
-      <c r="E40" s="23"/>
-      <c r="F40" s="24" t="s">
+      <c r="D41" s="22"/>
+      <c r="E41" s="22"/>
+      <c r="F41" s="23" t="s">
         <v>250</v>
       </c>
-      <c r="G40" s="85" t="s">
+      <c r="G41" s="83" t="s">
         <v>249</v>
       </c>
-      <c r="H40" s="85" t="s">
+      <c r="H41" s="83" t="s">
         <v>21</v>
       </c>
-      <c r="I40" s="24" t="s">
+      <c r="I41" s="23" t="s">
         <v>252</v>
       </c>
-      <c r="J40" s="27" t="s">
+      <c r="J41" s="26" t="s">
         <v>253</v>
       </c>
-      <c r="K40" s="76"/>
-      <c r="L40" s="25" t="s">
+      <c r="K41" s="74"/>
+      <c r="L41" s="24" t="s">
         <v>254</v>
       </c>
-      <c r="M40" s="25" t="s">
+      <c r="M41" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="N40" s="23"/>
-      <c r="O40" s="7"/>
-      <c r="P40" s="7"/>
-      <c r="Q40" s="7"/>
-      <c r="R40" s="7"/>
-      <c r="S40" s="7"/>
-      <c r="T40" s="7"/>
-      <c r="U40" s="7"/>
-      <c r="V40" s="7"/>
-    </row>
-    <row r="41" spans="1:22" s="14" customFormat="1" ht="13">
-      <c r="A41" s="18"/>
-      <c r="B41" s="29" t="s">
+      <c r="N41" s="22"/>
+      <c r="O41" s="7"/>
+      <c r="P41" s="7"/>
+      <c r="Q41" s="7"/>
+      <c r="R41" s="7"/>
+      <c r="S41" s="7"/>
+      <c r="T41" s="7"/>
+      <c r="U41" s="7"/>
+      <c r="V41" s="7"/>
+    </row>
+    <row r="42" spans="1:22" s="14" customFormat="1" ht="13">
+      <c r="A42" s="17"/>
+      <c r="B42" s="28" t="s">
         <v>215</v>
       </c>
-      <c r="C41" s="29" t="s">
+      <c r="C42" s="28" t="s">
         <v>216</v>
       </c>
-      <c r="D41" s="18"/>
-      <c r="E41" s="18"/>
-      <c r="F41" s="29" t="s">
+      <c r="D42" s="17"/>
+      <c r="E42" s="17"/>
+      <c r="F42" s="28" t="s">
         <v>217</v>
       </c>
-      <c r="G41" s="86" t="s">
+      <c r="G42" s="84" t="s">
         <v>214</v>
       </c>
-      <c r="H41" s="86" t="s">
+      <c r="H42" s="84" t="s">
         <v>21</v>
       </c>
-      <c r="I41" s="29" t="s">
+      <c r="I42" s="28" t="s">
         <v>219</v>
       </c>
-      <c r="J41" s="30" t="s">
+      <c r="J42" s="29" t="s">
         <v>218</v>
       </c>
-      <c r="K41" s="87"/>
-      <c r="L41" s="31">
+      <c r="K42" s="85"/>
+      <c r="L42" s="30">
         <v>392</v>
       </c>
-      <c r="M41" s="20" t="s">
+      <c r="M42" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="N41" s="18"/>
-      <c r="O41" s="5"/>
-      <c r="P41" s="5"/>
-      <c r="Q41" s="5"/>
-      <c r="R41" s="5"/>
-      <c r="S41" s="5"/>
-      <c r="T41" s="5"/>
-      <c r="U41" s="5"/>
-      <c r="V41" s="5"/>
-    </row>
-    <row r="42" spans="1:22" s="10" customFormat="1" ht="13">
-      <c r="A42" s="23"/>
-      <c r="B42" s="34" t="s">
+      <c r="N42" s="17"/>
+      <c r="O42" s="5"/>
+      <c r="P42" s="5"/>
+      <c r="Q42" s="5"/>
+      <c r="R42" s="5"/>
+      <c r="S42" s="5"/>
+      <c r="T42" s="5"/>
+      <c r="U42" s="5"/>
+      <c r="V42" s="5"/>
+    </row>
+    <row r="43" spans="1:22" s="10" customFormat="1" ht="13">
+      <c r="A43" s="22"/>
+      <c r="B43" s="33" t="s">
         <v>230</v>
       </c>
-      <c r="C42" s="34" t="s">
+      <c r="C43" s="33" t="s">
         <v>229</v>
       </c>
-      <c r="D42" s="23"/>
-      <c r="E42" s="23"/>
-      <c r="F42" s="34" t="s">
+      <c r="D43" s="22"/>
+      <c r="E43" s="22"/>
+      <c r="F43" s="33" t="s">
         <v>228</v>
       </c>
-      <c r="G42" s="34" t="s">
+      <c r="G43" s="33" t="s">
         <v>226</v>
       </c>
-      <c r="H42" s="85" t="s">
+      <c r="H43" s="83" t="s">
         <v>21</v>
       </c>
-      <c r="I42" s="34" t="s">
+      <c r="I43" s="33" t="s">
         <v>227</v>
       </c>
-      <c r="J42" s="70" t="s">
+      <c r="J43" s="68" t="s">
         <v>231</v>
       </c>
-      <c r="K42" s="76"/>
-      <c r="L42" s="36">
+      <c r="K43" s="74"/>
+      <c r="L43" s="35">
         <v>41306</v>
       </c>
-      <c r="M42" s="25" t="s">
+      <c r="M43" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="N42" s="23"/>
-      <c r="O42" s="7"/>
-      <c r="P42" s="7"/>
-      <c r="Q42" s="7"/>
-      <c r="R42" s="7"/>
-      <c r="S42" s="7"/>
-      <c r="T42" s="7"/>
-      <c r="U42" s="7"/>
-      <c r="V42" s="7"/>
-    </row>
-    <row r="43" spans="1:22" ht="13">
-      <c r="A43" s="17" t="s">
+      <c r="N43" s="22"/>
+      <c r="O43" s="7"/>
+      <c r="P43" s="7"/>
+      <c r="Q43" s="7"/>
+      <c r="R43" s="7"/>
+      <c r="S43" s="7"/>
+      <c r="T43" s="7"/>
+      <c r="U43" s="7"/>
+      <c r="V43" s="7"/>
+    </row>
+    <row r="44" spans="1:22" ht="13">
+      <c r="A44" s="92" t="s">
         <v>179</v>
       </c>
-      <c r="B43" s="17"/>
-      <c r="C43" s="17"/>
-      <c r="D43" s="17"/>
-      <c r="E43" s="17"/>
-      <c r="F43" s="17"/>
-      <c r="G43" s="17"/>
-      <c r="H43" s="17"/>
-      <c r="I43" s="17"/>
-      <c r="J43" s="17"/>
-      <c r="K43" s="17"/>
-      <c r="L43" s="17"/>
-      <c r="M43" s="17"/>
-      <c r="N43" s="17"/>
-      <c r="O43" s="2"/>
-      <c r="P43" s="2"/>
-      <c r="Q43" s="2"/>
-      <c r="R43" s="2"/>
-      <c r="S43" s="2"/>
-      <c r="T43" s="2"/>
-      <c r="U43" s="2"/>
-      <c r="V43" s="2"/>
-    </row>
-    <row r="44" spans="1:22" ht="13">
-      <c r="A44" s="41"/>
-      <c r="B44" s="88" t="s">
-        <v>180</v>
-      </c>
-      <c r="C44" s="45" t="s">
-        <v>181</v>
-      </c>
-      <c r="D44" s="41" t="s">
-        <v>182</v>
-      </c>
-      <c r="E44" s="41"/>
-      <c r="F44" s="43" t="s">
-        <v>183</v>
-      </c>
-      <c r="G44" s="43" t="s">
-        <v>184</v>
-      </c>
-      <c r="H44" s="41" t="s">
-        <v>21</v>
-      </c>
-      <c r="I44" s="43" t="s">
-        <v>185</v>
-      </c>
-      <c r="J44" s="89" t="s">
-        <v>186</v>
-      </c>
-      <c r="K44" s="79"/>
-      <c r="L44" s="90" t="s">
-        <v>187</v>
-      </c>
-      <c r="M44" s="42" t="s">
-        <v>60</v>
-      </c>
-      <c r="N44" s="41" t="s">
-        <v>188</v>
-      </c>
+      <c r="B44" s="92"/>
+      <c r="C44" s="92"/>
+      <c r="D44" s="92"/>
+      <c r="E44" s="92"/>
+      <c r="F44" s="92"/>
+      <c r="G44" s="92"/>
+      <c r="H44" s="92"/>
+      <c r="I44" s="92"/>
+      <c r="J44" s="92"/>
+      <c r="K44" s="92"/>
+      <c r="L44" s="92"/>
+      <c r="M44" s="92"/>
+      <c r="N44" s="92"/>
       <c r="O44" s="2"/>
       <c r="P44" s="2"/>
       <c r="Q44" s="2"/>
@@ -3142,40 +3182,42 @@
       <c r="V44" s="2"/>
     </row>
     <row r="45" spans="1:22" ht="13">
-      <c r="A45" s="46"/>
-      <c r="B45" s="47" t="s">
-        <v>189</v>
-      </c>
-      <c r="C45" s="50" t="s">
-        <v>190</v>
-      </c>
-      <c r="D45" s="46" t="s">
-        <v>191</v>
-      </c>
-      <c r="E45" s="46"/>
-      <c r="F45" s="47" t="s">
+      <c r="A45" s="40"/>
+      <c r="B45" s="86" t="s">
+        <v>180</v>
+      </c>
+      <c r="C45" s="44" t="s">
+        <v>181</v>
+      </c>
+      <c r="D45" s="40" t="s">
+        <v>182</v>
+      </c>
+      <c r="E45" s="40"/>
+      <c r="F45" s="42" t="s">
         <v>183</v>
       </c>
-      <c r="G45" s="46" t="s">
-        <v>192</v>
-      </c>
-      <c r="H45" s="46" t="s">
+      <c r="G45" s="42" t="s">
+        <v>184</v>
+      </c>
+      <c r="H45" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="I45" s="47" t="s">
-        <v>193</v>
-      </c>
-      <c r="J45" s="49" t="s">
-        <v>194</v>
-      </c>
-      <c r="K45" s="46"/>
-      <c r="L45" s="91">
-        <v>2019</v>
-      </c>
-      <c r="M45" s="48" t="s">
+      <c r="I45" s="42" t="s">
+        <v>185</v>
+      </c>
+      <c r="J45" s="87" t="s">
+        <v>186</v>
+      </c>
+      <c r="K45" s="77"/>
+      <c r="L45" s="88" t="s">
+        <v>187</v>
+      </c>
+      <c r="M45" s="41" t="s">
         <v>60</v>
       </c>
-      <c r="N45" s="46"/>
+      <c r="N45" s="40" t="s">
+        <v>188</v>
+      </c>
       <c r="O45" s="2"/>
       <c r="P45" s="2"/>
       <c r="Q45" s="2"/>
@@ -3183,24 +3225,43 @@
       <c r="S45" s="2"/>
       <c r="T45" s="2"/>
       <c r="U45" s="2"/>
+      <c r="V45" s="2"/>
     </row>
     <row r="46" spans="1:22" ht="13">
-      <c r="A46" s="17" t="s">
-        <v>220</v>
-      </c>
-      <c r="B46" s="17"/>
-      <c r="C46" s="17"/>
-      <c r="D46" s="17"/>
-      <c r="E46" s="17"/>
-      <c r="F46" s="17"/>
-      <c r="G46" s="17"/>
-      <c r="H46" s="17"/>
-      <c r="I46" s="17"/>
-      <c r="J46" s="17"/>
-      <c r="K46" s="17"/>
-      <c r="L46" s="17"/>
-      <c r="M46" s="17"/>
-      <c r="N46" s="17"/>
+      <c r="A46" s="45"/>
+      <c r="B46" s="46" t="s">
+        <v>189</v>
+      </c>
+      <c r="C46" s="49" t="s">
+        <v>190</v>
+      </c>
+      <c r="D46" s="45" t="s">
+        <v>191</v>
+      </c>
+      <c r="E46" s="45"/>
+      <c r="F46" s="46" t="s">
+        <v>183</v>
+      </c>
+      <c r="G46" s="45" t="s">
+        <v>192</v>
+      </c>
+      <c r="H46" s="45" t="s">
+        <v>21</v>
+      </c>
+      <c r="I46" s="46" t="s">
+        <v>193</v>
+      </c>
+      <c r="J46" s="48" t="s">
+        <v>194</v>
+      </c>
+      <c r="K46" s="45"/>
+      <c r="L46" s="89">
+        <v>2019</v>
+      </c>
+      <c r="M46" s="47" t="s">
+        <v>60</v>
+      </c>
+      <c r="N46" s="45"/>
       <c r="O46" s="2"/>
       <c r="P46" s="2"/>
       <c r="Q46" s="2"/>
@@ -3208,63 +3269,64 @@
       <c r="S46" s="2"/>
       <c r="T46" s="2"/>
       <c r="U46" s="2"/>
-      <c r="V46" s="2"/>
-    </row>
-    <row r="47" spans="1:22" s="4" customFormat="1" ht="13">
-      <c r="A47" s="92"/>
-      <c r="B47" s="77" t="s">
-        <v>225</v>
-      </c>
+    </row>
+    <row r="47" spans="1:22" ht="13">
+      <c r="A47" s="92" t="s">
+        <v>220</v>
+      </c>
+      <c r="B47" s="92"/>
       <c r="C47" s="92"/>
       <c r="D47" s="92"/>
       <c r="E47" s="92"/>
-      <c r="F47" s="77" t="s">
+      <c r="F47" s="92"/>
+      <c r="G47" s="92"/>
+      <c r="H47" s="92"/>
+      <c r="I47" s="92"/>
+      <c r="J47" s="92"/>
+      <c r="K47" s="92"/>
+      <c r="L47" s="92"/>
+      <c r="M47" s="92"/>
+      <c r="N47" s="92"/>
+      <c r="O47" s="2"/>
+      <c r="P47" s="2"/>
+      <c r="Q47" s="2"/>
+      <c r="R47" s="2"/>
+      <c r="S47" s="2"/>
+      <c r="T47" s="2"/>
+      <c r="U47" s="2"/>
+      <c r="V47" s="2"/>
+    </row>
+    <row r="48" spans="1:22" s="4" customFormat="1" ht="13">
+      <c r="A48" s="90"/>
+      <c r="B48" s="75" t="s">
+        <v>225</v>
+      </c>
+      <c r="C48" s="90"/>
+      <c r="D48" s="90"/>
+      <c r="E48" s="90"/>
+      <c r="F48" s="75" t="s">
         <v>221</v>
       </c>
-      <c r="G47" s="77" t="s">
+      <c r="G48" s="75" t="s">
         <v>222</v>
       </c>
-      <c r="H47" s="41" t="s">
+      <c r="H48" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="I47" s="77" t="s">
+      <c r="I48" s="75" t="s">
         <v>223</v>
       </c>
-      <c r="J47" s="78" t="s">
+      <c r="J48" s="76" t="s">
         <v>224</v>
       </c>
-      <c r="K47" s="92"/>
-      <c r="L47" s="80">
+      <c r="K48" s="90"/>
+      <c r="L48" s="78">
         <v>4957</v>
       </c>
-      <c r="M47" s="42" t="s">
+      <c r="M48" s="41" t="s">
         <v>60</v>
       </c>
-      <c r="N47" s="92"/>
-      <c r="O47" s="1"/>
-      <c r="P47" s="1"/>
-      <c r="Q47" s="1"/>
-      <c r="R47" s="1"/>
-      <c r="S47" s="1"/>
-      <c r="T47" s="1"/>
-      <c r="U47" s="1"/>
-      <c r="V47" s="1"/>
-    </row>
-    <row r="48" spans="1:22" ht="12.5" hidden="1">
-      <c r="A48" s="1"/>
-      <c r="B48" s="1"/>
-      <c r="C48" s="1"/>
-      <c r="D48" s="1"/>
-      <c r="E48" s="1"/>
-      <c r="F48" s="1"/>
-      <c r="G48" s="1"/>
-      <c r="H48" s="1"/>
-      <c r="I48" s="1"/>
-      <c r="J48" s="1"/>
-      <c r="K48" s="1"/>
-      <c r="L48" s="1"/>
-      <c r="M48" s="1"/>
-      <c r="N48" s="1"/>
+      <c r="N48" s="90"/>
       <c r="O48" s="1"/>
       <c r="P48" s="1"/>
       <c r="Q48" s="1"/>
@@ -24970,17 +25032,41 @@
       <c r="U952" s="1"/>
       <c r="V952" s="1"/>
     </row>
+    <row r="953" spans="1:22" ht="12.5" hidden="1">
+      <c r="A953" s="1"/>
+      <c r="B953" s="1"/>
+      <c r="C953" s="1"/>
+      <c r="D953" s="1"/>
+      <c r="E953" s="1"/>
+      <c r="F953" s="1"/>
+      <c r="G953" s="1"/>
+      <c r="H953" s="1"/>
+      <c r="I953" s="1"/>
+      <c r="J953" s="1"/>
+      <c r="K953" s="1"/>
+      <c r="L953" s="1"/>
+      <c r="M953" s="1"/>
+      <c r="N953" s="1"/>
+      <c r="O953" s="1"/>
+      <c r="P953" s="1"/>
+      <c r="Q953" s="1"/>
+      <c r="R953" s="1"/>
+      <c r="S953" s="1"/>
+      <c r="T953" s="1"/>
+      <c r="U953" s="1"/>
+      <c r="V953" s="1"/>
+    </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="A31:N31"/>
-    <mergeCell ref="A38:N38"/>
-    <mergeCell ref="A43:N43"/>
-    <mergeCell ref="A46:N46"/>
+    <mergeCell ref="A32:N32"/>
+    <mergeCell ref="A39:N39"/>
+    <mergeCell ref="A44:N44"/>
+    <mergeCell ref="A47:N47"/>
     <mergeCell ref="A1:N1"/>
     <mergeCell ref="A3:N3"/>
     <mergeCell ref="A14:N14"/>
     <mergeCell ref="A25:N25"/>
-    <mergeCell ref="A29:N29"/>
+    <mergeCell ref="A30:N30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Adding TLV62569DBVR to BOM
</commit_message>
<xml_diff>
--- a/BOM/MIMXRT1064 MCU Module  - BOM.xlsx
+++ b/BOM/MIMXRT1064 MCU Module  - BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\32470\Documents\GitHub\MIMXRT1064-MCU-Module\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41749008-04AA-43FC-B02E-842824F829C6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53C424A2-76DF-4996-B997-D395DE352795}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="265">
   <si>
     <t>MIMXRT1064 MCU Module  - BOM</t>
   </si>
@@ -807,6 +807,15 @@
   </si>
   <si>
     <t>$0.081</t>
+  </si>
+  <si>
+    <t>TLV62569DBVR</t>
+  </si>
+  <si>
+    <t>C141836</t>
+  </si>
+  <si>
+    <t>$0.0942</t>
   </si>
 </sst>
 </file>
@@ -988,7 +997,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="101">
+  <cellXfs count="100">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1018,10 +1027,8 @@
     </xf>
     <xf numFmtId="49" fontId="5" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="4" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="5" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -1060,9 +1067,7 @@
     </xf>
     <xf numFmtId="49" fontId="5" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="4" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1124,21 +1129,10 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="49" fontId="5" fillId="14" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="14" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1148,6 +1142,26 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1368,10 +1382,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:V953"/>
+  <dimension ref="A1:V954"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45:N45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15.75" customHeight="1" zeroHeight="1"/>
@@ -1394,22 +1408,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="30" customHeight="1">
-      <c r="A1" s="93" t="s">
+      <c r="A1" s="94" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="93"/>
-      <c r="C1" s="93"/>
-      <c r="D1" s="93"/>
-      <c r="E1" s="93"/>
-      <c r="F1" s="93"/>
-      <c r="G1" s="93"/>
-      <c r="H1" s="93"/>
-      <c r="I1" s="93"/>
-      <c r="J1" s="93"/>
-      <c r="K1" s="93"/>
-      <c r="L1" s="93"/>
-      <c r="M1" s="93"/>
-      <c r="N1" s="93"/>
+      <c r="B1" s="94"/>
+      <c r="C1" s="94"/>
+      <c r="D1" s="94"/>
+      <c r="E1" s="94"/>
+      <c r="F1" s="94"/>
+      <c r="G1" s="94"/>
+      <c r="H1" s="94"/>
+      <c r="I1" s="94"/>
+      <c r="J1" s="94"/>
+      <c r="K1" s="94"/>
+      <c r="L1" s="94"/>
+      <c r="M1" s="94"/>
+      <c r="N1" s="94"/>
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
@@ -1472,22 +1486,22 @@
       <c r="V2" s="1"/>
     </row>
     <row r="3" spans="1:22" ht="13">
-      <c r="A3" s="92" t="s">
+      <c r="A3" s="93" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="92"/>
-      <c r="C3" s="92"/>
-      <c r="D3" s="92"/>
-      <c r="E3" s="92"/>
-      <c r="F3" s="92"/>
-      <c r="G3" s="92"/>
-      <c r="H3" s="92"/>
-      <c r="I3" s="92"/>
-      <c r="J3" s="92"/>
-      <c r="K3" s="92"/>
-      <c r="L3" s="92"/>
-      <c r="M3" s="92"/>
-      <c r="N3" s="92"/>
+      <c r="B3" s="93"/>
+      <c r="C3" s="93"/>
+      <c r="D3" s="93"/>
+      <c r="E3" s="93"/>
+      <c r="F3" s="93"/>
+      <c r="G3" s="93"/>
+      <c r="H3" s="93"/>
+      <c r="I3" s="93"/>
+      <c r="J3" s="93"/>
+      <c r="K3" s="93"/>
+      <c r="L3" s="93"/>
+      <c r="M3" s="93"/>
+      <c r="N3" s="93"/>
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
@@ -1543,10 +1557,10 @@
     </row>
     <row r="5" spans="1:22" s="8" customFormat="1" ht="13">
       <c r="A5" s="22"/>
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="31" t="s">
         <v>248</v>
       </c>
-      <c r="C5" s="24" t="s">
+      <c r="C5" s="23" t="s">
         <v>26</v>
       </c>
       <c r="D5" s="22" t="s">
@@ -1556,23 +1570,23 @@
       <c r="F5" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="G5" s="25" t="s">
+      <c r="G5" s="24" t="s">
         <v>245</v>
       </c>
       <c r="H5" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="I5" s="23" t="s">
+      <c r="I5" s="31" t="s">
         <v>247</v>
       </c>
-      <c r="J5" s="26" t="s">
+      <c r="J5" s="64" t="s">
         <v>28</v>
       </c>
       <c r="K5" s="22"/>
-      <c r="L5" s="27" t="s">
+      <c r="L5" s="25" t="s">
         <v>246</v>
       </c>
-      <c r="M5" s="24" t="s">
+      <c r="M5" s="23" t="s">
         <v>25</v>
       </c>
       <c r="N5" s="22"/>
@@ -1606,14 +1620,14 @@
       <c r="H6" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="I6" s="28" t="s">
+      <c r="I6" s="26" t="s">
         <v>201</v>
       </c>
-      <c r="J6" s="29" t="s">
+      <c r="J6" s="27" t="s">
         <v>202</v>
       </c>
       <c r="K6" s="17"/>
-      <c r="L6" s="30">
+      <c r="L6" s="28">
         <v>4500</v>
       </c>
       <c r="M6" s="19" t="s">
@@ -1630,40 +1644,40 @@
       <c r="V6" s="5"/>
     </row>
     <row r="7" spans="1:22" s="8" customFormat="1" ht="13">
-      <c r="A7" s="31"/>
-      <c r="B7" s="25" t="s">
+      <c r="A7" s="29"/>
+      <c r="B7" s="24" t="s">
         <v>199</v>
       </c>
-      <c r="C7" s="32" t="s">
+      <c r="C7" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="31" t="s">
+      <c r="D7" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="31"/>
-      <c r="F7" s="31" t="s">
+      <c r="E7" s="29"/>
+      <c r="F7" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="G7" s="31" t="s">
+      <c r="G7" s="29" t="s">
         <v>195</v>
       </c>
-      <c r="H7" s="31" t="s">
+      <c r="H7" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="I7" s="33" t="s">
+      <c r="I7" s="31" t="s">
         <v>196</v>
       </c>
-      <c r="J7" s="34" t="s">
+      <c r="J7" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="K7" s="31"/>
-      <c r="L7" s="35">
+      <c r="K7" s="29"/>
+      <c r="L7" s="33">
         <v>751492</v>
       </c>
-      <c r="M7" s="32" t="s">
+      <c r="M7" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="N7" s="31"/>
+      <c r="N7" s="29"/>
       <c r="O7" s="13"/>
       <c r="P7" s="13"/>
       <c r="Q7" s="13"/>
@@ -1718,40 +1732,40 @@
       <c r="V8" s="5"/>
     </row>
     <row r="9" spans="1:22" s="8" customFormat="1" ht="13">
-      <c r="A9" s="31"/>
-      <c r="B9" s="36" t="s">
+      <c r="A9" s="29"/>
+      <c r="B9" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="C9" s="32" t="s">
+      <c r="C9" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="31" t="s">
+      <c r="D9" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="E9" s="31"/>
-      <c r="F9" s="31" t="s">
+      <c r="E9" s="29"/>
+      <c r="F9" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="G9" s="36" t="s">
+      <c r="G9" s="34" t="s">
         <v>37</v>
       </c>
-      <c r="H9" s="31" t="s">
+      <c r="H9" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="I9" s="37" t="s">
+      <c r="I9" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="J9" s="38" t="s">
+      <c r="J9" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="K9" s="31"/>
-      <c r="L9" s="39" t="s">
+      <c r="K9" s="29"/>
+      <c r="L9" s="37" t="s">
         <v>39</v>
       </c>
-      <c r="M9" s="32" t="s">
+      <c r="M9" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="N9" s="31"/>
+      <c r="N9" s="29"/>
       <c r="O9" s="13"/>
       <c r="P9" s="13"/>
       <c r="Q9" s="13"/>
@@ -1806,40 +1820,40 @@
       <c r="V10" s="5"/>
     </row>
     <row r="11" spans="1:22" s="8" customFormat="1" ht="17.25" customHeight="1">
-      <c r="A11" s="31"/>
-      <c r="B11" s="36" t="s">
+      <c r="A11" s="29"/>
+      <c r="B11" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="C11" s="32" t="s">
+      <c r="C11" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="31" t="s">
+      <c r="D11" s="29" t="s">
         <v>46</v>
       </c>
-      <c r="E11" s="31"/>
-      <c r="F11" s="31" t="s">
+      <c r="E11" s="29"/>
+      <c r="F11" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="G11" s="36" t="s">
+      <c r="G11" s="34" t="s">
         <v>47</v>
       </c>
-      <c r="H11" s="31" t="s">
+      <c r="H11" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="I11" s="36" t="s">
+      <c r="I11" s="34" t="s">
         <v>48</v>
       </c>
-      <c r="J11" s="38" t="s">
+      <c r="J11" s="36" t="s">
         <v>33</v>
       </c>
-      <c r="K11" s="31"/>
-      <c r="L11" s="39" t="s">
+      <c r="K11" s="29"/>
+      <c r="L11" s="37" t="s">
         <v>49</v>
       </c>
-      <c r="M11" s="32" t="s">
+      <c r="M11" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="N11" s="31"/>
+      <c r="N11" s="29"/>
       <c r="O11" s="13"/>
       <c r="P11" s="13"/>
       <c r="Q11" s="13"/>
@@ -1894,40 +1908,40 @@
       <c r="V12" s="5"/>
     </row>
     <row r="13" spans="1:22" s="8" customFormat="1" ht="13">
-      <c r="A13" s="31"/>
-      <c r="B13" s="36" t="s">
+      <c r="A13" s="29"/>
+      <c r="B13" s="34" t="s">
         <v>55</v>
       </c>
-      <c r="C13" s="32" t="s">
+      <c r="C13" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="D13" s="31" t="s">
+      <c r="D13" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="E13" s="31"/>
-      <c r="F13" s="31" t="s">
+      <c r="E13" s="29"/>
+      <c r="F13" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="G13" s="36" t="s">
+      <c r="G13" s="34" t="s">
         <v>57</v>
       </c>
-      <c r="H13" s="31" t="s">
+      <c r="H13" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="I13" s="36" t="s">
+      <c r="I13" s="34" t="s">
         <v>58</v>
       </c>
-      <c r="J13" s="38" t="s">
+      <c r="J13" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="K13" s="31"/>
-      <c r="L13" s="39" t="s">
+      <c r="K13" s="29"/>
+      <c r="L13" s="37" t="s">
         <v>59</v>
       </c>
-      <c r="M13" s="32" t="s">
+      <c r="M13" s="30" t="s">
         <v>60</v>
       </c>
-      <c r="N13" s="31"/>
+      <c r="N13" s="29"/>
       <c r="O13" s="13"/>
       <c r="P13" s="13"/>
       <c r="Q13" s="13"/>
@@ -1938,22 +1952,22 @@
       <c r="V13" s="13"/>
     </row>
     <row r="14" spans="1:22" ht="13">
-      <c r="A14" s="92" t="s">
+      <c r="A14" s="93" t="s">
         <v>61</v>
       </c>
-      <c r="B14" s="92"/>
-      <c r="C14" s="92"/>
-      <c r="D14" s="92"/>
-      <c r="E14" s="92"/>
-      <c r="F14" s="92"/>
-      <c r="G14" s="92"/>
-      <c r="H14" s="92"/>
-      <c r="I14" s="92"/>
-      <c r="J14" s="92"/>
-      <c r="K14" s="92"/>
-      <c r="L14" s="92"/>
-      <c r="M14" s="92"/>
-      <c r="N14" s="92"/>
+      <c r="B14" s="93"/>
+      <c r="C14" s="93"/>
+      <c r="D14" s="93"/>
+      <c r="E14" s="93"/>
+      <c r="F14" s="93"/>
+      <c r="G14" s="93"/>
+      <c r="H14" s="93"/>
+      <c r="I14" s="93"/>
+      <c r="J14" s="93"/>
+      <c r="K14" s="93"/>
+      <c r="L14" s="93"/>
+      <c r="M14" s="93"/>
+      <c r="N14" s="93"/>
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
       <c r="Q14" s="1"/>
@@ -1964,40 +1978,40 @@
       <c r="V14" s="1"/>
     </row>
     <row r="15" spans="1:22" ht="13">
-      <c r="A15" s="40"/>
-      <c r="B15" s="40" t="s">
+      <c r="A15" s="38"/>
+      <c r="B15" s="38" t="s">
         <v>62</v>
       </c>
-      <c r="C15" s="41" t="s">
+      <c r="C15" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="D15" s="40" t="s">
+      <c r="D15" s="38" t="s">
         <v>63</v>
       </c>
-      <c r="E15" s="40"/>
-      <c r="F15" s="42" t="s">
+      <c r="E15" s="38"/>
+      <c r="F15" s="40" t="s">
         <v>64</v>
       </c>
-      <c r="G15" s="40" t="s">
+      <c r="G15" s="38" t="s">
         <v>65</v>
       </c>
-      <c r="H15" s="40" t="s">
+      <c r="H15" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="I15" s="42" t="s">
+      <c r="I15" s="40" t="s">
         <v>66</v>
       </c>
-      <c r="J15" s="43" t="s">
+      <c r="J15" s="41" t="s">
         <v>67</v>
       </c>
-      <c r="K15" s="40"/>
-      <c r="L15" s="44" t="s">
+      <c r="K15" s="38"/>
+      <c r="L15" s="42" t="s">
         <v>68</v>
       </c>
-      <c r="M15" s="41" t="s">
+      <c r="M15" s="39" t="s">
         <v>60</v>
       </c>
-      <c r="N15" s="40"/>
+      <c r="N15" s="38"/>
       <c r="O15" s="2"/>
       <c r="P15" s="2"/>
       <c r="Q15" s="2"/>
@@ -2008,40 +2022,40 @@
       <c r="V15" s="2"/>
     </row>
     <row r="16" spans="1:22" ht="13">
-      <c r="A16" s="45"/>
-      <c r="B16" s="46" t="s">
+      <c r="A16" s="43"/>
+      <c r="B16" s="44" t="s">
         <v>69</v>
       </c>
-      <c r="C16" s="47" t="s">
+      <c r="C16" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="D16" s="45" t="s">
+      <c r="D16" s="43" t="s">
         <v>70</v>
       </c>
-      <c r="E16" s="45"/>
-      <c r="F16" s="46" t="s">
+      <c r="E16" s="43"/>
+      <c r="F16" s="44" t="s">
         <v>64</v>
       </c>
-      <c r="G16" s="45" t="s">
+      <c r="G16" s="43" t="s">
         <v>71</v>
       </c>
-      <c r="H16" s="45" t="s">
+      <c r="H16" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="I16" s="46" t="s">
+      <c r="I16" s="44" t="s">
         <v>72</v>
       </c>
-      <c r="J16" s="48" t="s">
+      <c r="J16" s="46" t="s">
         <v>73</v>
       </c>
-      <c r="K16" s="45"/>
-      <c r="L16" s="49" t="s">
+      <c r="K16" s="43"/>
+      <c r="L16" s="47" t="s">
         <v>74</v>
       </c>
-      <c r="M16" s="47" t="s">
+      <c r="M16" s="45" t="s">
         <v>60</v>
       </c>
-      <c r="N16" s="45"/>
+      <c r="N16" s="43"/>
       <c r="O16" s="2"/>
       <c r="P16" s="2"/>
       <c r="Q16" s="2"/>
@@ -2052,40 +2066,40 @@
       <c r="V16" s="2"/>
     </row>
     <row r="17" spans="1:22" ht="13">
-      <c r="A17" s="40"/>
-      <c r="B17" s="40" t="s">
+      <c r="A17" s="38"/>
+      <c r="B17" s="38" t="s">
         <v>75</v>
       </c>
-      <c r="C17" s="41" t="s">
+      <c r="C17" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="D17" s="40" t="s">
+      <c r="D17" s="38" t="s">
         <v>76</v>
       </c>
-      <c r="E17" s="40"/>
-      <c r="F17" s="42" t="s">
+      <c r="E17" s="38"/>
+      <c r="F17" s="40" t="s">
         <v>77</v>
       </c>
-      <c r="G17" s="42" t="s">
+      <c r="G17" s="40" t="s">
         <v>78</v>
       </c>
-      <c r="H17" s="40" t="s">
+      <c r="H17" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="I17" s="42" t="s">
+      <c r="I17" s="40" t="s">
         <v>79</v>
       </c>
-      <c r="J17" s="43" t="s">
+      <c r="J17" s="41" t="s">
         <v>28</v>
       </c>
-      <c r="K17" s="40"/>
-      <c r="L17" s="44" t="s">
+      <c r="K17" s="38"/>
+      <c r="L17" s="42" t="s">
         <v>80</v>
       </c>
-      <c r="M17" s="41" t="s">
+      <c r="M17" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="N17" s="40"/>
+      <c r="N17" s="38"/>
       <c r="O17" s="2"/>
       <c r="P17" s="2"/>
       <c r="Q17" s="2"/>
@@ -2096,40 +2110,40 @@
       <c r="V17" s="2"/>
     </row>
     <row r="18" spans="1:22" ht="13">
-      <c r="A18" s="45"/>
-      <c r="B18" s="45" t="s">
+      <c r="A18" s="43"/>
+      <c r="B18" s="43" t="s">
         <v>81</v>
       </c>
-      <c r="C18" s="47" t="s">
+      <c r="C18" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="D18" s="45" t="s">
+      <c r="D18" s="43" t="s">
         <v>82</v>
       </c>
-      <c r="E18" s="45"/>
-      <c r="F18" s="46" t="s">
+      <c r="E18" s="43"/>
+      <c r="F18" s="44" t="s">
         <v>83</v>
       </c>
-      <c r="G18" s="46" t="s">
+      <c r="G18" s="44" t="s">
         <v>84</v>
       </c>
-      <c r="H18" s="45" t="s">
+      <c r="H18" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="I18" s="46" t="s">
+      <c r="I18" s="44" t="s">
         <v>85</v>
       </c>
-      <c r="J18" s="48" t="s">
+      <c r="J18" s="46" t="s">
         <v>86</v>
       </c>
-      <c r="K18" s="45"/>
-      <c r="L18" s="49" t="s">
+      <c r="K18" s="43"/>
+      <c r="L18" s="47" t="s">
         <v>87</v>
       </c>
-      <c r="M18" s="47" t="s">
+      <c r="M18" s="45" t="s">
         <v>25</v>
       </c>
-      <c r="N18" s="45"/>
+      <c r="N18" s="43"/>
       <c r="O18" s="2"/>
       <c r="P18" s="2"/>
       <c r="Q18" s="2"/>
@@ -2140,40 +2154,40 @@
       <c r="V18" s="2"/>
     </row>
     <row r="19" spans="1:22" ht="13">
-      <c r="A19" s="40"/>
-      <c r="B19" s="42" t="s">
+      <c r="A19" s="38"/>
+      <c r="B19" s="40" t="s">
         <v>88</v>
       </c>
-      <c r="C19" s="41" t="s">
+      <c r="C19" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="D19" s="40" t="s">
+      <c r="D19" s="38" t="s">
         <v>89</v>
       </c>
-      <c r="E19" s="40"/>
-      <c r="F19" s="42" t="s">
+      <c r="E19" s="38"/>
+      <c r="F19" s="40" t="s">
         <v>83</v>
       </c>
-      <c r="G19" s="42" t="s">
+      <c r="G19" s="40" t="s">
         <v>90</v>
       </c>
-      <c r="H19" s="40" t="s">
+      <c r="H19" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="I19" s="42" t="s">
+      <c r="I19" s="40" t="s">
         <v>91</v>
       </c>
-      <c r="J19" s="43" t="s">
+      <c r="J19" s="41" t="s">
         <v>92</v>
       </c>
-      <c r="K19" s="40"/>
-      <c r="L19" s="44" t="s">
+      <c r="K19" s="38"/>
+      <c r="L19" s="42" t="s">
         <v>93</v>
       </c>
-      <c r="M19" s="41" t="s">
+      <c r="M19" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="N19" s="40"/>
+      <c r="N19" s="38"/>
       <c r="O19" s="2"/>
       <c r="P19" s="2"/>
       <c r="Q19" s="2"/>
@@ -2184,40 +2198,40 @@
       <c r="V19" s="2"/>
     </row>
     <row r="20" spans="1:22" ht="13">
-      <c r="A20" s="45"/>
-      <c r="B20" s="46" t="s">
+      <c r="A20" s="43"/>
+      <c r="B20" s="44" t="s">
         <v>94</v>
       </c>
-      <c r="C20" s="47" t="s">
+      <c r="C20" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="D20" s="45" t="s">
+      <c r="D20" s="43" t="s">
         <v>95</v>
       </c>
-      <c r="E20" s="45"/>
-      <c r="F20" s="46" t="s">
+      <c r="E20" s="43"/>
+      <c r="F20" s="44" t="s">
         <v>83</v>
       </c>
-      <c r="G20" s="46" t="s">
+      <c r="G20" s="44" t="s">
         <v>96</v>
       </c>
-      <c r="H20" s="45" t="s">
+      <c r="H20" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="I20" s="46" t="s">
+      <c r="I20" s="44" t="s">
         <v>97</v>
       </c>
-      <c r="J20" s="48" t="s">
+      <c r="J20" s="46" t="s">
         <v>98</v>
       </c>
-      <c r="K20" s="45"/>
-      <c r="L20" s="49" t="s">
+      <c r="K20" s="43"/>
+      <c r="L20" s="47" t="s">
         <v>99</v>
       </c>
-      <c r="M20" s="47" t="s">
+      <c r="M20" s="45" t="s">
         <v>25</v>
       </c>
-      <c r="N20" s="45"/>
+      <c r="N20" s="43"/>
       <c r="O20" s="2"/>
       <c r="P20" s="2"/>
       <c r="Q20" s="2"/>
@@ -2228,40 +2242,40 @@
       <c r="V20" s="2"/>
     </row>
     <row r="21" spans="1:22" ht="13">
-      <c r="A21" s="40"/>
-      <c r="B21" s="42" t="s">
+      <c r="A21" s="38"/>
+      <c r="B21" s="40" t="s">
         <v>100</v>
       </c>
-      <c r="C21" s="41" t="s">
+      <c r="C21" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="D21" s="40" t="s">
+      <c r="D21" s="38" t="s">
         <v>101</v>
       </c>
-      <c r="E21" s="40"/>
-      <c r="F21" s="42" t="s">
+      <c r="E21" s="38"/>
+      <c r="F21" s="40" t="s">
         <v>83</v>
       </c>
-      <c r="G21" s="42" t="s">
+      <c r="G21" s="40" t="s">
         <v>102</v>
       </c>
-      <c r="H21" s="40" t="s">
+      <c r="H21" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="I21" s="42" t="s">
+      <c r="I21" s="40" t="s">
         <v>103</v>
       </c>
-      <c r="J21" s="43" t="s">
+      <c r="J21" s="41" t="s">
         <v>104</v>
       </c>
-      <c r="K21" s="40"/>
-      <c r="L21" s="44" t="s">
+      <c r="K21" s="38"/>
+      <c r="L21" s="42" t="s">
         <v>105</v>
       </c>
-      <c r="M21" s="41" t="s">
+      <c r="M21" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="N21" s="40"/>
+      <c r="N21" s="38"/>
       <c r="O21" s="2"/>
       <c r="P21" s="2"/>
       <c r="Q21" s="2"/>
@@ -2272,40 +2286,40 @@
       <c r="V21" s="2"/>
     </row>
     <row r="22" spans="1:22" ht="13">
-      <c r="A22" s="45"/>
-      <c r="B22" s="46" t="s">
+      <c r="A22" s="43"/>
+      <c r="B22" s="44" t="s">
         <v>106</v>
       </c>
-      <c r="C22" s="47" t="s">
+      <c r="C22" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="D22" s="45" t="s">
+      <c r="D22" s="43" t="s">
         <v>107</v>
       </c>
-      <c r="E22" s="45"/>
-      <c r="F22" s="46" t="s">
+      <c r="E22" s="43"/>
+      <c r="F22" s="44" t="s">
         <v>83</v>
       </c>
-      <c r="G22" s="46" t="s">
+      <c r="G22" s="44" t="s">
         <v>108</v>
       </c>
-      <c r="H22" s="45" t="s">
+      <c r="H22" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="I22" s="46" t="s">
+      <c r="I22" s="44" t="s">
         <v>109</v>
       </c>
-      <c r="J22" s="48" t="s">
+      <c r="J22" s="46" t="s">
         <v>110</v>
       </c>
-      <c r="K22" s="45"/>
-      <c r="L22" s="49" t="s">
+      <c r="K22" s="43"/>
+      <c r="L22" s="47" t="s">
         <v>111</v>
       </c>
-      <c r="M22" s="47" t="s">
+      <c r="M22" s="45" t="s">
         <v>25</v>
       </c>
-      <c r="N22" s="45"/>
+      <c r="N22" s="43"/>
       <c r="O22" s="2"/>
       <c r="P22" s="2"/>
       <c r="Q22" s="2"/>
@@ -2316,40 +2330,40 @@
       <c r="V22" s="2"/>
     </row>
     <row r="23" spans="1:22" ht="13">
-      <c r="A23" s="40"/>
-      <c r="B23" s="42" t="s">
+      <c r="A23" s="38"/>
+      <c r="B23" s="40" t="s">
         <v>112</v>
       </c>
-      <c r="C23" s="41" t="s">
+      <c r="C23" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="D23" s="40" t="s">
+      <c r="D23" s="38" t="s">
         <v>113</v>
       </c>
-      <c r="E23" s="40"/>
-      <c r="F23" s="42" t="s">
+      <c r="E23" s="38"/>
+      <c r="F23" s="40" t="s">
         <v>83</v>
       </c>
-      <c r="G23" s="42" t="s">
+      <c r="G23" s="40" t="s">
         <v>114</v>
       </c>
-      <c r="H23" s="40" t="s">
+      <c r="H23" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="I23" s="42" t="s">
+      <c r="I23" s="40" t="s">
         <v>115</v>
       </c>
-      <c r="J23" s="43" t="s">
+      <c r="J23" s="41" t="s">
         <v>116</v>
       </c>
-      <c r="K23" s="40"/>
-      <c r="L23" s="44" t="s">
+      <c r="K23" s="38"/>
+      <c r="L23" s="42" t="s">
         <v>117</v>
       </c>
-      <c r="M23" s="41" t="s">
+      <c r="M23" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="N23" s="40"/>
+      <c r="N23" s="38"/>
       <c r="O23" s="2"/>
       <c r="P23" s="2"/>
       <c r="Q23" s="2"/>
@@ -2360,40 +2374,40 @@
       <c r="V23" s="2"/>
     </row>
     <row r="24" spans="1:22" ht="13">
-      <c r="A24" s="45"/>
-      <c r="B24" s="46" t="s">
+      <c r="A24" s="43"/>
+      <c r="B24" s="44" t="s">
         <v>118</v>
       </c>
-      <c r="C24" s="47" t="s">
+      <c r="C24" s="45" t="s">
         <v>26</v>
       </c>
-      <c r="D24" s="45" t="s">
+      <c r="D24" s="43" t="s">
         <v>119</v>
       </c>
-      <c r="E24" s="45"/>
-      <c r="F24" s="46" t="s">
+      <c r="E24" s="43"/>
+      <c r="F24" s="44" t="s">
         <v>83</v>
       </c>
-      <c r="G24" s="46" t="s">
+      <c r="G24" s="44" t="s">
         <v>120</v>
       </c>
-      <c r="H24" s="45" t="s">
+      <c r="H24" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="I24" s="46" t="s">
+      <c r="I24" s="44" t="s">
         <v>121</v>
       </c>
-      <c r="J24" s="48" t="s">
+      <c r="J24" s="46" t="s">
         <v>122</v>
       </c>
-      <c r="K24" s="45"/>
-      <c r="L24" s="49" t="s">
+      <c r="K24" s="43"/>
+      <c r="L24" s="47" t="s">
         <v>123</v>
       </c>
-      <c r="M24" s="47" t="s">
+      <c r="M24" s="45" t="s">
         <v>25</v>
       </c>
-      <c r="N24" s="45"/>
+      <c r="N24" s="43"/>
       <c r="O24" s="2"/>
       <c r="P24" s="2"/>
       <c r="Q24" s="2"/>
@@ -2404,22 +2418,22 @@
       <c r="V24" s="2"/>
     </row>
     <row r="25" spans="1:22" ht="13">
-      <c r="A25" s="92" t="s">
+      <c r="A25" s="93" t="s">
         <v>124</v>
       </c>
-      <c r="B25" s="92"/>
-      <c r="C25" s="92"/>
-      <c r="D25" s="92"/>
-      <c r="E25" s="92"/>
-      <c r="F25" s="92"/>
-      <c r="G25" s="92"/>
-      <c r="H25" s="92"/>
-      <c r="I25" s="92"/>
-      <c r="J25" s="92"/>
-      <c r="K25" s="92"/>
-      <c r="L25" s="92"/>
-      <c r="M25" s="92"/>
-      <c r="N25" s="92"/>
+      <c r="B25" s="93"/>
+      <c r="C25" s="93"/>
+      <c r="D25" s="93"/>
+      <c r="E25" s="93"/>
+      <c r="F25" s="93"/>
+      <c r="G25" s="93"/>
+      <c r="H25" s="93"/>
+      <c r="I25" s="93"/>
+      <c r="J25" s="93"/>
+      <c r="K25" s="93"/>
+      <c r="L25" s="93"/>
+      <c r="M25" s="93"/>
+      <c r="N25" s="93"/>
       <c r="O25" s="2"/>
       <c r="P25" s="2"/>
       <c r="Q25" s="2"/>
@@ -2430,40 +2444,40 @@
       <c r="V25" s="2"/>
     </row>
     <row r="26" spans="1:22" s="6" customFormat="1" ht="13">
-      <c r="A26" s="50"/>
-      <c r="B26" s="51" t="s">
+      <c r="A26" s="48"/>
+      <c r="B26" s="71" t="s">
         <v>243</v>
       </c>
-      <c r="C26" s="52" t="s">
+      <c r="C26" s="49" t="s">
         <v>17</v>
       </c>
-      <c r="D26" s="50" t="s">
+      <c r="D26" s="48" t="s">
         <v>242</v>
       </c>
-      <c r="E26" s="50"/>
-      <c r="F26" s="50" t="s">
+      <c r="E26" s="48"/>
+      <c r="F26" s="48" t="s">
         <v>241</v>
       </c>
-      <c r="G26" s="50" t="s">
+      <c r="G26" s="48" t="s">
         <v>238</v>
       </c>
-      <c r="H26" s="40" t="s">
+      <c r="H26" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="I26" s="51" t="s">
+      <c r="I26" s="71" t="s">
         <v>240</v>
       </c>
-      <c r="J26" s="53" t="s">
+      <c r="J26" s="72" t="s">
         <v>239</v>
       </c>
-      <c r="K26" s="50"/>
-      <c r="L26" s="54">
+      <c r="K26" s="48"/>
+      <c r="L26" s="50">
         <v>20488</v>
       </c>
-      <c r="M26" s="41" t="s">
+      <c r="M26" s="39" t="s">
         <v>60</v>
       </c>
-      <c r="N26" s="50"/>
+      <c r="N26" s="48"/>
       <c r="O26" s="5"/>
       <c r="P26" s="5"/>
       <c r="Q26" s="5"/>
@@ -2478,7 +2492,7 @@
       <c r="B27" s="22" t="s">
         <v>125</v>
       </c>
-      <c r="C27" s="24" t="s">
+      <c r="C27" s="23" t="s">
         <v>126</v>
       </c>
       <c r="D27" s="22" t="s">
@@ -2501,10 +2515,10 @@
         <v>131</v>
       </c>
       <c r="K27" s="22"/>
-      <c r="L27" s="24" t="s">
+      <c r="L27" s="23" t="s">
         <v>132</v>
       </c>
-      <c r="M27" s="24" t="s">
+      <c r="M27" s="23" t="s">
         <v>60</v>
       </c>
       <c r="N27" s="22"/>
@@ -2518,40 +2532,40 @@
       <c r="V27" s="7"/>
     </row>
     <row r="28" spans="1:22" s="6" customFormat="1" ht="13">
-      <c r="A28" s="55"/>
-      <c r="B28" s="56" t="s">
+      <c r="A28" s="51"/>
+      <c r="B28" s="52" t="s">
         <v>133</v>
       </c>
-      <c r="C28" s="57" t="s">
+      <c r="C28" s="53" t="s">
         <v>134</v>
       </c>
-      <c r="D28" s="55" t="s">
+      <c r="D28" s="51" t="s">
         <v>135</v>
       </c>
-      <c r="E28" s="55"/>
-      <c r="F28" s="55" t="s">
+      <c r="E28" s="51"/>
+      <c r="F28" s="51" t="s">
         <v>128</v>
       </c>
-      <c r="G28" s="56" t="s">
+      <c r="G28" s="52" t="s">
         <v>136</v>
       </c>
-      <c r="H28" s="55" t="s">
+      <c r="H28" s="51" t="s">
         <v>21</v>
       </c>
-      <c r="I28" s="56" t="s">
+      <c r="I28" s="52" t="s">
         <v>137</v>
       </c>
-      <c r="J28" s="58" t="s">
+      <c r="J28" s="54" t="s">
         <v>138</v>
       </c>
-      <c r="K28" s="55"/>
-      <c r="L28" s="57" t="s">
+      <c r="K28" s="51"/>
+      <c r="L28" s="53" t="s">
         <v>139</v>
       </c>
-      <c r="M28" s="52" t="s">
+      <c r="M28" s="49" t="s">
         <v>60</v>
       </c>
-      <c r="N28" s="55"/>
+      <c r="N28" s="51"/>
       <c r="O28" s="5"/>
       <c r="P28" s="5"/>
       <c r="Q28" s="5"/>
@@ -2561,67 +2575,67 @@
       <c r="U28" s="5"/>
       <c r="V28" s="5"/>
     </row>
-    <row r="29" spans="1:22" s="100" customFormat="1" ht="13">
-      <c r="A29" s="94"/>
-      <c r="B29" s="95" t="s">
+    <row r="29" spans="1:22" s="91" customFormat="1" ht="13">
+      <c r="A29" s="87"/>
+      <c r="B29" s="33" t="s">
         <v>255</v>
       </c>
-      <c r="C29" s="96" t="s">
+      <c r="C29" s="88" t="s">
         <v>256</v>
       </c>
-      <c r="D29" s="94" t="s">
+      <c r="D29" s="87" t="s">
         <v>257</v>
       </c>
-      <c r="E29" s="94"/>
-      <c r="F29" s="94" t="s">
+      <c r="E29" s="87"/>
+      <c r="F29" s="87" t="s">
         <v>258</v>
       </c>
-      <c r="G29" s="95" t="s">
+      <c r="G29" s="33" t="s">
         <v>259</v>
       </c>
-      <c r="H29" s="94" t="s">
+      <c r="H29" s="87" t="s">
         <v>21</v>
       </c>
-      <c r="I29" s="95" t="s">
+      <c r="I29" s="33" t="s">
         <v>260</v>
       </c>
-      <c r="J29" s="97" t="s">
+      <c r="J29" s="99" t="s">
         <v>261</v>
       </c>
-      <c r="K29" s="94"/>
-      <c r="L29" s="95">
+      <c r="K29" s="87"/>
+      <c r="L29" s="33">
         <v>965</v>
       </c>
-      <c r="M29" s="98" t="s">
+      <c r="M29" s="89" t="s">
         <v>60</v>
       </c>
-      <c r="N29" s="94"/>
-      <c r="O29" s="99"/>
-      <c r="P29" s="99"/>
-      <c r="Q29" s="99"/>
-      <c r="R29" s="99"/>
-      <c r="S29" s="99"/>
-      <c r="T29" s="99"/>
-      <c r="U29" s="99"/>
-      <c r="V29" s="99"/>
+      <c r="N29" s="87"/>
+      <c r="O29" s="90"/>
+      <c r="P29" s="90"/>
+      <c r="Q29" s="90"/>
+      <c r="R29" s="90"/>
+      <c r="S29" s="90"/>
+      <c r="T29" s="90"/>
+      <c r="U29" s="90"/>
+      <c r="V29" s="90"/>
     </row>
     <row r="30" spans="1:22" ht="13">
-      <c r="A30" s="92" t="s">
+      <c r="A30" s="93" t="s">
         <v>140</v>
       </c>
-      <c r="B30" s="92"/>
-      <c r="C30" s="92"/>
-      <c r="D30" s="92"/>
-      <c r="E30" s="92"/>
-      <c r="F30" s="92"/>
-      <c r="G30" s="92"/>
-      <c r="H30" s="92"/>
-      <c r="I30" s="92"/>
-      <c r="J30" s="92"/>
-      <c r="K30" s="92"/>
-      <c r="L30" s="92"/>
-      <c r="M30" s="92"/>
-      <c r="N30" s="92"/>
+      <c r="B30" s="93"/>
+      <c r="C30" s="93"/>
+      <c r="D30" s="93"/>
+      <c r="E30" s="93"/>
+      <c r="F30" s="93"/>
+      <c r="G30" s="93"/>
+      <c r="H30" s="93"/>
+      <c r="I30" s="93"/>
+      <c r="J30" s="93"/>
+      <c r="K30" s="93"/>
+      <c r="L30" s="93"/>
+      <c r="M30" s="93"/>
+      <c r="N30" s="93"/>
       <c r="O30" s="2"/>
       <c r="P30" s="2"/>
       <c r="Q30" s="2"/>
@@ -2632,40 +2646,40 @@
       <c r="V30" s="2"/>
     </row>
     <row r="31" spans="1:22" ht="13">
-      <c r="A31" s="40"/>
-      <c r="B31" s="40" t="s">
+      <c r="A31" s="38"/>
+      <c r="B31" s="38" t="s">
         <v>141</v>
       </c>
-      <c r="C31" s="41" t="s">
+      <c r="C31" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="D31" s="40" t="s">
+      <c r="D31" s="38" t="s">
         <v>142</v>
       </c>
-      <c r="E31" s="40"/>
-      <c r="F31" s="40" t="s">
+      <c r="E31" s="38"/>
+      <c r="F31" s="38" t="s">
         <v>143</v>
       </c>
-      <c r="G31" s="40" t="s">
+      <c r="G31" s="38" t="s">
         <v>144</v>
       </c>
-      <c r="H31" s="40" t="s">
+      <c r="H31" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="I31" s="40" t="s">
+      <c r="I31" s="38" t="s">
         <v>145</v>
       </c>
-      <c r="J31" s="40" t="s">
+      <c r="J31" s="38" t="s">
         <v>146</v>
       </c>
-      <c r="K31" s="40"/>
-      <c r="L31" s="44" t="s">
+      <c r="K31" s="38"/>
+      <c r="L31" s="42" t="s">
         <v>147</v>
       </c>
-      <c r="M31" s="41" t="s">
+      <c r="M31" s="39" t="s">
         <v>60</v>
       </c>
-      <c r="N31" s="40"/>
+      <c r="N31" s="38"/>
       <c r="O31" s="2"/>
       <c r="P31" s="2"/>
       <c r="Q31" s="2"/>
@@ -2676,22 +2690,22 @@
       <c r="V31" s="2"/>
     </row>
     <row r="32" spans="1:22" ht="13">
-      <c r="A32" s="91" t="s">
+      <c r="A32" s="92" t="s">
         <v>148</v>
       </c>
-      <c r="B32" s="91"/>
-      <c r="C32" s="91"/>
-      <c r="D32" s="91"/>
-      <c r="E32" s="91"/>
-      <c r="F32" s="91"/>
-      <c r="G32" s="91"/>
-      <c r="H32" s="91"/>
-      <c r="I32" s="91"/>
-      <c r="J32" s="91"/>
-      <c r="K32" s="91"/>
-      <c r="L32" s="91"/>
-      <c r="M32" s="91"/>
-      <c r="N32" s="91"/>
+      <c r="B32" s="92"/>
+      <c r="C32" s="92"/>
+      <c r="D32" s="92"/>
+      <c r="E32" s="92"/>
+      <c r="F32" s="92"/>
+      <c r="G32" s="92"/>
+      <c r="H32" s="92"/>
+      <c r="I32" s="92"/>
+      <c r="J32" s="92"/>
+      <c r="K32" s="92"/>
+      <c r="L32" s="92"/>
+      <c r="M32" s="92"/>
+      <c r="N32" s="92"/>
       <c r="O32" s="2"/>
       <c r="P32" s="2"/>
       <c r="Q32" s="2"/>
@@ -2702,38 +2716,38 @@
       <c r="V32" s="2"/>
     </row>
     <row r="33" spans="1:22" ht="13">
-      <c r="A33" s="59"/>
-      <c r="B33" s="60" t="s">
+      <c r="A33" s="55"/>
+      <c r="B33" s="56" t="s">
         <v>149</v>
       </c>
-      <c r="C33" s="42" t="s">
+      <c r="C33" s="40" t="s">
         <v>150</v>
       </c>
-      <c r="D33" s="61"/>
-      <c r="E33" s="62"/>
-      <c r="F33" s="42" t="s">
+      <c r="D33" s="57"/>
+      <c r="E33" s="58"/>
+      <c r="F33" s="40" t="s">
         <v>151</v>
       </c>
-      <c r="G33" s="62" t="s">
+      <c r="G33" s="58" t="s">
         <v>152</v>
       </c>
-      <c r="H33" s="62" t="s">
+      <c r="H33" s="58" t="s">
         <v>21</v>
       </c>
-      <c r="I33" s="42" t="s">
+      <c r="I33" s="40" t="s">
         <v>153</v>
       </c>
-      <c r="J33" s="43" t="s">
+      <c r="J33" s="41" t="s">
         <v>154</v>
       </c>
-      <c r="K33" s="63"/>
-      <c r="L33" s="64" t="s">
+      <c r="K33" s="59"/>
+      <c r="L33" s="60" t="s">
         <v>155</v>
       </c>
-      <c r="M33" s="64" t="s">
+      <c r="M33" s="60" t="s">
         <v>60</v>
       </c>
-      <c r="N33" s="62" t="s">
+      <c r="N33" s="58" t="s">
         <v>156</v>
       </c>
       <c r="O33" s="2"/>
@@ -2746,38 +2760,38 @@
       <c r="V33" s="2"/>
     </row>
     <row r="34" spans="1:22" s="10" customFormat="1" ht="13">
-      <c r="A34" s="65"/>
-      <c r="B34" s="33" t="s">
+      <c r="A34" s="61"/>
+      <c r="B34" s="31" t="s">
         <v>237</v>
       </c>
-      <c r="C34" s="33" t="s">
+      <c r="C34" s="31" t="s">
         <v>235</v>
       </c>
-      <c r="D34" s="66"/>
-      <c r="E34" s="67"/>
-      <c r="F34" s="33" t="s">
+      <c r="D34" s="62"/>
+      <c r="E34" s="63"/>
+      <c r="F34" s="31" t="s">
         <v>234</v>
       </c>
-      <c r="G34" s="33" t="s">
+      <c r="G34" s="31" t="s">
         <v>232</v>
       </c>
-      <c r="H34" s="67" t="s">
+      <c r="H34" s="63" t="s">
         <v>21</v>
       </c>
-      <c r="I34" s="33" t="s">
+      <c r="I34" s="31" t="s">
         <v>233</v>
       </c>
-      <c r="J34" s="68" t="s">
+      <c r="J34" s="64" t="s">
         <v>236</v>
       </c>
-      <c r="K34" s="69"/>
-      <c r="L34" s="35">
+      <c r="K34" s="65"/>
+      <c r="L34" s="33">
         <v>1266</v>
       </c>
-      <c r="M34" s="70" t="s">
+      <c r="M34" s="66" t="s">
         <v>60</v>
       </c>
-      <c r="N34" s="67"/>
+      <c r="N34" s="63"/>
       <c r="O34" s="7"/>
       <c r="P34" s="7"/>
       <c r="Q34" s="7"/>
@@ -2788,40 +2802,40 @@
       <c r="V34" s="7"/>
     </row>
     <row r="35" spans="1:22" s="6" customFormat="1" ht="13">
-      <c r="A35" s="55"/>
-      <c r="B35" s="71" t="s">
+      <c r="A35" s="51"/>
+      <c r="B35" s="67" t="s">
         <v>157</v>
       </c>
-      <c r="C35" s="56" t="s">
+      <c r="C35" s="52" t="s">
         <v>158</v>
       </c>
-      <c r="D35" s="55" t="s">
+      <c r="D35" s="51" t="s">
         <v>159</v>
       </c>
-      <c r="E35" s="55"/>
-      <c r="F35" s="55" t="s">
+      <c r="E35" s="51"/>
+      <c r="F35" s="51" t="s">
         <v>160</v>
       </c>
-      <c r="G35" s="72" t="s">
+      <c r="G35" s="68" t="s">
         <v>161</v>
       </c>
-      <c r="H35" s="55" t="s">
+      <c r="H35" s="51" t="s">
         <v>21</v>
       </c>
-      <c r="I35" s="56" t="s">
+      <c r="I35" s="52" t="s">
         <v>162</v>
       </c>
-      <c r="J35" s="71" t="s">
+      <c r="J35" s="67" t="s">
         <v>163</v>
       </c>
-      <c r="K35" s="73"/>
-      <c r="L35" s="57">
+      <c r="K35" s="69"/>
+      <c r="L35" s="53">
         <v>280</v>
       </c>
-      <c r="M35" s="52" t="s">
+      <c r="M35" s="49" t="s">
         <v>60</v>
       </c>
-      <c r="N35" s="55"/>
+      <c r="N35" s="51"/>
       <c r="O35" s="9"/>
       <c r="P35" s="9"/>
       <c r="Q35" s="9"/>
@@ -2858,11 +2872,11 @@
       <c r="J36" s="22" t="s">
         <v>169</v>
       </c>
-      <c r="K36" s="74"/>
-      <c r="L36" s="24">
+      <c r="K36" s="70"/>
+      <c r="L36" s="23">
         <v>2304</v>
       </c>
-      <c r="M36" s="24" t="s">
+      <c r="M36" s="23" t="s">
         <v>60</v>
       </c>
       <c r="N36" s="22"/>
@@ -2876,38 +2890,38 @@
       <c r="V36" s="11"/>
     </row>
     <row r="37" spans="1:22" ht="13">
-      <c r="A37" s="40"/>
-      <c r="B37" s="75" t="s">
+      <c r="A37" s="38"/>
+      <c r="B37" s="71" t="s">
         <v>208</v>
       </c>
-      <c r="C37" s="75" t="s">
+      <c r="C37" s="71" t="s">
         <v>207</v>
       </c>
-      <c r="D37" s="40"/>
-      <c r="E37" s="40"/>
-      <c r="F37" s="75" t="s">
+      <c r="D37" s="38"/>
+      <c r="E37" s="38"/>
+      <c r="F37" s="71" t="s">
         <v>206</v>
       </c>
-      <c r="G37" s="40" t="s">
+      <c r="G37" s="38" t="s">
         <v>203</v>
       </c>
-      <c r="H37" s="40" t="s">
+      <c r="H37" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="I37" s="75" t="s">
+      <c r="I37" s="71" t="s">
         <v>204</v>
       </c>
-      <c r="J37" s="76" t="s">
+      <c r="J37" s="72" t="s">
         <v>205</v>
       </c>
-      <c r="K37" s="77"/>
-      <c r="L37" s="78">
+      <c r="K37" s="73"/>
+      <c r="L37" s="74">
         <v>5850</v>
       </c>
-      <c r="M37" s="41" t="s">
+      <c r="M37" s="39" t="s">
         <v>60</v>
       </c>
-      <c r="N37" s="40"/>
+      <c r="N37" s="38"/>
       <c r="O37" s="3"/>
       <c r="P37" s="3"/>
       <c r="Q37" s="3"/>
@@ -2919,15 +2933,15 @@
     </row>
     <row r="38" spans="1:22" s="10" customFormat="1" ht="13">
       <c r="A38" s="22"/>
-      <c r="B38" s="33" t="s">
+      <c r="B38" s="31" t="s">
         <v>213</v>
       </c>
-      <c r="C38" s="33" t="s">
+      <c r="C38" s="31" t="s">
         <v>212</v>
       </c>
       <c r="D38" s="22"/>
       <c r="E38" s="22"/>
-      <c r="F38" s="33" t="s">
+      <c r="F38" s="31" t="s">
         <v>206</v>
       </c>
       <c r="G38" s="22" t="s">
@@ -2936,17 +2950,17 @@
       <c r="H38" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="I38" s="33" t="s">
+      <c r="I38" s="31" t="s">
         <v>210</v>
       </c>
-      <c r="J38" s="68" t="s">
+      <c r="J38" s="64" t="s">
         <v>211</v>
       </c>
-      <c r="K38" s="74"/>
-      <c r="L38" s="35">
+      <c r="K38" s="70"/>
+      <c r="L38" s="33">
         <v>4376</v>
       </c>
-      <c r="M38" s="24" t="s">
+      <c r="M38" s="23" t="s">
         <v>60</v>
       </c>
       <c r="N38" s="22"/>
@@ -2960,22 +2974,22 @@
       <c r="V38" s="12"/>
     </row>
     <row r="39" spans="1:22" ht="13">
-      <c r="A39" s="92" t="s">
+      <c r="A39" s="93" t="s">
         <v>170</v>
       </c>
-      <c r="B39" s="92"/>
-      <c r="C39" s="92"/>
-      <c r="D39" s="92"/>
-      <c r="E39" s="92"/>
-      <c r="F39" s="92"/>
-      <c r="G39" s="92"/>
-      <c r="H39" s="92"/>
-      <c r="I39" s="92"/>
-      <c r="J39" s="92"/>
-      <c r="K39" s="92"/>
-      <c r="L39" s="92"/>
-      <c r="M39" s="92"/>
-      <c r="N39" s="92"/>
+      <c r="B39" s="93"/>
+      <c r="C39" s="93"/>
+      <c r="D39" s="93"/>
+      <c r="E39" s="93"/>
+      <c r="F39" s="93"/>
+      <c r="G39" s="93"/>
+      <c r="H39" s="93"/>
+      <c r="I39" s="93"/>
+      <c r="J39" s="93"/>
+      <c r="K39" s="93"/>
+      <c r="L39" s="93"/>
+      <c r="M39" s="93"/>
+      <c r="N39" s="93"/>
       <c r="O39" s="2"/>
       <c r="P39" s="2"/>
       <c r="Q39" s="2"/>
@@ -2986,38 +3000,38 @@
       <c r="V39" s="2"/>
     </row>
     <row r="40" spans="1:22" ht="13">
-      <c r="A40" s="40"/>
-      <c r="B40" s="79" t="s">
+      <c r="A40" s="38"/>
+      <c r="B40" s="75" t="s">
         <v>171</v>
       </c>
-      <c r="C40" s="80" t="s">
+      <c r="C40" s="76" t="s">
         <v>172</v>
       </c>
-      <c r="D40" s="40"/>
-      <c r="E40" s="40"/>
-      <c r="F40" s="79" t="s">
+      <c r="D40" s="38"/>
+      <c r="E40" s="38"/>
+      <c r="F40" s="75" t="s">
         <v>173</v>
       </c>
-      <c r="G40" s="79" t="s">
+      <c r="G40" s="75" t="s">
         <v>174</v>
       </c>
-      <c r="H40" s="79" t="s">
+      <c r="H40" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="I40" s="79" t="s">
+      <c r="I40" s="75" t="s">
         <v>175</v>
       </c>
-      <c r="J40" s="81" t="s">
+      <c r="J40" s="77" t="s">
         <v>176</v>
       </c>
-      <c r="K40" s="77"/>
-      <c r="L40" s="41" t="s">
+      <c r="K40" s="73"/>
+      <c r="L40" s="39" t="s">
         <v>177</v>
       </c>
-      <c r="M40" s="41" t="s">
+      <c r="M40" s="39" t="s">
         <v>60</v>
       </c>
-      <c r="N40" s="40" t="s">
+      <c r="N40" s="38" t="s">
         <v>178</v>
       </c>
       <c r="O40" s="2"/>
@@ -3029,76 +3043,76 @@
       <c r="U40" s="2"/>
       <c r="V40" s="2"/>
     </row>
-    <row r="41" spans="1:22" s="8" customFormat="1" ht="13">
-      <c r="A41" s="22"/>
-      <c r="B41" s="23" t="s">
+    <row r="41" spans="1:22" s="91" customFormat="1" ht="13">
+      <c r="A41" s="96"/>
+      <c r="B41" s="79" t="s">
+        <v>171</v>
+      </c>
+      <c r="C41" s="78" t="s">
+        <v>172</v>
+      </c>
+      <c r="D41" s="96"/>
+      <c r="E41" s="96"/>
+      <c r="F41" s="33" t="s">
+        <v>250</v>
+      </c>
+      <c r="G41" s="33" t="s">
+        <v>262</v>
+      </c>
+      <c r="H41" s="79" t="s">
+        <v>21</v>
+      </c>
+      <c r="I41" s="33" t="s">
+        <v>263</v>
+      </c>
+      <c r="J41" s="99" t="s">
+        <v>264</v>
+      </c>
+      <c r="K41" s="97"/>
+      <c r="L41" s="33">
+        <v>41649</v>
+      </c>
+      <c r="M41" s="98" t="s">
+        <v>60</v>
+      </c>
+      <c r="N41" s="96"/>
+      <c r="O41" s="90"/>
+      <c r="P41" s="90"/>
+      <c r="Q41" s="90"/>
+      <c r="R41" s="90"/>
+      <c r="S41" s="90"/>
+      <c r="T41" s="90"/>
+      <c r="U41" s="90"/>
+      <c r="V41" s="90"/>
+    </row>
+    <row r="42" spans="1:22" s="6" customFormat="1" ht="13">
+      <c r="A42" s="17"/>
+      <c r="B42" s="26" t="s">
         <v>251</v>
       </c>
-      <c r="C41" s="82" t="s">
+      <c r="C42" s="95" t="s">
         <v>172</v>
-      </c>
-      <c r="D41" s="22"/>
-      <c r="E41" s="22"/>
-      <c r="F41" s="23" t="s">
-        <v>250</v>
-      </c>
-      <c r="G41" s="83" t="s">
-        <v>249</v>
-      </c>
-      <c r="H41" s="83" t="s">
-        <v>21</v>
-      </c>
-      <c r="I41" s="23" t="s">
-        <v>252</v>
-      </c>
-      <c r="J41" s="26" t="s">
-        <v>253</v>
-      </c>
-      <c r="K41" s="74"/>
-      <c r="L41" s="24" t="s">
-        <v>254</v>
-      </c>
-      <c r="M41" s="24" t="s">
-        <v>60</v>
-      </c>
-      <c r="N41" s="22"/>
-      <c r="O41" s="7"/>
-      <c r="P41" s="7"/>
-      <c r="Q41" s="7"/>
-      <c r="R41" s="7"/>
-      <c r="S41" s="7"/>
-      <c r="T41" s="7"/>
-      <c r="U41" s="7"/>
-      <c r="V41" s="7"/>
-    </row>
-    <row r="42" spans="1:22" s="14" customFormat="1" ht="13">
-      <c r="A42" s="17"/>
-      <c r="B42" s="28" t="s">
-        <v>215</v>
-      </c>
-      <c r="C42" s="28" t="s">
-        <v>216</v>
       </c>
       <c r="D42" s="17"/>
       <c r="E42" s="17"/>
-      <c r="F42" s="28" t="s">
-        <v>217</v>
-      </c>
-      <c r="G42" s="84" t="s">
-        <v>214</v>
-      </c>
-      <c r="H42" s="84" t="s">
+      <c r="F42" s="26" t="s">
+        <v>250</v>
+      </c>
+      <c r="G42" s="80" t="s">
+        <v>249</v>
+      </c>
+      <c r="H42" s="80" t="s">
         <v>21</v>
       </c>
-      <c r="I42" s="28" t="s">
-        <v>219</v>
-      </c>
-      <c r="J42" s="29" t="s">
-        <v>218</v>
-      </c>
-      <c r="K42" s="85"/>
-      <c r="L42" s="30">
-        <v>392</v>
+      <c r="I42" s="26" t="s">
+        <v>252</v>
+      </c>
+      <c r="J42" s="27" t="s">
+        <v>253</v>
+      </c>
+      <c r="K42" s="81"/>
+      <c r="L42" s="19" t="s">
+        <v>254</v>
       </c>
       <c r="M42" s="19" t="s">
         <v>60</v>
@@ -3115,34 +3129,34 @@
     </row>
     <row r="43" spans="1:22" s="10" customFormat="1" ht="13">
       <c r="A43" s="22"/>
-      <c r="B43" s="33" t="s">
-        <v>230</v>
-      </c>
-      <c r="C43" s="33" t="s">
-        <v>229</v>
+      <c r="B43" s="31" t="s">
+        <v>215</v>
+      </c>
+      <c r="C43" s="31" t="s">
+        <v>216</v>
       </c>
       <c r="D43" s="22"/>
       <c r="E43" s="22"/>
-      <c r="F43" s="33" t="s">
-        <v>228</v>
-      </c>
-      <c r="G43" s="33" t="s">
-        <v>226</v>
-      </c>
-      <c r="H43" s="83" t="s">
+      <c r="F43" s="31" t="s">
+        <v>217</v>
+      </c>
+      <c r="G43" s="79" t="s">
+        <v>214</v>
+      </c>
+      <c r="H43" s="79" t="s">
         <v>21</v>
       </c>
-      <c r="I43" s="33" t="s">
-        <v>227</v>
-      </c>
-      <c r="J43" s="68" t="s">
-        <v>231</v>
-      </c>
-      <c r="K43" s="74"/>
-      <c r="L43" s="35">
-        <v>41306</v>
-      </c>
-      <c r="M43" s="24" t="s">
+      <c r="I43" s="31" t="s">
+        <v>219</v>
+      </c>
+      <c r="J43" s="64" t="s">
+        <v>218</v>
+      </c>
+      <c r="K43" s="70"/>
+      <c r="L43" s="33">
+        <v>392</v>
+      </c>
+      <c r="M43" s="23" t="s">
         <v>60</v>
       </c>
       <c r="N43" s="22"/>
@@ -3155,69 +3169,65 @@
       <c r="U43" s="7"/>
       <c r="V43" s="7"/>
     </row>
-    <row r="44" spans="1:22" ht="13">
-      <c r="A44" s="92" t="s">
+    <row r="44" spans="1:22" s="14" customFormat="1" ht="13">
+      <c r="A44" s="17"/>
+      <c r="B44" s="26" t="s">
+        <v>230</v>
+      </c>
+      <c r="C44" s="26" t="s">
+        <v>229</v>
+      </c>
+      <c r="D44" s="17"/>
+      <c r="E44" s="17"/>
+      <c r="F44" s="26" t="s">
+        <v>228</v>
+      </c>
+      <c r="G44" s="26" t="s">
+        <v>226</v>
+      </c>
+      <c r="H44" s="80" t="s">
+        <v>21</v>
+      </c>
+      <c r="I44" s="26" t="s">
+        <v>227</v>
+      </c>
+      <c r="J44" s="27" t="s">
+        <v>231</v>
+      </c>
+      <c r="K44" s="81"/>
+      <c r="L44" s="28">
+        <v>41306</v>
+      </c>
+      <c r="M44" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="N44" s="17"/>
+      <c r="O44" s="5"/>
+      <c r="P44" s="5"/>
+      <c r="Q44" s="5"/>
+      <c r="R44" s="5"/>
+      <c r="S44" s="5"/>
+      <c r="T44" s="5"/>
+      <c r="U44" s="5"/>
+      <c r="V44" s="5"/>
+    </row>
+    <row r="45" spans="1:22" ht="13">
+      <c r="A45" s="93" t="s">
         <v>179</v>
       </c>
-      <c r="B44" s="92"/>
-      <c r="C44" s="92"/>
-      <c r="D44" s="92"/>
-      <c r="E44" s="92"/>
-      <c r="F44" s="92"/>
-      <c r="G44" s="92"/>
-      <c r="H44" s="92"/>
-      <c r="I44" s="92"/>
-      <c r="J44" s="92"/>
-      <c r="K44" s="92"/>
-      <c r="L44" s="92"/>
-      <c r="M44" s="92"/>
-      <c r="N44" s="92"/>
-      <c r="O44" s="2"/>
-      <c r="P44" s="2"/>
-      <c r="Q44" s="2"/>
-      <c r="R44" s="2"/>
-      <c r="S44" s="2"/>
-      <c r="T44" s="2"/>
-      <c r="U44" s="2"/>
-      <c r="V44" s="2"/>
-    </row>
-    <row r="45" spans="1:22" ht="13">
-      <c r="A45" s="40"/>
-      <c r="B45" s="86" t="s">
-        <v>180</v>
-      </c>
-      <c r="C45" s="44" t="s">
-        <v>181</v>
-      </c>
-      <c r="D45" s="40" t="s">
-        <v>182</v>
-      </c>
-      <c r="E45" s="40"/>
-      <c r="F45" s="42" t="s">
-        <v>183</v>
-      </c>
-      <c r="G45" s="42" t="s">
-        <v>184</v>
-      </c>
-      <c r="H45" s="40" t="s">
-        <v>21</v>
-      </c>
-      <c r="I45" s="42" t="s">
-        <v>185</v>
-      </c>
-      <c r="J45" s="87" t="s">
-        <v>186</v>
-      </c>
-      <c r="K45" s="77"/>
-      <c r="L45" s="88" t="s">
-        <v>187</v>
-      </c>
-      <c r="M45" s="41" t="s">
-        <v>60</v>
-      </c>
-      <c r="N45" s="40" t="s">
-        <v>188</v>
-      </c>
+      <c r="B45" s="93"/>
+      <c r="C45" s="93"/>
+      <c r="D45" s="93"/>
+      <c r="E45" s="93"/>
+      <c r="F45" s="93"/>
+      <c r="G45" s="93"/>
+      <c r="H45" s="93"/>
+      <c r="I45" s="93"/>
+      <c r="J45" s="93"/>
+      <c r="K45" s="93"/>
+      <c r="L45" s="93"/>
+      <c r="M45" s="93"/>
+      <c r="N45" s="93"/>
       <c r="O45" s="2"/>
       <c r="P45" s="2"/>
       <c r="Q45" s="2"/>
@@ -3228,40 +3238,42 @@
       <c r="V45" s="2"/>
     </row>
     <row r="46" spans="1:22" ht="13">
-      <c r="A46" s="45"/>
-      <c r="B46" s="46" t="s">
-        <v>189</v>
-      </c>
-      <c r="C46" s="49" t="s">
-        <v>190</v>
-      </c>
-      <c r="D46" s="45" t="s">
-        <v>191</v>
-      </c>
-      <c r="E46" s="45"/>
-      <c r="F46" s="46" t="s">
+      <c r="A46" s="38"/>
+      <c r="B46" s="82" t="s">
+        <v>180</v>
+      </c>
+      <c r="C46" s="42" t="s">
+        <v>181</v>
+      </c>
+      <c r="D46" s="38" t="s">
+        <v>182</v>
+      </c>
+      <c r="E46" s="38"/>
+      <c r="F46" s="40" t="s">
         <v>183</v>
       </c>
-      <c r="G46" s="45" t="s">
-        <v>192</v>
-      </c>
-      <c r="H46" s="45" t="s">
+      <c r="G46" s="40" t="s">
+        <v>184</v>
+      </c>
+      <c r="H46" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="I46" s="46" t="s">
-        <v>193</v>
-      </c>
-      <c r="J46" s="48" t="s">
-        <v>194</v>
-      </c>
-      <c r="K46" s="45"/>
-      <c r="L46" s="89">
-        <v>2019</v>
-      </c>
-      <c r="M46" s="47" t="s">
+      <c r="I46" s="40" t="s">
+        <v>185</v>
+      </c>
+      <c r="J46" s="83" t="s">
+        <v>186</v>
+      </c>
+      <c r="K46" s="73"/>
+      <c r="L46" s="84" t="s">
+        <v>187</v>
+      </c>
+      <c r="M46" s="39" t="s">
         <v>60</v>
       </c>
-      <c r="N46" s="45"/>
+      <c r="N46" s="38" t="s">
+        <v>188</v>
+      </c>
       <c r="O46" s="2"/>
       <c r="P46" s="2"/>
       <c r="Q46" s="2"/>
@@ -3269,24 +3281,43 @@
       <c r="S46" s="2"/>
       <c r="T46" s="2"/>
       <c r="U46" s="2"/>
+      <c r="V46" s="2"/>
     </row>
     <row r="47" spans="1:22" ht="13">
-      <c r="A47" s="92" t="s">
-        <v>220</v>
-      </c>
-      <c r="B47" s="92"/>
-      <c r="C47" s="92"/>
-      <c r="D47" s="92"/>
-      <c r="E47" s="92"/>
-      <c r="F47" s="92"/>
-      <c r="G47" s="92"/>
-      <c r="H47" s="92"/>
-      <c r="I47" s="92"/>
-      <c r="J47" s="92"/>
-      <c r="K47" s="92"/>
-      <c r="L47" s="92"/>
-      <c r="M47" s="92"/>
-      <c r="N47" s="92"/>
+      <c r="A47" s="43"/>
+      <c r="B47" s="44" t="s">
+        <v>189</v>
+      </c>
+      <c r="C47" s="47" t="s">
+        <v>190</v>
+      </c>
+      <c r="D47" s="43" t="s">
+        <v>191</v>
+      </c>
+      <c r="E47" s="43"/>
+      <c r="F47" s="44" t="s">
+        <v>183</v>
+      </c>
+      <c r="G47" s="43" t="s">
+        <v>192</v>
+      </c>
+      <c r="H47" s="43" t="s">
+        <v>21</v>
+      </c>
+      <c r="I47" s="44" t="s">
+        <v>193</v>
+      </c>
+      <c r="J47" s="46" t="s">
+        <v>194</v>
+      </c>
+      <c r="K47" s="43"/>
+      <c r="L47" s="85">
+        <v>2019</v>
+      </c>
+      <c r="M47" s="45" t="s">
+        <v>60</v>
+      </c>
+      <c r="N47" s="43"/>
       <c r="O47" s="2"/>
       <c r="P47" s="2"/>
       <c r="Q47" s="2"/>
@@ -3294,63 +3325,64 @@
       <c r="S47" s="2"/>
       <c r="T47" s="2"/>
       <c r="U47" s="2"/>
-      <c r="V47" s="2"/>
-    </row>
-    <row r="48" spans="1:22" s="4" customFormat="1" ht="13">
-      <c r="A48" s="90"/>
-      <c r="B48" s="75" t="s">
+    </row>
+    <row r="48" spans="1:22" ht="13">
+      <c r="A48" s="93" t="s">
+        <v>220</v>
+      </c>
+      <c r="B48" s="93"/>
+      <c r="C48" s="93"/>
+      <c r="D48" s="93"/>
+      <c r="E48" s="93"/>
+      <c r="F48" s="93"/>
+      <c r="G48" s="93"/>
+      <c r="H48" s="93"/>
+      <c r="I48" s="93"/>
+      <c r="J48" s="93"/>
+      <c r="K48" s="93"/>
+      <c r="L48" s="93"/>
+      <c r="M48" s="93"/>
+      <c r="N48" s="93"/>
+      <c r="O48" s="2"/>
+      <c r="P48" s="2"/>
+      <c r="Q48" s="2"/>
+      <c r="R48" s="2"/>
+      <c r="S48" s="2"/>
+      <c r="T48" s="2"/>
+      <c r="U48" s="2"/>
+      <c r="V48" s="2"/>
+    </row>
+    <row r="49" spans="1:22" s="4" customFormat="1" ht="13">
+      <c r="A49" s="86"/>
+      <c r="B49" s="71" t="s">
         <v>225</v>
       </c>
-      <c r="C48" s="90"/>
-      <c r="D48" s="90"/>
-      <c r="E48" s="90"/>
-      <c r="F48" s="75" t="s">
+      <c r="C49" s="86"/>
+      <c r="D49" s="86"/>
+      <c r="E49" s="86"/>
+      <c r="F49" s="71" t="s">
         <v>221</v>
       </c>
-      <c r="G48" s="75" t="s">
+      <c r="G49" s="71" t="s">
         <v>222</v>
       </c>
-      <c r="H48" s="40" t="s">
+      <c r="H49" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="I48" s="75" t="s">
+      <c r="I49" s="71" t="s">
         <v>223</v>
       </c>
-      <c r="J48" s="76" t="s">
+      <c r="J49" s="72" t="s">
         <v>224</v>
       </c>
-      <c r="K48" s="90"/>
-      <c r="L48" s="78">
+      <c r="K49" s="86"/>
+      <c r="L49" s="74">
         <v>4957</v>
       </c>
-      <c r="M48" s="41" t="s">
+      <c r="M49" s="39" t="s">
         <v>60</v>
       </c>
-      <c r="N48" s="90"/>
-      <c r="O48" s="1"/>
-      <c r="P48" s="1"/>
-      <c r="Q48" s="1"/>
-      <c r="R48" s="1"/>
-      <c r="S48" s="1"/>
-      <c r="T48" s="1"/>
-      <c r="U48" s="1"/>
-      <c r="V48" s="1"/>
-    </row>
-    <row r="49" spans="1:22" ht="12.5" hidden="1">
-      <c r="A49" s="1"/>
-      <c r="B49" s="1"/>
-      <c r="C49" s="1"/>
-      <c r="D49" s="1"/>
-      <c r="E49" s="1"/>
-      <c r="F49" s="1"/>
-      <c r="G49" s="1"/>
-      <c r="H49" s="1"/>
-      <c r="I49" s="1"/>
-      <c r="J49" s="1"/>
-      <c r="K49" s="1"/>
-      <c r="L49" s="1"/>
-      <c r="M49" s="1"/>
-      <c r="N49" s="1"/>
+      <c r="N49" s="86"/>
       <c r="O49" s="1"/>
       <c r="P49" s="1"/>
       <c r="Q49" s="1"/>
@@ -25056,12 +25088,36 @@
       <c r="U953" s="1"/>
       <c r="V953" s="1"/>
     </row>
+    <row r="954" spans="1:22" ht="12.5" hidden="1">
+      <c r="A954" s="1"/>
+      <c r="B954" s="1"/>
+      <c r="C954" s="1"/>
+      <c r="D954" s="1"/>
+      <c r="E954" s="1"/>
+      <c r="F954" s="1"/>
+      <c r="G954" s="1"/>
+      <c r="H954" s="1"/>
+      <c r="I954" s="1"/>
+      <c r="J954" s="1"/>
+      <c r="K954" s="1"/>
+      <c r="L954" s="1"/>
+      <c r="M954" s="1"/>
+      <c r="N954" s="1"/>
+      <c r="O954" s="1"/>
+      <c r="P954" s="1"/>
+      <c r="Q954" s="1"/>
+      <c r="R954" s="1"/>
+      <c r="S954" s="1"/>
+      <c r="T954" s="1"/>
+      <c r="U954" s="1"/>
+      <c r="V954" s="1"/>
+    </row>
   </sheetData>
   <mergeCells count="9">
     <mergeCell ref="A32:N32"/>
     <mergeCell ref="A39:N39"/>
-    <mergeCell ref="A44:N44"/>
-    <mergeCell ref="A47:N47"/>
+    <mergeCell ref="A45:N45"/>
+    <mergeCell ref="A48:N48"/>
     <mergeCell ref="A1:N1"/>
     <mergeCell ref="A3:N3"/>
     <mergeCell ref="A14:N14"/>

</xml_diff>

<commit_message>
Removing Sylergy DCDC from sheets
</commit_message>
<xml_diff>
--- a/BOM/MIMXRT1064 MCU Module  - BOM.xlsx
+++ b/BOM/MIMXRT1064 MCU Module  - BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\32470\Documents\GitHub\MIMXRT1064-MCU-Module\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53C424A2-76DF-4996-B997-D395DE352795}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04F87890-C499-4A07-9712-73162693FD44}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="259">
   <si>
     <t>MIMXRT1064 MCU Module  - BOM</t>
   </si>
@@ -540,24 +540,6 @@
   </si>
   <si>
     <t>SOT-23-5</t>
-  </si>
-  <si>
-    <t>SILERGY CORP</t>
-  </si>
-  <si>
-    <t>SY8089AAAC</t>
-  </si>
-  <si>
-    <t>C78988</t>
-  </si>
-  <si>
-    <t>$0.2160</t>
-  </si>
-  <si>
-    <t>1230</t>
-  </si>
-  <si>
-    <t>Digital supply</t>
   </si>
   <si>
     <t>CRYSTALS</t>
@@ -997,7 +979,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="100">
+  <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1099,15 +1081,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="49" fontId="7" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1144,11 +1117,6 @@
     <xf numFmtId="0" fontId="7" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="49" fontId="7" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1162,6 +1130,11 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1385,7 +1358,7 @@
   <dimension ref="A1:V954"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45:N45"/>
+      <selection activeCell="A40" sqref="A40:XFD40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15.75" customHeight="1" zeroHeight="1"/>
@@ -1408,22 +1381,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="30" customHeight="1">
-      <c r="A1" s="94" t="s">
+      <c r="A1" s="96" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="94"/>
-      <c r="C1" s="94"/>
-      <c r="D1" s="94"/>
-      <c r="E1" s="94"/>
-      <c r="F1" s="94"/>
-      <c r="G1" s="94"/>
-      <c r="H1" s="94"/>
-      <c r="I1" s="94"/>
-      <c r="J1" s="94"/>
-      <c r="K1" s="94"/>
-      <c r="L1" s="94"/>
-      <c r="M1" s="94"/>
-      <c r="N1" s="94"/>
+      <c r="B1" s="96"/>
+      <c r="C1" s="96"/>
+      <c r="D1" s="96"/>
+      <c r="E1" s="96"/>
+      <c r="F1" s="96"/>
+      <c r="G1" s="96"/>
+      <c r="H1" s="96"/>
+      <c r="I1" s="96"/>
+      <c r="J1" s="96"/>
+      <c r="K1" s="96"/>
+      <c r="L1" s="96"/>
+      <c r="M1" s="96"/>
+      <c r="N1" s="96"/>
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
@@ -1486,22 +1459,22 @@
       <c r="V2" s="1"/>
     </row>
     <row r="3" spans="1:22" ht="13">
-      <c r="A3" s="93" t="s">
+      <c r="A3" s="95" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="93"/>
-      <c r="C3" s="93"/>
-      <c r="D3" s="93"/>
-      <c r="E3" s="93"/>
-      <c r="F3" s="93"/>
-      <c r="G3" s="93"/>
-      <c r="H3" s="93"/>
-      <c r="I3" s="93"/>
-      <c r="J3" s="93"/>
-      <c r="K3" s="93"/>
-      <c r="L3" s="93"/>
-      <c r="M3" s="93"/>
-      <c r="N3" s="93"/>
+      <c r="B3" s="95"/>
+      <c r="C3" s="95"/>
+      <c r="D3" s="95"/>
+      <c r="E3" s="95"/>
+      <c r="F3" s="95"/>
+      <c r="G3" s="95"/>
+      <c r="H3" s="95"/>
+      <c r="I3" s="95"/>
+      <c r="J3" s="95"/>
+      <c r="K3" s="95"/>
+      <c r="L3" s="95"/>
+      <c r="M3" s="95"/>
+      <c r="N3" s="95"/>
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
@@ -1558,33 +1531,33 @@
     <row r="5" spans="1:22" s="8" customFormat="1" ht="13">
       <c r="A5" s="22"/>
       <c r="B5" s="31" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="C5" s="23" t="s">
         <v>26</v>
       </c>
       <c r="D5" s="22" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="E5" s="22"/>
       <c r="F5" s="22" t="s">
         <v>19</v>
       </c>
       <c r="G5" s="24" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="H5" s="22" t="s">
         <v>21</v>
       </c>
       <c r="I5" s="31" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="J5" s="64" t="s">
         <v>28</v>
       </c>
       <c r="K5" s="22"/>
       <c r="L5" s="25" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="M5" s="23" t="s">
         <v>25</v>
@@ -1602,29 +1575,29 @@
     <row r="6" spans="1:22" s="6" customFormat="1" ht="13">
       <c r="A6" s="17"/>
       <c r="B6" s="18" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="C6" s="19" t="s">
         <v>17</v>
       </c>
       <c r="D6" s="17" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="E6" s="17"/>
       <c r="F6" s="17" t="s">
         <v>19</v>
       </c>
       <c r="G6" s="18" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="H6" s="17" t="s">
         <v>21</v>
       </c>
       <c r="I6" s="26" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="J6" s="27" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="K6" s="17"/>
       <c r="L6" s="28">
@@ -1646,7 +1619,7 @@
     <row r="7" spans="1:22" s="8" customFormat="1" ht="13">
       <c r="A7" s="29"/>
       <c r="B7" s="24" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="C7" s="30" t="s">
         <v>17</v>
@@ -1659,13 +1632,13 @@
         <v>19</v>
       </c>
       <c r="G7" s="29" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="H7" s="29" t="s">
         <v>21</v>
       </c>
       <c r="I7" s="31" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="J7" s="32" t="s">
         <v>23</v>
@@ -1952,22 +1925,22 @@
       <c r="V13" s="13"/>
     </row>
     <row r="14" spans="1:22" ht="13">
-      <c r="A14" s="93" t="s">
+      <c r="A14" s="95" t="s">
         <v>61</v>
       </c>
-      <c r="B14" s="93"/>
-      <c r="C14" s="93"/>
-      <c r="D14" s="93"/>
-      <c r="E14" s="93"/>
-      <c r="F14" s="93"/>
-      <c r="G14" s="93"/>
-      <c r="H14" s="93"/>
-      <c r="I14" s="93"/>
-      <c r="J14" s="93"/>
-      <c r="K14" s="93"/>
-      <c r="L14" s="93"/>
-      <c r="M14" s="93"/>
-      <c r="N14" s="93"/>
+      <c r="B14" s="95"/>
+      <c r="C14" s="95"/>
+      <c r="D14" s="95"/>
+      <c r="E14" s="95"/>
+      <c r="F14" s="95"/>
+      <c r="G14" s="95"/>
+      <c r="H14" s="95"/>
+      <c r="I14" s="95"/>
+      <c r="J14" s="95"/>
+      <c r="K14" s="95"/>
+      <c r="L14" s="95"/>
+      <c r="M14" s="95"/>
+      <c r="N14" s="95"/>
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
       <c r="Q14" s="1"/>
@@ -2418,22 +2391,22 @@
       <c r="V24" s="2"/>
     </row>
     <row r="25" spans="1:22" ht="13">
-      <c r="A25" s="93" t="s">
+      <c r="A25" s="95" t="s">
         <v>124</v>
       </c>
-      <c r="B25" s="93"/>
-      <c r="C25" s="93"/>
-      <c r="D25" s="93"/>
-      <c r="E25" s="93"/>
-      <c r="F25" s="93"/>
-      <c r="G25" s="93"/>
-      <c r="H25" s="93"/>
-      <c r="I25" s="93"/>
-      <c r="J25" s="93"/>
-      <c r="K25" s="93"/>
-      <c r="L25" s="93"/>
-      <c r="M25" s="93"/>
-      <c r="N25" s="93"/>
+      <c r="B25" s="95"/>
+      <c r="C25" s="95"/>
+      <c r="D25" s="95"/>
+      <c r="E25" s="95"/>
+      <c r="F25" s="95"/>
+      <c r="G25" s="95"/>
+      <c r="H25" s="95"/>
+      <c r="I25" s="95"/>
+      <c r="J25" s="95"/>
+      <c r="K25" s="95"/>
+      <c r="L25" s="95"/>
+      <c r="M25" s="95"/>
+      <c r="N25" s="95"/>
       <c r="O25" s="2"/>
       <c r="P25" s="2"/>
       <c r="Q25" s="2"/>
@@ -2446,29 +2419,29 @@
     <row r="26" spans="1:22" s="6" customFormat="1" ht="13">
       <c r="A26" s="48"/>
       <c r="B26" s="71" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="C26" s="49" t="s">
         <v>17</v>
       </c>
       <c r="D26" s="48" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="E26" s="48"/>
       <c r="F26" s="48" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="G26" s="48" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="H26" s="38" t="s">
         <v>21</v>
       </c>
       <c r="I26" s="71" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="J26" s="72" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="K26" s="48"/>
       <c r="L26" s="50">
@@ -2575,67 +2548,67 @@
       <c r="U28" s="5"/>
       <c r="V28" s="5"/>
     </row>
-    <row r="29" spans="1:22" s="91" customFormat="1" ht="13">
-      <c r="A29" s="87"/>
+    <row r="29" spans="1:22" s="88" customFormat="1" ht="13">
+      <c r="A29" s="84"/>
       <c r="B29" s="33" t="s">
+        <v>249</v>
+      </c>
+      <c r="C29" s="85" t="s">
+        <v>250</v>
+      </c>
+      <c r="D29" s="84" t="s">
+        <v>251</v>
+      </c>
+      <c r="E29" s="84"/>
+      <c r="F29" s="84" t="s">
+        <v>252</v>
+      </c>
+      <c r="G29" s="33" t="s">
+        <v>253</v>
+      </c>
+      <c r="H29" s="84" t="s">
+        <v>21</v>
+      </c>
+      <c r="I29" s="33" t="s">
+        <v>254</v>
+      </c>
+      <c r="J29" s="93" t="s">
         <v>255</v>
       </c>
-      <c r="C29" s="88" t="s">
-        <v>256</v>
-      </c>
-      <c r="D29" s="87" t="s">
-        <v>257</v>
-      </c>
-      <c r="E29" s="87"/>
-      <c r="F29" s="87" t="s">
-        <v>258</v>
-      </c>
-      <c r="G29" s="33" t="s">
-        <v>259</v>
-      </c>
-      <c r="H29" s="87" t="s">
-        <v>21</v>
-      </c>
-      <c r="I29" s="33" t="s">
-        <v>260</v>
-      </c>
-      <c r="J29" s="99" t="s">
-        <v>261</v>
-      </c>
-      <c r="K29" s="87"/>
+      <c r="K29" s="84"/>
       <c r="L29" s="33">
         <v>965</v>
       </c>
-      <c r="M29" s="89" t="s">
+      <c r="M29" s="86" t="s">
         <v>60</v>
       </c>
-      <c r="N29" s="87"/>
-      <c r="O29" s="90"/>
-      <c r="P29" s="90"/>
-      <c r="Q29" s="90"/>
-      <c r="R29" s="90"/>
-      <c r="S29" s="90"/>
-      <c r="T29" s="90"/>
-      <c r="U29" s="90"/>
-      <c r="V29" s="90"/>
+      <c r="N29" s="84"/>
+      <c r="O29" s="87"/>
+      <c r="P29" s="87"/>
+      <c r="Q29" s="87"/>
+      <c r="R29" s="87"/>
+      <c r="S29" s="87"/>
+      <c r="T29" s="87"/>
+      <c r="U29" s="87"/>
+      <c r="V29" s="87"/>
     </row>
     <row r="30" spans="1:22" ht="13">
-      <c r="A30" s="93" t="s">
+      <c r="A30" s="95" t="s">
         <v>140</v>
       </c>
-      <c r="B30" s="93"/>
-      <c r="C30" s="93"/>
-      <c r="D30" s="93"/>
-      <c r="E30" s="93"/>
-      <c r="F30" s="93"/>
-      <c r="G30" s="93"/>
-      <c r="H30" s="93"/>
-      <c r="I30" s="93"/>
-      <c r="J30" s="93"/>
-      <c r="K30" s="93"/>
-      <c r="L30" s="93"/>
-      <c r="M30" s="93"/>
-      <c r="N30" s="93"/>
+      <c r="B30" s="95"/>
+      <c r="C30" s="95"/>
+      <c r="D30" s="95"/>
+      <c r="E30" s="95"/>
+      <c r="F30" s="95"/>
+      <c r="G30" s="95"/>
+      <c r="H30" s="95"/>
+      <c r="I30" s="95"/>
+      <c r="J30" s="95"/>
+      <c r="K30" s="95"/>
+      <c r="L30" s="95"/>
+      <c r="M30" s="95"/>
+      <c r="N30" s="95"/>
       <c r="O30" s="2"/>
       <c r="P30" s="2"/>
       <c r="Q30" s="2"/>
@@ -2690,22 +2663,22 @@
       <c r="V31" s="2"/>
     </row>
     <row r="32" spans="1:22" ht="13">
-      <c r="A32" s="92" t="s">
+      <c r="A32" s="94" t="s">
         <v>148</v>
       </c>
-      <c r="B32" s="92"/>
-      <c r="C32" s="92"/>
-      <c r="D32" s="92"/>
-      <c r="E32" s="92"/>
-      <c r="F32" s="92"/>
-      <c r="G32" s="92"/>
-      <c r="H32" s="92"/>
-      <c r="I32" s="92"/>
-      <c r="J32" s="92"/>
-      <c r="K32" s="92"/>
-      <c r="L32" s="92"/>
-      <c r="M32" s="92"/>
-      <c r="N32" s="92"/>
+      <c r="B32" s="94"/>
+      <c r="C32" s="94"/>
+      <c r="D32" s="94"/>
+      <c r="E32" s="94"/>
+      <c r="F32" s="94"/>
+      <c r="G32" s="94"/>
+      <c r="H32" s="94"/>
+      <c r="I32" s="94"/>
+      <c r="J32" s="94"/>
+      <c r="K32" s="94"/>
+      <c r="L32" s="94"/>
+      <c r="M32" s="94"/>
+      <c r="N32" s="94"/>
       <c r="O32" s="2"/>
       <c r="P32" s="2"/>
       <c r="Q32" s="2"/>
@@ -2762,27 +2735,27 @@
     <row r="34" spans="1:22" s="10" customFormat="1" ht="13">
       <c r="A34" s="61"/>
       <c r="B34" s="31" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="C34" s="31" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="D34" s="62"/>
       <c r="E34" s="63"/>
       <c r="F34" s="31" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="G34" s="31" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="H34" s="63" t="s">
         <v>21</v>
       </c>
       <c r="I34" s="31" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="J34" s="64" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="K34" s="65"/>
       <c r="L34" s="33">
@@ -2892,27 +2865,27 @@
     <row r="37" spans="1:22" ht="13">
       <c r="A37" s="38"/>
       <c r="B37" s="71" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="C37" s="71" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="D37" s="38"/>
       <c r="E37" s="38"/>
       <c r="F37" s="71" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="G37" s="38" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="H37" s="38" t="s">
         <v>21</v>
       </c>
       <c r="I37" s="71" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="J37" s="72" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="K37" s="73"/>
       <c r="L37" s="74">
@@ -2934,27 +2907,27 @@
     <row r="38" spans="1:22" s="10" customFormat="1" ht="13">
       <c r="A38" s="22"/>
       <c r="B38" s="31" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="C38" s="31" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="D38" s="22"/>
       <c r="E38" s="22"/>
       <c r="F38" s="31" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="G38" s="22" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="H38" s="22" t="s">
         <v>21</v>
       </c>
       <c r="I38" s="31" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="J38" s="64" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="K38" s="70"/>
       <c r="L38" s="33">
@@ -2974,22 +2947,22 @@
       <c r="V38" s="12"/>
     </row>
     <row r="39" spans="1:22" ht="13">
-      <c r="A39" s="93" t="s">
+      <c r="A39" s="95" t="s">
         <v>170</v>
       </c>
-      <c r="B39" s="93"/>
-      <c r="C39" s="93"/>
-      <c r="D39" s="93"/>
-      <c r="E39" s="93"/>
-      <c r="F39" s="93"/>
-      <c r="G39" s="93"/>
-      <c r="H39" s="93"/>
-      <c r="I39" s="93"/>
-      <c r="J39" s="93"/>
-      <c r="K39" s="93"/>
-      <c r="L39" s="93"/>
-      <c r="M39" s="93"/>
-      <c r="N39" s="93"/>
+      <c r="B39" s="95"/>
+      <c r="C39" s="95"/>
+      <c r="D39" s="95"/>
+      <c r="E39" s="95"/>
+      <c r="F39" s="95"/>
+      <c r="G39" s="95"/>
+      <c r="H39" s="95"/>
+      <c r="I39" s="95"/>
+      <c r="J39" s="95"/>
+      <c r="K39" s="95"/>
+      <c r="L39" s="95"/>
+      <c r="M39" s="95"/>
+      <c r="N39" s="95"/>
       <c r="O39" s="2"/>
       <c r="P39" s="2"/>
       <c r="Q39" s="2"/>
@@ -2999,235 +2972,237 @@
       <c r="U39" s="2"/>
       <c r="V39" s="2"/>
     </row>
-    <row r="40" spans="1:22" ht="13">
-      <c r="A40" s="38"/>
-      <c r="B40" s="75" t="s">
+    <row r="40" spans="1:22" s="88" customFormat="1" ht="13">
+      <c r="A40" s="90"/>
+      <c r="B40" s="76" t="s">
         <v>171</v>
       </c>
-      <c r="C40" s="76" t="s">
+      <c r="C40" s="75" t="s">
         <v>172</v>
       </c>
-      <c r="D40" s="38"/>
-      <c r="E40" s="38"/>
-      <c r="F40" s="75" t="s">
+      <c r="D40" s="90"/>
+      <c r="E40" s="90"/>
+      <c r="F40" s="33" t="s">
+        <v>244</v>
+      </c>
+      <c r="G40" s="33" t="s">
+        <v>256</v>
+      </c>
+      <c r="H40" s="76" t="s">
+        <v>21</v>
+      </c>
+      <c r="I40" s="33" t="s">
+        <v>257</v>
+      </c>
+      <c r="J40" s="93" t="s">
+        <v>258</v>
+      </c>
+      <c r="K40" s="91"/>
+      <c r="L40" s="33">
+        <v>41649</v>
+      </c>
+      <c r="M40" s="92" t="s">
+        <v>60</v>
+      </c>
+      <c r="N40" s="90"/>
+      <c r="O40" s="87"/>
+      <c r="P40" s="87"/>
+      <c r="Q40" s="87"/>
+      <c r="R40" s="87"/>
+      <c r="S40" s="87"/>
+      <c r="T40" s="87"/>
+      <c r="U40" s="87"/>
+      <c r="V40" s="87"/>
+    </row>
+    <row r="41" spans="1:22" s="6" customFormat="1" ht="13">
+      <c r="A41" s="17"/>
+      <c r="B41" s="26" t="s">
+        <v>245</v>
+      </c>
+      <c r="C41" s="89" t="s">
+        <v>172</v>
+      </c>
+      <c r="D41" s="17"/>
+      <c r="E41" s="17"/>
+      <c r="F41" s="26" t="s">
+        <v>244</v>
+      </c>
+      <c r="G41" s="77" t="s">
+        <v>243</v>
+      </c>
+      <c r="H41" s="77" t="s">
+        <v>21</v>
+      </c>
+      <c r="I41" s="26" t="s">
+        <v>246</v>
+      </c>
+      <c r="J41" s="27" t="s">
+        <v>247</v>
+      </c>
+      <c r="K41" s="78"/>
+      <c r="L41" s="19" t="s">
+        <v>248</v>
+      </c>
+      <c r="M41" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="N41" s="17"/>
+      <c r="O41" s="5"/>
+      <c r="P41" s="5"/>
+      <c r="Q41" s="5"/>
+      <c r="R41" s="5"/>
+      <c r="S41" s="5"/>
+      <c r="T41" s="5"/>
+      <c r="U41" s="5"/>
+      <c r="V41" s="5"/>
+    </row>
+    <row r="42" spans="1:22" s="10" customFormat="1" ht="13">
+      <c r="A42" s="22"/>
+      <c r="B42" s="31" t="s">
+        <v>209</v>
+      </c>
+      <c r="C42" s="31" t="s">
+        <v>210</v>
+      </c>
+      <c r="D42" s="22"/>
+      <c r="E42" s="22"/>
+      <c r="F42" s="31" t="s">
+        <v>211</v>
+      </c>
+      <c r="G42" s="76" t="s">
+        <v>208</v>
+      </c>
+      <c r="H42" s="76" t="s">
+        <v>21</v>
+      </c>
+      <c r="I42" s="31" t="s">
+        <v>213</v>
+      </c>
+      <c r="J42" s="64" t="s">
+        <v>212</v>
+      </c>
+      <c r="K42" s="70"/>
+      <c r="L42" s="33">
+        <v>392</v>
+      </c>
+      <c r="M42" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="N42" s="22"/>
+      <c r="O42" s="7"/>
+      <c r="P42" s="7"/>
+      <c r="Q42" s="7"/>
+      <c r="R42" s="7"/>
+      <c r="S42" s="7"/>
+      <c r="T42" s="7"/>
+      <c r="U42" s="7"/>
+      <c r="V42" s="7"/>
+    </row>
+    <row r="43" spans="1:22" s="14" customFormat="1" ht="13">
+      <c r="A43" s="17"/>
+      <c r="B43" s="26" t="s">
+        <v>224</v>
+      </c>
+      <c r="C43" s="26" t="s">
+        <v>223</v>
+      </c>
+      <c r="D43" s="17"/>
+      <c r="E43" s="17"/>
+      <c r="F43" s="26" t="s">
+        <v>222</v>
+      </c>
+      <c r="G43" s="26" t="s">
+        <v>220</v>
+      </c>
+      <c r="H43" s="77" t="s">
+        <v>21</v>
+      </c>
+      <c r="I43" s="26" t="s">
+        <v>221</v>
+      </c>
+      <c r="J43" s="27" t="s">
+        <v>225</v>
+      </c>
+      <c r="K43" s="78"/>
+      <c r="L43" s="28">
+        <v>41306</v>
+      </c>
+      <c r="M43" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="N43" s="17"/>
+      <c r="O43" s="5"/>
+      <c r="P43" s="5"/>
+      <c r="Q43" s="5"/>
+      <c r="R43" s="5"/>
+      <c r="S43" s="5"/>
+      <c r="T43" s="5"/>
+      <c r="U43" s="5"/>
+      <c r="V43" s="5"/>
+    </row>
+    <row r="44" spans="1:22" ht="13">
+      <c r="A44" s="95" t="s">
         <v>173</v>
       </c>
-      <c r="G40" s="75" t="s">
+      <c r="B44" s="95"/>
+      <c r="C44" s="95"/>
+      <c r="D44" s="95"/>
+      <c r="E44" s="95"/>
+      <c r="F44" s="95"/>
+      <c r="G44" s="95"/>
+      <c r="H44" s="95"/>
+      <c r="I44" s="95"/>
+      <c r="J44" s="95"/>
+      <c r="K44" s="95"/>
+      <c r="L44" s="95"/>
+      <c r="M44" s="95"/>
+      <c r="N44" s="95"/>
+      <c r="O44" s="2"/>
+      <c r="P44" s="2"/>
+      <c r="Q44" s="2"/>
+      <c r="R44" s="2"/>
+      <c r="S44" s="2"/>
+      <c r="T44" s="2"/>
+      <c r="U44" s="2"/>
+      <c r="V44" s="2"/>
+    </row>
+    <row r="45" spans="1:22" ht="13">
+      <c r="A45" s="38"/>
+      <c r="B45" s="79" t="s">
         <v>174</v>
       </c>
-      <c r="H40" s="75" t="s">
+      <c r="C45" s="42" t="s">
+        <v>175</v>
+      </c>
+      <c r="D45" s="38" t="s">
+        <v>176</v>
+      </c>
+      <c r="E45" s="38"/>
+      <c r="F45" s="40" t="s">
+        <v>177</v>
+      </c>
+      <c r="G45" s="40" t="s">
+        <v>178</v>
+      </c>
+      <c r="H45" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="I40" s="75" t="s">
-        <v>175</v>
-      </c>
-      <c r="J40" s="77" t="s">
-        <v>176</v>
-      </c>
-      <c r="K40" s="73"/>
-      <c r="L40" s="39" t="s">
-        <v>177</v>
-      </c>
-      <c r="M40" s="39" t="s">
+      <c r="I45" s="40" t="s">
+        <v>179</v>
+      </c>
+      <c r="J45" s="80" t="s">
+        <v>180</v>
+      </c>
+      <c r="K45" s="73"/>
+      <c r="L45" s="81" t="s">
+        <v>181</v>
+      </c>
+      <c r="M45" s="39" t="s">
         <v>60</v>
       </c>
-      <c r="N40" s="38" t="s">
-        <v>178</v>
-      </c>
-      <c r="O40" s="2"/>
-      <c r="P40" s="2"/>
-      <c r="Q40" s="2"/>
-      <c r="R40" s="2"/>
-      <c r="S40" s="2"/>
-      <c r="T40" s="2"/>
-      <c r="U40" s="2"/>
-      <c r="V40" s="2"/>
-    </row>
-    <row r="41" spans="1:22" s="91" customFormat="1" ht="13">
-      <c r="A41" s="96"/>
-      <c r="B41" s="79" t="s">
-        <v>171</v>
-      </c>
-      <c r="C41" s="78" t="s">
-        <v>172</v>
-      </c>
-      <c r="D41" s="96"/>
-      <c r="E41" s="96"/>
-      <c r="F41" s="33" t="s">
-        <v>250</v>
-      </c>
-      <c r="G41" s="33" t="s">
-        <v>262</v>
-      </c>
-      <c r="H41" s="79" t="s">
-        <v>21</v>
-      </c>
-      <c r="I41" s="33" t="s">
-        <v>263</v>
-      </c>
-      <c r="J41" s="99" t="s">
-        <v>264</v>
-      </c>
-      <c r="K41" s="97"/>
-      <c r="L41" s="33">
-        <v>41649</v>
-      </c>
-      <c r="M41" s="98" t="s">
-        <v>60</v>
-      </c>
-      <c r="N41" s="96"/>
-      <c r="O41" s="90"/>
-      <c r="P41" s="90"/>
-      <c r="Q41" s="90"/>
-      <c r="R41" s="90"/>
-      <c r="S41" s="90"/>
-      <c r="T41" s="90"/>
-      <c r="U41" s="90"/>
-      <c r="V41" s="90"/>
-    </row>
-    <row r="42" spans="1:22" s="6" customFormat="1" ht="13">
-      <c r="A42" s="17"/>
-      <c r="B42" s="26" t="s">
-        <v>251</v>
-      </c>
-      <c r="C42" s="95" t="s">
-        <v>172</v>
-      </c>
-      <c r="D42" s="17"/>
-      <c r="E42" s="17"/>
-      <c r="F42" s="26" t="s">
-        <v>250</v>
-      </c>
-      <c r="G42" s="80" t="s">
-        <v>249</v>
-      </c>
-      <c r="H42" s="80" t="s">
-        <v>21</v>
-      </c>
-      <c r="I42" s="26" t="s">
-        <v>252</v>
-      </c>
-      <c r="J42" s="27" t="s">
-        <v>253</v>
-      </c>
-      <c r="K42" s="81"/>
-      <c r="L42" s="19" t="s">
-        <v>254</v>
-      </c>
-      <c r="M42" s="19" t="s">
-        <v>60</v>
-      </c>
-      <c r="N42" s="17"/>
-      <c r="O42" s="5"/>
-      <c r="P42" s="5"/>
-      <c r="Q42" s="5"/>
-      <c r="R42" s="5"/>
-      <c r="S42" s="5"/>
-      <c r="T42" s="5"/>
-      <c r="U42" s="5"/>
-      <c r="V42" s="5"/>
-    </row>
-    <row r="43" spans="1:22" s="10" customFormat="1" ht="13">
-      <c r="A43" s="22"/>
-      <c r="B43" s="31" t="s">
-        <v>215</v>
-      </c>
-      <c r="C43" s="31" t="s">
-        <v>216</v>
-      </c>
-      <c r="D43" s="22"/>
-      <c r="E43" s="22"/>
-      <c r="F43" s="31" t="s">
-        <v>217</v>
-      </c>
-      <c r="G43" s="79" t="s">
-        <v>214</v>
-      </c>
-      <c r="H43" s="79" t="s">
-        <v>21</v>
-      </c>
-      <c r="I43" s="31" t="s">
-        <v>219</v>
-      </c>
-      <c r="J43" s="64" t="s">
-        <v>218</v>
-      </c>
-      <c r="K43" s="70"/>
-      <c r="L43" s="33">
-        <v>392</v>
-      </c>
-      <c r="M43" s="23" t="s">
-        <v>60</v>
-      </c>
-      <c r="N43" s="22"/>
-      <c r="O43" s="7"/>
-      <c r="P43" s="7"/>
-      <c r="Q43" s="7"/>
-      <c r="R43" s="7"/>
-      <c r="S43" s="7"/>
-      <c r="T43" s="7"/>
-      <c r="U43" s="7"/>
-      <c r="V43" s="7"/>
-    </row>
-    <row r="44" spans="1:22" s="14" customFormat="1" ht="13">
-      <c r="A44" s="17"/>
-      <c r="B44" s="26" t="s">
-        <v>230</v>
-      </c>
-      <c r="C44" s="26" t="s">
-        <v>229</v>
-      </c>
-      <c r="D44" s="17"/>
-      <c r="E44" s="17"/>
-      <c r="F44" s="26" t="s">
-        <v>228</v>
-      </c>
-      <c r="G44" s="26" t="s">
-        <v>226</v>
-      </c>
-      <c r="H44" s="80" t="s">
-        <v>21</v>
-      </c>
-      <c r="I44" s="26" t="s">
-        <v>227</v>
-      </c>
-      <c r="J44" s="27" t="s">
-        <v>231</v>
-      </c>
-      <c r="K44" s="81"/>
-      <c r="L44" s="28">
-        <v>41306</v>
-      </c>
-      <c r="M44" s="19" t="s">
-        <v>60</v>
-      </c>
-      <c r="N44" s="17"/>
-      <c r="O44" s="5"/>
-      <c r="P44" s="5"/>
-      <c r="Q44" s="5"/>
-      <c r="R44" s="5"/>
-      <c r="S44" s="5"/>
-      <c r="T44" s="5"/>
-      <c r="U44" s="5"/>
-      <c r="V44" s="5"/>
-    </row>
-    <row r="45" spans="1:22" ht="13">
-      <c r="A45" s="93" t="s">
-        <v>179</v>
-      </c>
-      <c r="B45" s="93"/>
-      <c r="C45" s="93"/>
-      <c r="D45" s="93"/>
-      <c r="E45" s="93"/>
-      <c r="F45" s="93"/>
-      <c r="G45" s="93"/>
-      <c r="H45" s="93"/>
-      <c r="I45" s="93"/>
-      <c r="J45" s="93"/>
-      <c r="K45" s="93"/>
-      <c r="L45" s="93"/>
-      <c r="M45" s="93"/>
-      <c r="N45" s="93"/>
+      <c r="N45" s="38" t="s">
+        <v>182</v>
+      </c>
       <c r="O45" s="2"/>
       <c r="P45" s="2"/>
       <c r="Q45" s="2"/>
@@ -3238,42 +3213,40 @@
       <c r="V45" s="2"/>
     </row>
     <row r="46" spans="1:22" ht="13">
-      <c r="A46" s="38"/>
-      <c r="B46" s="82" t="s">
-        <v>180</v>
-      </c>
-      <c r="C46" s="42" t="s">
-        <v>181</v>
-      </c>
-      <c r="D46" s="38" t="s">
-        <v>182</v>
-      </c>
-      <c r="E46" s="38"/>
-      <c r="F46" s="40" t="s">
+      <c r="A46" s="43"/>
+      <c r="B46" s="44" t="s">
         <v>183</v>
       </c>
-      <c r="G46" s="40" t="s">
+      <c r="C46" s="47" t="s">
         <v>184</v>
       </c>
-      <c r="H46" s="38" t="s">
+      <c r="D46" s="43" t="s">
+        <v>185</v>
+      </c>
+      <c r="E46" s="43"/>
+      <c r="F46" s="44" t="s">
+        <v>177</v>
+      </c>
+      <c r="G46" s="43" t="s">
+        <v>186</v>
+      </c>
+      <c r="H46" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="I46" s="40" t="s">
-        <v>185</v>
-      </c>
-      <c r="J46" s="83" t="s">
-        <v>186</v>
-      </c>
-      <c r="K46" s="73"/>
-      <c r="L46" s="84" t="s">
+      <c r="I46" s="44" t="s">
         <v>187</v>
       </c>
-      <c r="M46" s="39" t="s">
+      <c r="J46" s="46" t="s">
+        <v>188</v>
+      </c>
+      <c r="K46" s="43"/>
+      <c r="L46" s="82">
+        <v>2019</v>
+      </c>
+      <c r="M46" s="45" t="s">
         <v>60</v>
       </c>
-      <c r="N46" s="38" t="s">
-        <v>188</v>
-      </c>
+      <c r="N46" s="43"/>
       <c r="O46" s="2"/>
       <c r="P46" s="2"/>
       <c r="Q46" s="2"/>
@@ -3281,43 +3254,24 @@
       <c r="S46" s="2"/>
       <c r="T46" s="2"/>
       <c r="U46" s="2"/>
-      <c r="V46" s="2"/>
     </row>
     <row r="47" spans="1:22" ht="13">
-      <c r="A47" s="43"/>
-      <c r="B47" s="44" t="s">
-        <v>189</v>
-      </c>
-      <c r="C47" s="47" t="s">
-        <v>190</v>
-      </c>
-      <c r="D47" s="43" t="s">
-        <v>191</v>
-      </c>
-      <c r="E47" s="43"/>
-      <c r="F47" s="44" t="s">
-        <v>183</v>
-      </c>
-      <c r="G47" s="43" t="s">
-        <v>192</v>
-      </c>
-      <c r="H47" s="43" t="s">
-        <v>21</v>
-      </c>
-      <c r="I47" s="44" t="s">
-        <v>193</v>
-      </c>
-      <c r="J47" s="46" t="s">
-        <v>194</v>
-      </c>
-      <c r="K47" s="43"/>
-      <c r="L47" s="85">
-        <v>2019</v>
-      </c>
-      <c r="M47" s="45" t="s">
-        <v>60</v>
-      </c>
-      <c r="N47" s="43"/>
+      <c r="A47" s="95" t="s">
+        <v>214</v>
+      </c>
+      <c r="B47" s="95"/>
+      <c r="C47" s="95"/>
+      <c r="D47" s="95"/>
+      <c r="E47" s="95"/>
+      <c r="F47" s="95"/>
+      <c r="G47" s="95"/>
+      <c r="H47" s="95"/>
+      <c r="I47" s="95"/>
+      <c r="J47" s="95"/>
+      <c r="K47" s="95"/>
+      <c r="L47" s="95"/>
+      <c r="M47" s="95"/>
+      <c r="N47" s="95"/>
       <c r="O47" s="2"/>
       <c r="P47" s="2"/>
       <c r="Q47" s="2"/>
@@ -3325,64 +3279,63 @@
       <c r="S47" s="2"/>
       <c r="T47" s="2"/>
       <c r="U47" s="2"/>
-    </row>
-    <row r="48" spans="1:22" ht="13">
-      <c r="A48" s="93" t="s">
-        <v>220</v>
-      </c>
-      <c r="B48" s="93"/>
-      <c r="C48" s="93"/>
-      <c r="D48" s="93"/>
-      <c r="E48" s="93"/>
-      <c r="F48" s="93"/>
-      <c r="G48" s="93"/>
-      <c r="H48" s="93"/>
-      <c r="I48" s="93"/>
-      <c r="J48" s="93"/>
-      <c r="K48" s="93"/>
-      <c r="L48" s="93"/>
-      <c r="M48" s="93"/>
-      <c r="N48" s="93"/>
-      <c r="O48" s="2"/>
-      <c r="P48" s="2"/>
-      <c r="Q48" s="2"/>
-      <c r="R48" s="2"/>
-      <c r="S48" s="2"/>
-      <c r="T48" s="2"/>
-      <c r="U48" s="2"/>
-      <c r="V48" s="2"/>
-    </row>
-    <row r="49" spans="1:22" s="4" customFormat="1" ht="13">
-      <c r="A49" s="86"/>
-      <c r="B49" s="71" t="s">
-        <v>225</v>
-      </c>
-      <c r="C49" s="86"/>
-      <c r="D49" s="86"/>
-      <c r="E49" s="86"/>
-      <c r="F49" s="71" t="s">
-        <v>221</v>
-      </c>
-      <c r="G49" s="71" t="s">
-        <v>222</v>
-      </c>
-      <c r="H49" s="38" t="s">
+      <c r="V47" s="2"/>
+    </row>
+    <row r="48" spans="1:22" s="4" customFormat="1" ht="13">
+      <c r="A48" s="83"/>
+      <c r="B48" s="71" t="s">
+        <v>219</v>
+      </c>
+      <c r="C48" s="83"/>
+      <c r="D48" s="83"/>
+      <c r="E48" s="83"/>
+      <c r="F48" s="71" t="s">
+        <v>215</v>
+      </c>
+      <c r="G48" s="71" t="s">
+        <v>216</v>
+      </c>
+      <c r="H48" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="I49" s="71" t="s">
-        <v>223</v>
-      </c>
-      <c r="J49" s="72" t="s">
-        <v>224</v>
-      </c>
-      <c r="K49" s="86"/>
-      <c r="L49" s="74">
+      <c r="I48" s="71" t="s">
+        <v>217</v>
+      </c>
+      <c r="J48" s="72" t="s">
+        <v>218</v>
+      </c>
+      <c r="K48" s="83"/>
+      <c r="L48" s="74">
         <v>4957</v>
       </c>
-      <c r="M49" s="39" t="s">
+      <c r="M48" s="39" t="s">
         <v>60</v>
       </c>
-      <c r="N49" s="86"/>
+      <c r="N48" s="83"/>
+      <c r="O48" s="1"/>
+      <c r="P48" s="1"/>
+      <c r="Q48" s="1"/>
+      <c r="R48" s="1"/>
+      <c r="S48" s="1"/>
+      <c r="T48" s="1"/>
+      <c r="U48" s="1"/>
+      <c r="V48" s="1"/>
+    </row>
+    <row r="49" spans="1:22" ht="12.5" hidden="1">
+      <c r="A49" s="1"/>
+      <c r="B49" s="1"/>
+      <c r="C49" s="1"/>
+      <c r="D49" s="1"/>
+      <c r="E49" s="1"/>
+      <c r="F49" s="1"/>
+      <c r="G49" s="1"/>
+      <c r="H49" s="1"/>
+      <c r="I49" s="1"/>
+      <c r="J49" s="1"/>
+      <c r="K49" s="1"/>
+      <c r="L49" s="1"/>
+      <c r="M49" s="1"/>
+      <c r="N49" s="1"/>
       <c r="O49" s="1"/>
       <c r="P49" s="1"/>
       <c r="Q49" s="1"/>
@@ -25088,36 +25041,13 @@
       <c r="U953" s="1"/>
       <c r="V953" s="1"/>
     </row>
-    <row r="954" spans="1:22" ht="12.5" hidden="1">
-      <c r="A954" s="1"/>
-      <c r="B954" s="1"/>
-      <c r="C954" s="1"/>
-      <c r="D954" s="1"/>
-      <c r="E954" s="1"/>
-      <c r="F954" s="1"/>
-      <c r="G954" s="1"/>
-      <c r="H954" s="1"/>
-      <c r="I954" s="1"/>
-      <c r="J954" s="1"/>
-      <c r="K954" s="1"/>
-      <c r="L954" s="1"/>
-      <c r="M954" s="1"/>
-      <c r="N954" s="1"/>
-      <c r="O954" s="1"/>
-      <c r="P954" s="1"/>
-      <c r="Q954" s="1"/>
-      <c r="R954" s="1"/>
-      <c r="S954" s="1"/>
-      <c r="T954" s="1"/>
-      <c r="U954" s="1"/>
-      <c r="V954" s="1"/>
-    </row>
+    <row r="954" spans="1:22" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="9">
     <mergeCell ref="A32:N32"/>
     <mergeCell ref="A39:N39"/>
-    <mergeCell ref="A45:N45"/>
-    <mergeCell ref="A48:N48"/>
+    <mergeCell ref="A44:N44"/>
+    <mergeCell ref="A47:N47"/>
     <mergeCell ref="A1:N1"/>
     <mergeCell ref="A3:N3"/>
     <mergeCell ref="A14:N14"/>

</xml_diff>

<commit_message>
Adding power on led
</commit_message>
<xml_diff>
--- a/BOM/MIMXRT1064 MCU Module  - BOM.xlsx
+++ b/BOM/MIMXRT1064 MCU Module  - BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\32470\Documents\GitHub\MIMXRT1064-MCU-Module\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04F87890-C499-4A07-9712-73162693FD44}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7CB67F9-99FB-4982-AF40-41481354B8D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="264">
   <si>
     <t>MIMXRT1064 MCU Module  - BOM</t>
   </si>
@@ -798,6 +798,21 @@
   </si>
   <si>
     <t>$0.0942</t>
+  </si>
+  <si>
+    <t>19-218_BHC-ZL1M2QY_3T</t>
+  </si>
+  <si>
+    <t>C264488</t>
+  </si>
+  <si>
+    <t>Everlight Elec</t>
+  </si>
+  <si>
+    <t>$0.064</t>
+  </si>
+  <si>
+    <t>blue 0603 Light Emitting Diodes</t>
   </si>
 </sst>
 </file>
@@ -979,7 +994,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="97">
+  <cellXfs count="103">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1120,21 +1135,39 @@
     <xf numFmtId="49" fontId="7" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1355,10 +1388,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:V954"/>
+  <dimension ref="A1:V955"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40:XFD40"/>
+      <selection activeCell="A32" sqref="A32:N32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15.75" customHeight="1" zeroHeight="1"/>
@@ -1381,22 +1414,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="30" customHeight="1">
-      <c r="A1" s="96" t="s">
+      <c r="A1" s="93" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="96"/>
-      <c r="C1" s="96"/>
-      <c r="D1" s="96"/>
-      <c r="E1" s="96"/>
-      <c r="F1" s="96"/>
-      <c r="G1" s="96"/>
-      <c r="H1" s="96"/>
-      <c r="I1" s="96"/>
-      <c r="J1" s="96"/>
-      <c r="K1" s="96"/>
-      <c r="L1" s="96"/>
-      <c r="M1" s="96"/>
-      <c r="N1" s="96"/>
+      <c r="B1" s="93"/>
+      <c r="C1" s="93"/>
+      <c r="D1" s="93"/>
+      <c r="E1" s="93"/>
+      <c r="F1" s="93"/>
+      <c r="G1" s="93"/>
+      <c r="H1" s="93"/>
+      <c r="I1" s="93"/>
+      <c r="J1" s="93"/>
+      <c r="K1" s="93"/>
+      <c r="L1" s="93"/>
+      <c r="M1" s="93"/>
+      <c r="N1" s="93"/>
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
@@ -1459,22 +1492,22 @@
       <c r="V2" s="1"/>
     </row>
     <row r="3" spans="1:22" ht="13">
-      <c r="A3" s="95" t="s">
+      <c r="A3" s="92" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="95"/>
-      <c r="C3" s="95"/>
-      <c r="D3" s="95"/>
-      <c r="E3" s="95"/>
-      <c r="F3" s="95"/>
-      <c r="G3" s="95"/>
-      <c r="H3" s="95"/>
-      <c r="I3" s="95"/>
-      <c r="J3" s="95"/>
-      <c r="K3" s="95"/>
-      <c r="L3" s="95"/>
-      <c r="M3" s="95"/>
-      <c r="N3" s="95"/>
+      <c r="B3" s="92"/>
+      <c r="C3" s="92"/>
+      <c r="D3" s="92"/>
+      <c r="E3" s="92"/>
+      <c r="F3" s="92"/>
+      <c r="G3" s="92"/>
+      <c r="H3" s="92"/>
+      <c r="I3" s="92"/>
+      <c r="J3" s="92"/>
+      <c r="K3" s="92"/>
+      <c r="L3" s="92"/>
+      <c r="M3" s="92"/>
+      <c r="N3" s="92"/>
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
@@ -1925,22 +1958,22 @@
       <c r="V13" s="13"/>
     </row>
     <row r="14" spans="1:22" ht="13">
-      <c r="A14" s="95" t="s">
+      <c r="A14" s="92" t="s">
         <v>61</v>
       </c>
-      <c r="B14" s="95"/>
-      <c r="C14" s="95"/>
-      <c r="D14" s="95"/>
-      <c r="E14" s="95"/>
-      <c r="F14" s="95"/>
-      <c r="G14" s="95"/>
-      <c r="H14" s="95"/>
-      <c r="I14" s="95"/>
-      <c r="J14" s="95"/>
-      <c r="K14" s="95"/>
-      <c r="L14" s="95"/>
-      <c r="M14" s="95"/>
-      <c r="N14" s="95"/>
+      <c r="B14" s="92"/>
+      <c r="C14" s="92"/>
+      <c r="D14" s="92"/>
+      <c r="E14" s="92"/>
+      <c r="F14" s="92"/>
+      <c r="G14" s="92"/>
+      <c r="H14" s="92"/>
+      <c r="I14" s="92"/>
+      <c r="J14" s="92"/>
+      <c r="K14" s="92"/>
+      <c r="L14" s="92"/>
+      <c r="M14" s="92"/>
+      <c r="N14" s="92"/>
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
       <c r="Q14" s="1"/>
@@ -2391,22 +2424,22 @@
       <c r="V24" s="2"/>
     </row>
     <row r="25" spans="1:22" ht="13">
-      <c r="A25" s="95" t="s">
+      <c r="A25" s="92" t="s">
         <v>124</v>
       </c>
-      <c r="B25" s="95"/>
-      <c r="C25" s="95"/>
-      <c r="D25" s="95"/>
-      <c r="E25" s="95"/>
-      <c r="F25" s="95"/>
-      <c r="G25" s="95"/>
-      <c r="H25" s="95"/>
-      <c r="I25" s="95"/>
-      <c r="J25" s="95"/>
-      <c r="K25" s="95"/>
-      <c r="L25" s="95"/>
-      <c r="M25" s="95"/>
-      <c r="N25" s="95"/>
+      <c r="B25" s="92"/>
+      <c r="C25" s="92"/>
+      <c r="D25" s="92"/>
+      <c r="E25" s="92"/>
+      <c r="F25" s="92"/>
+      <c r="G25" s="92"/>
+      <c r="H25" s="92"/>
+      <c r="I25" s="92"/>
+      <c r="J25" s="92"/>
+      <c r="K25" s="92"/>
+      <c r="L25" s="92"/>
+      <c r="M25" s="92"/>
+      <c r="N25" s="92"/>
       <c r="O25" s="2"/>
       <c r="P25" s="2"/>
       <c r="Q25" s="2"/>
@@ -2572,7 +2605,7 @@
       <c r="I29" s="33" t="s">
         <v>254</v>
       </c>
-      <c r="J29" s="93" t="s">
+      <c r="J29" s="90" t="s">
         <v>255</v>
       </c>
       <c r="K29" s="84"/>
@@ -2593,22 +2626,22 @@
       <c r="V29" s="87"/>
     </row>
     <row r="30" spans="1:22" ht="13">
-      <c r="A30" s="95" t="s">
+      <c r="A30" s="92" t="s">
         <v>140</v>
       </c>
-      <c r="B30" s="95"/>
-      <c r="C30" s="95"/>
-      <c r="D30" s="95"/>
-      <c r="E30" s="95"/>
-      <c r="F30" s="95"/>
-      <c r="G30" s="95"/>
-      <c r="H30" s="95"/>
-      <c r="I30" s="95"/>
-      <c r="J30" s="95"/>
-      <c r="K30" s="95"/>
-      <c r="L30" s="95"/>
-      <c r="M30" s="95"/>
-      <c r="N30" s="95"/>
+      <c r="B30" s="92"/>
+      <c r="C30" s="92"/>
+      <c r="D30" s="92"/>
+      <c r="E30" s="92"/>
+      <c r="F30" s="92"/>
+      <c r="G30" s="92"/>
+      <c r="H30" s="92"/>
+      <c r="I30" s="92"/>
+      <c r="J30" s="92"/>
+      <c r="K30" s="92"/>
+      <c r="L30" s="92"/>
+      <c r="M30" s="92"/>
+      <c r="N30" s="92"/>
       <c r="O30" s="2"/>
       <c r="P30" s="2"/>
       <c r="Q30" s="2"/>
@@ -2663,22 +2696,22 @@
       <c r="V31" s="2"/>
     </row>
     <row r="32" spans="1:22" ht="13">
-      <c r="A32" s="94" t="s">
+      <c r="A32" s="91" t="s">
         <v>148</v>
       </c>
-      <c r="B32" s="94"/>
-      <c r="C32" s="94"/>
-      <c r="D32" s="94"/>
-      <c r="E32" s="94"/>
-      <c r="F32" s="94"/>
-      <c r="G32" s="94"/>
-      <c r="H32" s="94"/>
-      <c r="I32" s="94"/>
-      <c r="J32" s="94"/>
-      <c r="K32" s="94"/>
-      <c r="L32" s="94"/>
-      <c r="M32" s="94"/>
-      <c r="N32" s="94"/>
+      <c r="B32" s="91"/>
+      <c r="C32" s="91"/>
+      <c r="D32" s="91"/>
+      <c r="E32" s="91"/>
+      <c r="F32" s="91"/>
+      <c r="G32" s="91"/>
+      <c r="H32" s="91"/>
+      <c r="I32" s="91"/>
+      <c r="J32" s="91"/>
+      <c r="K32" s="91"/>
+      <c r="L32" s="91"/>
+      <c r="M32" s="91"/>
+      <c r="N32" s="91"/>
       <c r="O32" s="2"/>
       <c r="P32" s="2"/>
       <c r="Q32" s="2"/>
@@ -2947,22 +2980,22 @@
       <c r="V38" s="12"/>
     </row>
     <row r="39" spans="1:22" ht="13">
-      <c r="A39" s="95" t="s">
+      <c r="A39" s="92" t="s">
         <v>170</v>
       </c>
-      <c r="B39" s="95"/>
-      <c r="C39" s="95"/>
-      <c r="D39" s="95"/>
-      <c r="E39" s="95"/>
-      <c r="F39" s="95"/>
-      <c r="G39" s="95"/>
-      <c r="H39" s="95"/>
-      <c r="I39" s="95"/>
-      <c r="J39" s="95"/>
-      <c r="K39" s="95"/>
-      <c r="L39" s="95"/>
-      <c r="M39" s="95"/>
-      <c r="N39" s="95"/>
+      <c r="B39" s="92"/>
+      <c r="C39" s="92"/>
+      <c r="D39" s="92"/>
+      <c r="E39" s="92"/>
+      <c r="F39" s="92"/>
+      <c r="G39" s="92"/>
+      <c r="H39" s="92"/>
+      <c r="I39" s="92"/>
+      <c r="J39" s="92"/>
+      <c r="K39" s="92"/>
+      <c r="L39" s="92"/>
+      <c r="M39" s="92"/>
+      <c r="N39" s="92"/>
       <c r="O39" s="2"/>
       <c r="P39" s="2"/>
       <c r="Q39" s="2"/>
@@ -2972,237 +3005,233 @@
       <c r="U39" s="2"/>
       <c r="V39" s="2"/>
     </row>
-    <row r="40" spans="1:22" s="88" customFormat="1" ht="13">
-      <c r="A40" s="90"/>
-      <c r="B40" s="76" t="s">
+    <row r="40" spans="1:22" s="101" customFormat="1" ht="13">
+      <c r="A40" s="94"/>
+      <c r="B40" s="77" t="s">
         <v>171</v>
       </c>
-      <c r="C40" s="75" t="s">
+      <c r="C40" s="89" t="s">
         <v>172</v>
       </c>
-      <c r="D40" s="90"/>
-      <c r="E40" s="90"/>
-      <c r="F40" s="33" t="s">
+      <c r="D40" s="94"/>
+      <c r="E40" s="94"/>
+      <c r="F40" s="28" t="s">
         <v>244</v>
       </c>
-      <c r="G40" s="33" t="s">
+      <c r="G40" s="28" t="s">
         <v>256</v>
       </c>
-      <c r="H40" s="76" t="s">
+      <c r="H40" s="77" t="s">
         <v>21</v>
       </c>
-      <c r="I40" s="33" t="s">
+      <c r="I40" s="28" t="s">
         <v>257</v>
       </c>
-      <c r="J40" s="93" t="s">
+      <c r="J40" s="102" t="s">
         <v>258</v>
       </c>
-      <c r="K40" s="91"/>
-      <c r="L40" s="33">
+      <c r="K40" s="98"/>
+      <c r="L40" s="28">
         <v>41649</v>
       </c>
-      <c r="M40" s="92" t="s">
+      <c r="M40" s="99" t="s">
         <v>60</v>
       </c>
-      <c r="N40" s="90"/>
-      <c r="O40" s="87"/>
-      <c r="P40" s="87"/>
-      <c r="Q40" s="87"/>
-      <c r="R40" s="87"/>
-      <c r="S40" s="87"/>
-      <c r="T40" s="87"/>
-      <c r="U40" s="87"/>
-      <c r="V40" s="87"/>
-    </row>
-    <row r="41" spans="1:22" s="6" customFormat="1" ht="13">
-      <c r="A41" s="17"/>
-      <c r="B41" s="26" t="s">
+      <c r="N40" s="94"/>
+      <c r="O40" s="100"/>
+      <c r="P40" s="100"/>
+      <c r="Q40" s="100"/>
+      <c r="R40" s="100"/>
+      <c r="S40" s="100"/>
+      <c r="T40" s="100"/>
+      <c r="U40" s="100"/>
+      <c r="V40" s="100"/>
+    </row>
+    <row r="41" spans="1:22" s="8" customFormat="1" ht="13">
+      <c r="A41" s="22"/>
+      <c r="B41" s="31" t="s">
         <v>245</v>
       </c>
-      <c r="C41" s="89" t="s">
+      <c r="C41" s="75" t="s">
         <v>172</v>
       </c>
-      <c r="D41" s="17"/>
-      <c r="E41" s="17"/>
-      <c r="F41" s="26" t="s">
+      <c r="D41" s="22"/>
+      <c r="E41" s="22"/>
+      <c r="F41" s="31" t="s">
         <v>244</v>
       </c>
-      <c r="G41" s="77" t="s">
+      <c r="G41" s="76" t="s">
         <v>243</v>
       </c>
-      <c r="H41" s="77" t="s">
+      <c r="H41" s="76" t="s">
         <v>21</v>
       </c>
-      <c r="I41" s="26" t="s">
+      <c r="I41" s="31" t="s">
         <v>246</v>
       </c>
-      <c r="J41" s="27" t="s">
+      <c r="J41" s="64" t="s">
         <v>247</v>
       </c>
-      <c r="K41" s="78"/>
-      <c r="L41" s="19" t="s">
+      <c r="K41" s="70"/>
+      <c r="L41" s="23" t="s">
         <v>248</v>
       </c>
-      <c r="M41" s="19" t="s">
+      <c r="M41" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="N41" s="17"/>
-      <c r="O41" s="5"/>
-      <c r="P41" s="5"/>
-      <c r="Q41" s="5"/>
-      <c r="R41" s="5"/>
-      <c r="S41" s="5"/>
-      <c r="T41" s="5"/>
-      <c r="U41" s="5"/>
-      <c r="V41" s="5"/>
-    </row>
-    <row r="42" spans="1:22" s="10" customFormat="1" ht="13">
-      <c r="A42" s="22"/>
-      <c r="B42" s="31" t="s">
+      <c r="N41" s="22"/>
+      <c r="O41" s="7"/>
+      <c r="P41" s="7"/>
+      <c r="Q41" s="7"/>
+      <c r="R41" s="7"/>
+      <c r="S41" s="7"/>
+      <c r="T41" s="7"/>
+      <c r="U41" s="7"/>
+      <c r="V41" s="7"/>
+    </row>
+    <row r="42" spans="1:22" s="14" customFormat="1" ht="13">
+      <c r="A42" s="17"/>
+      <c r="B42" s="26" t="s">
         <v>209</v>
       </c>
-      <c r="C42" s="31" t="s">
+      <c r="C42" s="26" t="s">
         <v>210</v>
       </c>
-      <c r="D42" s="22"/>
-      <c r="E42" s="22"/>
-      <c r="F42" s="31" t="s">
+      <c r="D42" s="17"/>
+      <c r="E42" s="17"/>
+      <c r="F42" s="26" t="s">
         <v>211</v>
       </c>
-      <c r="G42" s="76" t="s">
+      <c r="G42" s="77" t="s">
         <v>208</v>
       </c>
-      <c r="H42" s="76" t="s">
+      <c r="H42" s="77" t="s">
         <v>21</v>
       </c>
-      <c r="I42" s="31" t="s">
+      <c r="I42" s="26" t="s">
         <v>213</v>
       </c>
-      <c r="J42" s="64" t="s">
+      <c r="J42" s="27" t="s">
         <v>212</v>
       </c>
-      <c r="K42" s="70"/>
-      <c r="L42" s="33">
+      <c r="K42" s="78"/>
+      <c r="L42" s="28">
         <v>392</v>
       </c>
-      <c r="M42" s="23" t="s">
+      <c r="M42" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="N42" s="22"/>
-      <c r="O42" s="7"/>
-      <c r="P42" s="7"/>
-      <c r="Q42" s="7"/>
-      <c r="R42" s="7"/>
-      <c r="S42" s="7"/>
-      <c r="T42" s="7"/>
-      <c r="U42" s="7"/>
-      <c r="V42" s="7"/>
-    </row>
-    <row r="43" spans="1:22" s="14" customFormat="1" ht="13">
-      <c r="A43" s="17"/>
-      <c r="B43" s="26" t="s">
+      <c r="N42" s="17"/>
+      <c r="O42" s="5"/>
+      <c r="P42" s="5"/>
+      <c r="Q42" s="5"/>
+      <c r="R42" s="5"/>
+      <c r="S42" s="5"/>
+      <c r="T42" s="5"/>
+      <c r="U42" s="5"/>
+      <c r="V42" s="5"/>
+    </row>
+    <row r="43" spans="1:22" s="10" customFormat="1" ht="13">
+      <c r="A43" s="22"/>
+      <c r="B43" s="31" t="s">
         <v>224</v>
       </c>
-      <c r="C43" s="26" t="s">
+      <c r="C43" s="31" t="s">
         <v>223</v>
       </c>
-      <c r="D43" s="17"/>
-      <c r="E43" s="17"/>
-      <c r="F43" s="26" t="s">
+      <c r="D43" s="22"/>
+      <c r="E43" s="22"/>
+      <c r="F43" s="31" t="s">
         <v>222</v>
       </c>
-      <c r="G43" s="26" t="s">
+      <c r="G43" s="31" t="s">
         <v>220</v>
       </c>
-      <c r="H43" s="77" t="s">
+      <c r="H43" s="76" t="s">
         <v>21</v>
       </c>
-      <c r="I43" s="26" t="s">
+      <c r="I43" s="31" t="s">
         <v>221</v>
       </c>
-      <c r="J43" s="27" t="s">
+      <c r="J43" s="64" t="s">
         <v>225</v>
       </c>
-      <c r="K43" s="78"/>
-      <c r="L43" s="28">
+      <c r="K43" s="70"/>
+      <c r="L43" s="33">
         <v>41306</v>
       </c>
-      <c r="M43" s="19" t="s">
+      <c r="M43" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="N43" s="17"/>
-      <c r="O43" s="5"/>
-      <c r="P43" s="5"/>
-      <c r="Q43" s="5"/>
-      <c r="R43" s="5"/>
-      <c r="S43" s="5"/>
-      <c r="T43" s="5"/>
-      <c r="U43" s="5"/>
-      <c r="V43" s="5"/>
-    </row>
-    <row r="44" spans="1:22" ht="13">
-      <c r="A44" s="95" t="s">
+      <c r="N43" s="22"/>
+      <c r="O43" s="7"/>
+      <c r="P43" s="7"/>
+      <c r="Q43" s="7"/>
+      <c r="R43" s="7"/>
+      <c r="S43" s="7"/>
+      <c r="T43" s="7"/>
+      <c r="U43" s="7"/>
+      <c r="V43" s="7"/>
+    </row>
+    <row r="44" spans="1:22" s="101" customFormat="1" ht="13">
+      <c r="A44" s="94"/>
+      <c r="B44" s="95" t="s">
+        <v>263</v>
+      </c>
+      <c r="C44" s="96" t="s">
+        <v>26</v>
+      </c>
+      <c r="D44" s="94"/>
+      <c r="E44" s="94"/>
+      <c r="F44" s="95" t="s">
+        <v>261</v>
+      </c>
+      <c r="G44" s="28" t="s">
+        <v>259</v>
+      </c>
+      <c r="H44" s="77" t="s">
+        <v>21</v>
+      </c>
+      <c r="I44" s="95" t="s">
+        <v>260</v>
+      </c>
+      <c r="J44" s="97" t="s">
+        <v>262</v>
+      </c>
+      <c r="K44" s="98"/>
+      <c r="L44" s="95">
+        <v>2849</v>
+      </c>
+      <c r="M44" s="99" t="s">
+        <v>60</v>
+      </c>
+      <c r="N44" s="94"/>
+      <c r="O44" s="100"/>
+      <c r="P44" s="100"/>
+      <c r="Q44" s="100"/>
+      <c r="R44" s="100"/>
+      <c r="S44" s="100"/>
+      <c r="T44" s="100"/>
+      <c r="U44" s="100"/>
+      <c r="V44" s="100"/>
+    </row>
+    <row r="45" spans="1:22" ht="13">
+      <c r="A45" s="92" t="s">
         <v>173</v>
       </c>
-      <c r="B44" s="95"/>
-      <c r="C44" s="95"/>
-      <c r="D44" s="95"/>
-      <c r="E44" s="95"/>
-      <c r="F44" s="95"/>
-      <c r="G44" s="95"/>
-      <c r="H44" s="95"/>
-      <c r="I44" s="95"/>
-      <c r="J44" s="95"/>
-      <c r="K44" s="95"/>
-      <c r="L44" s="95"/>
-      <c r="M44" s="95"/>
-      <c r="N44" s="95"/>
-      <c r="O44" s="2"/>
-      <c r="P44" s="2"/>
-      <c r="Q44" s="2"/>
-      <c r="R44" s="2"/>
-      <c r="S44" s="2"/>
-      <c r="T44" s="2"/>
-      <c r="U44" s="2"/>
-      <c r="V44" s="2"/>
-    </row>
-    <row r="45" spans="1:22" ht="13">
-      <c r="A45" s="38"/>
-      <c r="B45" s="79" t="s">
-        <v>174</v>
-      </c>
-      <c r="C45" s="42" t="s">
-        <v>175</v>
-      </c>
-      <c r="D45" s="38" t="s">
-        <v>176</v>
-      </c>
-      <c r="E45" s="38"/>
-      <c r="F45" s="40" t="s">
-        <v>177</v>
-      </c>
-      <c r="G45" s="40" t="s">
-        <v>178</v>
-      </c>
-      <c r="H45" s="38" t="s">
-        <v>21</v>
-      </c>
-      <c r="I45" s="40" t="s">
-        <v>179</v>
-      </c>
-      <c r="J45" s="80" t="s">
-        <v>180</v>
-      </c>
-      <c r="K45" s="73"/>
-      <c r="L45" s="81" t="s">
-        <v>181</v>
-      </c>
-      <c r="M45" s="39" t="s">
-        <v>60</v>
-      </c>
-      <c r="N45" s="38" t="s">
-        <v>182</v>
-      </c>
+      <c r="B45" s="92"/>
+      <c r="C45" s="92"/>
+      <c r="D45" s="92"/>
+      <c r="E45" s="92"/>
+      <c r="F45" s="92"/>
+      <c r="G45" s="92"/>
+      <c r="H45" s="92"/>
+      <c r="I45" s="92"/>
+      <c r="J45" s="92"/>
+      <c r="K45" s="92"/>
+      <c r="L45" s="92"/>
+      <c r="M45" s="92"/>
+      <c r="N45" s="92"/>
       <c r="O45" s="2"/>
       <c r="P45" s="2"/>
       <c r="Q45" s="2"/>
@@ -3213,40 +3242,42 @@
       <c r="V45" s="2"/>
     </row>
     <row r="46" spans="1:22" ht="13">
-      <c r="A46" s="43"/>
-      <c r="B46" s="44" t="s">
-        <v>183</v>
-      </c>
-      <c r="C46" s="47" t="s">
-        <v>184</v>
-      </c>
-      <c r="D46" s="43" t="s">
-        <v>185</v>
-      </c>
-      <c r="E46" s="43"/>
-      <c r="F46" s="44" t="s">
+      <c r="A46" s="38"/>
+      <c r="B46" s="79" t="s">
+        <v>174</v>
+      </c>
+      <c r="C46" s="42" t="s">
+        <v>175</v>
+      </c>
+      <c r="D46" s="38" t="s">
+        <v>176</v>
+      </c>
+      <c r="E46" s="38"/>
+      <c r="F46" s="40" t="s">
         <v>177</v>
       </c>
-      <c r="G46" s="43" t="s">
-        <v>186</v>
-      </c>
-      <c r="H46" s="43" t="s">
+      <c r="G46" s="40" t="s">
+        <v>178</v>
+      </c>
+      <c r="H46" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="I46" s="44" t="s">
-        <v>187</v>
-      </c>
-      <c r="J46" s="46" t="s">
-        <v>188</v>
-      </c>
-      <c r="K46" s="43"/>
-      <c r="L46" s="82">
-        <v>2019</v>
-      </c>
-      <c r="M46" s="45" t="s">
+      <c r="I46" s="40" t="s">
+        <v>179</v>
+      </c>
+      <c r="J46" s="80" t="s">
+        <v>180</v>
+      </c>
+      <c r="K46" s="73"/>
+      <c r="L46" s="81" t="s">
+        <v>181</v>
+      </c>
+      <c r="M46" s="39" t="s">
         <v>60</v>
       </c>
-      <c r="N46" s="43"/>
+      <c r="N46" s="38" t="s">
+        <v>182</v>
+      </c>
       <c r="O46" s="2"/>
       <c r="P46" s="2"/>
       <c r="Q46" s="2"/>
@@ -3254,24 +3285,43 @@
       <c r="S46" s="2"/>
       <c r="T46" s="2"/>
       <c r="U46" s="2"/>
+      <c r="V46" s="2"/>
     </row>
     <row r="47" spans="1:22" ht="13">
-      <c r="A47" s="95" t="s">
-        <v>214</v>
-      </c>
-      <c r="B47" s="95"/>
-      <c r="C47" s="95"/>
-      <c r="D47" s="95"/>
-      <c r="E47" s="95"/>
-      <c r="F47" s="95"/>
-      <c r="G47" s="95"/>
-      <c r="H47" s="95"/>
-      <c r="I47" s="95"/>
-      <c r="J47" s="95"/>
-      <c r="K47" s="95"/>
-      <c r="L47" s="95"/>
-      <c r="M47" s="95"/>
-      <c r="N47" s="95"/>
+      <c r="A47" s="43"/>
+      <c r="B47" s="44" t="s">
+        <v>183</v>
+      </c>
+      <c r="C47" s="47" t="s">
+        <v>184</v>
+      </c>
+      <c r="D47" s="43" t="s">
+        <v>185</v>
+      </c>
+      <c r="E47" s="43"/>
+      <c r="F47" s="44" t="s">
+        <v>177</v>
+      </c>
+      <c r="G47" s="43" t="s">
+        <v>186</v>
+      </c>
+      <c r="H47" s="43" t="s">
+        <v>21</v>
+      </c>
+      <c r="I47" s="44" t="s">
+        <v>187</v>
+      </c>
+      <c r="J47" s="46" t="s">
+        <v>188</v>
+      </c>
+      <c r="K47" s="43"/>
+      <c r="L47" s="82">
+        <v>2019</v>
+      </c>
+      <c r="M47" s="45" t="s">
+        <v>60</v>
+      </c>
+      <c r="N47" s="43"/>
       <c r="O47" s="2"/>
       <c r="P47" s="2"/>
       <c r="Q47" s="2"/>
@@ -3279,63 +3329,64 @@
       <c r="S47" s="2"/>
       <c r="T47" s="2"/>
       <c r="U47" s="2"/>
-      <c r="V47" s="2"/>
-    </row>
-    <row r="48" spans="1:22" s="4" customFormat="1" ht="13">
-      <c r="A48" s="83"/>
-      <c r="B48" s="71" t="s">
+    </row>
+    <row r="48" spans="1:22" ht="13">
+      <c r="A48" s="92" t="s">
+        <v>214</v>
+      </c>
+      <c r="B48" s="92"/>
+      <c r="C48" s="92"/>
+      <c r="D48" s="92"/>
+      <c r="E48" s="92"/>
+      <c r="F48" s="92"/>
+      <c r="G48" s="92"/>
+      <c r="H48" s="92"/>
+      <c r="I48" s="92"/>
+      <c r="J48" s="92"/>
+      <c r="K48" s="92"/>
+      <c r="L48" s="92"/>
+      <c r="M48" s="92"/>
+      <c r="N48" s="92"/>
+      <c r="O48" s="2"/>
+      <c r="P48" s="2"/>
+      <c r="Q48" s="2"/>
+      <c r="R48" s="2"/>
+      <c r="S48" s="2"/>
+      <c r="T48" s="2"/>
+      <c r="U48" s="2"/>
+      <c r="V48" s="2"/>
+    </row>
+    <row r="49" spans="1:22" s="4" customFormat="1" ht="13">
+      <c r="A49" s="83"/>
+      <c r="B49" s="71" t="s">
         <v>219</v>
       </c>
-      <c r="C48" s="83"/>
-      <c r="D48" s="83"/>
-      <c r="E48" s="83"/>
-      <c r="F48" s="71" t="s">
+      <c r="C49" s="83"/>
+      <c r="D49" s="83"/>
+      <c r="E49" s="83"/>
+      <c r="F49" s="71" t="s">
         <v>215</v>
       </c>
-      <c r="G48" s="71" t="s">
+      <c r="G49" s="71" t="s">
         <v>216</v>
       </c>
-      <c r="H48" s="38" t="s">
+      <c r="H49" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="I48" s="71" t="s">
+      <c r="I49" s="71" t="s">
         <v>217</v>
       </c>
-      <c r="J48" s="72" t="s">
+      <c r="J49" s="72" t="s">
         <v>218</v>
       </c>
-      <c r="K48" s="83"/>
-      <c r="L48" s="74">
+      <c r="K49" s="83"/>
+      <c r="L49" s="74">
         <v>4957</v>
       </c>
-      <c r="M48" s="39" t="s">
+      <c r="M49" s="39" t="s">
         <v>60</v>
       </c>
-      <c r="N48" s="83"/>
-      <c r="O48" s="1"/>
-      <c r="P48" s="1"/>
-      <c r="Q48" s="1"/>
-      <c r="R48" s="1"/>
-      <c r="S48" s="1"/>
-      <c r="T48" s="1"/>
-      <c r="U48" s="1"/>
-      <c r="V48" s="1"/>
-    </row>
-    <row r="49" spans="1:22" ht="12.5" hidden="1">
-      <c r="A49" s="1"/>
-      <c r="B49" s="1"/>
-      <c r="C49" s="1"/>
-      <c r="D49" s="1"/>
-      <c r="E49" s="1"/>
-      <c r="F49" s="1"/>
-      <c r="G49" s="1"/>
-      <c r="H49" s="1"/>
-      <c r="I49" s="1"/>
-      <c r="J49" s="1"/>
-      <c r="K49" s="1"/>
-      <c r="L49" s="1"/>
-      <c r="M49" s="1"/>
-      <c r="N49" s="1"/>
+      <c r="N49" s="83"/>
       <c r="O49" s="1"/>
       <c r="P49" s="1"/>
       <c r="Q49" s="1"/>
@@ -25041,13 +25092,37 @@
       <c r="U953" s="1"/>
       <c r="V953" s="1"/>
     </row>
-    <row r="954" spans="1:22" ht="15.75" customHeight="1"/>
+    <row r="954" spans="1:22" ht="12.5" hidden="1">
+      <c r="A954" s="1"/>
+      <c r="B954" s="1"/>
+      <c r="C954" s="1"/>
+      <c r="D954" s="1"/>
+      <c r="E954" s="1"/>
+      <c r="F954" s="1"/>
+      <c r="G954" s="1"/>
+      <c r="H954" s="1"/>
+      <c r="I954" s="1"/>
+      <c r="J954" s="1"/>
+      <c r="K954" s="1"/>
+      <c r="L954" s="1"/>
+      <c r="M954" s="1"/>
+      <c r="N954" s="1"/>
+      <c r="O954" s="1"/>
+      <c r="P954" s="1"/>
+      <c r="Q954" s="1"/>
+      <c r="R954" s="1"/>
+      <c r="S954" s="1"/>
+      <c r="T954" s="1"/>
+      <c r="U954" s="1"/>
+      <c r="V954" s="1"/>
+    </row>
+    <row r="955" spans="1:22" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="9">
     <mergeCell ref="A32:N32"/>
     <mergeCell ref="A39:N39"/>
-    <mergeCell ref="A44:N44"/>
-    <mergeCell ref="A47:N47"/>
+    <mergeCell ref="A45:N45"/>
+    <mergeCell ref="A48:N48"/>
     <mergeCell ref="A1:N1"/>
     <mergeCell ref="A3:N3"/>
     <mergeCell ref="A14:N14"/>

</xml_diff>